<commit_message>
Udbygning af forenklet model
</commit_message>
<xml_diff>
--- a/REFA Forenklet VPO-model.xlsx
+++ b/REFA Forenklet VPO-model.xlsx
@@ -8,79 +8,80 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\REFA Affald\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981254EB-5831-4C67-A5EC-F5D93CEE0754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47F7748-BA8C-4E37-967C-FA2B05C7595F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{858EECC8-30FB-4D42-A70B-DA5455FDD71D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{858EECC8-30FB-4D42-A70B-DA5455FDD71D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Affald2021" sheetId="2" r:id="rId2"/>
+    <sheet name="SolverRepos" sheetId="3" r:id="rId1"/>
+    <sheet name="Model" sheetId="1" r:id="rId2"/>
+    <sheet name="Affald2021" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="AFV">Sheet1!$C$34</definedName>
-    <definedName name="AndelAffald">Sheet1!$C$23</definedName>
-    <definedName name="AndelBioaffald">Sheet1!$D$23</definedName>
-    <definedName name="ATL">Sheet1!$C$35</definedName>
-    <definedName name="CO2afgift">Sheet1!$C$36</definedName>
-    <definedName name="CO2indholdAfgift">Sheet1!$C$26</definedName>
-    <definedName name="CO2indholdKvote">Sheet1!$C$27</definedName>
-    <definedName name="DBmedRGK">Sheet1!$K$72</definedName>
-    <definedName name="DBudenRGK">Sheet1!$J$72</definedName>
-    <definedName name="Elpris">Sheet1!$C$31</definedName>
-    <definedName name="ElprodTarif">Sheet1!$C$32</definedName>
-    <definedName name="ENSkvoteLHV">Sheet1!$C$28</definedName>
-    <definedName name="EtaE">Sheet1!$D$17</definedName>
-    <definedName name="EtaQmaxOvn2">Sheet1!$C$16</definedName>
-    <definedName name="EtaQmaxOvn3">Sheet1!$D$16</definedName>
-    <definedName name="EtaQNomOvn2">Sheet1!$C$14</definedName>
-    <definedName name="EtaQNomOvn3">Sheet1!$D$14</definedName>
-    <definedName name="EtaRgkOvn2">Sheet1!$C$15</definedName>
-    <definedName name="EtaRgkOvn3">Sheet1!$D$15</definedName>
-    <definedName name="Ftotal">Sheet1!$C$40</definedName>
-    <definedName name="Htotal">Sheet1!$C$41</definedName>
-    <definedName name="KapQcool">Sheet1!$E$10</definedName>
-    <definedName name="KapQnomOvn2">Sheet1!$C$10</definedName>
-    <definedName name="KapQnomOvn3">Sheet1!$D$10</definedName>
-    <definedName name="Kvotepris">Sheet1!$C$33</definedName>
-    <definedName name="LHVaffald">Sheet1!$C$25</definedName>
-    <definedName name="LHVbioaffald">Sheet1!$D$25</definedName>
-    <definedName name="NSvarme">Sheet1!$E$22</definedName>
-    <definedName name="Qdemand">Sheet1!$C$39</definedName>
-    <definedName name="RGKudnyttelse">Sheet1!$C$5</definedName>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$C$5</definedName>
-    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$C$5</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$C$5</definedName>
-    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$K$72</definedName>
-    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="Varmesalgspris">Sheet1!$C$30</definedName>
+    <definedName name="AFV">Model!$C$34</definedName>
+    <definedName name="AndelAffald">Model!$C$23</definedName>
+    <definedName name="AndelBioaffald">Model!$D$23</definedName>
+    <definedName name="ATL">Model!$C$35</definedName>
+    <definedName name="CO2afgift">Model!$C$36</definedName>
+    <definedName name="CO2indholdAfgift">Model!$C$26</definedName>
+    <definedName name="CO2indholdKvote">Model!$C$27</definedName>
+    <definedName name="DBmedRGK">Model!$K$72</definedName>
+    <definedName name="DBudenRGK">Model!$J$72</definedName>
+    <definedName name="Elpris">Model!$C$31</definedName>
+    <definedName name="ElprodTarif">Model!$C$32</definedName>
+    <definedName name="ENSkvoteLHV">Model!$C$28</definedName>
+    <definedName name="EtaE">Model!$D$17</definedName>
+    <definedName name="EtaQmaxOvn2">Model!$C$16</definedName>
+    <definedName name="EtaQmaxOvn3">Model!$D$16</definedName>
+    <definedName name="EtaQNomOvn2">Model!$C$14</definedName>
+    <definedName name="EtaQNomOvn3">Model!$D$14</definedName>
+    <definedName name="EtaRgkOvn2">Model!$C$15</definedName>
+    <definedName name="EtaRgkOvn3">Model!$D$15</definedName>
+    <definedName name="Ftotal">Model!$C$40</definedName>
+    <definedName name="Htotal">Model!$C$41</definedName>
+    <definedName name="KapQcool">Model!$E$10</definedName>
+    <definedName name="KapQnomOvn2">Model!$C$10</definedName>
+    <definedName name="KapQnomOvn3">Model!$D$10</definedName>
+    <definedName name="Kvotepris">Model!$C$33</definedName>
+    <definedName name="LHVaffald">Model!$C$25</definedName>
+    <definedName name="LHVbioaffald">Model!$D$25</definedName>
+    <definedName name="NSvarme">Model!$E$22</definedName>
+    <definedName name="Qdemand">Model!$C$39</definedName>
+    <definedName name="RGKudnyttelse">Model!$C$5</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">Model!$C$5</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">Model!$C$5</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">Model!$C$5</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">Model!$K$72</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="Varmesalgspris">Model!$C$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -124,7 +125,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-</t>
+RGK-udnyttelsen gælder RGK-varme for begge ovne.</t>
         </r>
       </text>
     </comment>
@@ -349,7 +350,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="157">
   <si>
     <t>INPUT</t>
   </si>
@@ -802,6 +803,24 @@
   </si>
   <si>
     <t>RGK</t>
+  </si>
+  <si>
+    <t>AFBILDNINGER</t>
+  </si>
+  <si>
+    <t>Navn</t>
+  </si>
+  <si>
+    <t>SOLVER-opsætninger</t>
+  </si>
+  <si>
+    <t>Beskrivelse</t>
+  </si>
+  <si>
+    <t>Maksimerer dækningsbidrag med RGK-udnyttelse som fri variabel</t>
+  </si>
+  <si>
+    <t>Restriktioner</t>
   </si>
 </sst>
 </file>
@@ -811,8 +830,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="#,##0.0"/>
-    <numFmt numFmtId="172" formatCode="#,##0,"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="#,##0,"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -859,7 +878,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -880,6 +899,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -913,7 +938,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -935,9 +960,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -948,7 +970,7 @@
     <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -957,16 +979,28 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1009,7 +1043,7 @@
     <c:title>
       <c:tx>
         <c:strRef>
-          <c:f>Sheet1!$N$56</c:f>
+          <c:f>Model!$N$56</c:f>
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
@@ -1031,7 +1065,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1069,7 +1103,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$57</c:f>
+              <c:f>Model!$J$57</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1288,7 +1322,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$H$58:$H$72</c:f>
+              <c:f>Model!$H$58:$H$72</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -1335,7 +1369,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$58:$J$72</c:f>
+              <c:f>Model!$J$58:$J$72</c:f>
               <c:numCache>
                 <c:formatCode>#,##0,</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1392,11 +1426,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$57</c:f>
+              <c:f>Model!$K$57</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Med 37% RGK</c:v>
+                  <c:v>Med 100% RGK</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1470,7 +1504,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$H$58:$H$72</c:f>
+              <c:f>Model!$H$58:$H$72</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -1517,48 +1551,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$58:$K$72</c:f>
+              <c:f>Model!$K$58:$K$72</c:f>
               <c:numCache>
-                <c:formatCode>#.##0.</c:formatCode>
+                <c:formatCode>#,##0,</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>7499765</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3894811.3944341238</c:v>
+                  <c:v>3822931.3787708599</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>201644.13790164556</c:v>
+                  <c:v>201730.28555860883</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6006879.2997616511</c:v>
+                  <c:v>5444927.3260209365</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1069888.0854113866</c:v>
+                  <c:v>1100462.4495554105</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2239801.2000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2016441.3790164555</c:v>
+                  <c:v>2017302.855586088</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>418792.04678346473</c:v>
+                  <c:v>418970.96571441251</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2113334.554404716</c:v>
+                  <c:v>1915629.1461956135</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17603099.832097419</c:v>
+                  <c:v>16969353.990350407</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7858257.265616023</c:v>
+                  <c:v>7692166.617051525</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9744842.5664813966</c:v>
+                  <c:v>9277187.3732988816</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1856,7 +1890,7 @@
     <c:title>
       <c:tx>
         <c:strRef>
-          <c:f>Sheet1!$N$13</c:f>
+          <c:f>Model!$N$13</c:f>
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
@@ -1878,7 +1912,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1906,7 +1940,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$5</c:f>
+              <c:f>Model!$O$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1925,9 +1959,66 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="da-DK"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$N$6:$N$11</c:f>
+              <c:f>Model!$N$6:$N$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1953,7 +2044,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$6:$O$11</c:f>
+              <c:f>Model!$O$6:$O$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1989,11 +2080,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$5</c:f>
+              <c:f>Model!$P$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Med 37% RGK</c:v>
+                  <c:v>Med 100% RGK</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2008,9 +2099,66 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="da-DK"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$N$6:$N$11</c:f>
+              <c:f>Model!$N$6:$N$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2036,18 +2184,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$6:$P$11</c:f>
+              <c:f>Model!$P$6:$P$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6071.2528082144381</c:v>
+                  <c:v>3850.78947368421</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18043.747191785562</c:v>
+                  <c:v>20264.21052631579</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2084.8085411386446</c:v>
+                  <c:v>5142.2449555410485</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2291,7 +2439,7 @@
     <c:title>
       <c:tx>
         <c:strRef>
-          <c:f>Sheet1!$N$35</c:f>
+          <c:f>Model!$N$35</c:f>
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
@@ -2313,7 +2461,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2351,7 +2499,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$57</c:f>
+              <c:f>Model!$L$57</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2371,6 +2519,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0," sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2429,7 +2578,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$H$58:$H$72</c:f>
+              <c:f>Model!$H$58:$H$72</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -2476,48 +2625,48 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$58:$L$72</c:f>
+              <c:f>Model!$L$58:$L$72</c:f>
               <c:numCache>
-                <c:formatCode>#.##0.</c:formatCode>
+                <c:formatCode>#,##0,</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>95477</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-52521.05678538885</c:v>
+                  <c:v>-124401.0724486527</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>201644.13790164556</c:v>
+                  <c:v>201730.28555860883</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-273238.69067808148</c:v>
+                  <c:v>-835190.66441879608</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20848.085411386564</c:v>
+                  <c:v>51422.449555410538</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>28514.160000000149</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-254841.82098354469</c:v>
+                  <c:v>-253980.34441391216</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-52927.761216535233</c:v>
+                  <c:v>-52748.842285587452</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-96130.575927038211</c:v>
+                  <c:v>-293835.98413614067</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-28638.609561827034</c:v>
+                  <c:v>-662384.45130883902</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-354537.91271573212</c:v>
+                  <c:v>-520628.56128023006</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>325899.30315390602</c:v>
+                  <c:v>-141755.89002860896</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2690,7 +2839,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="#.##0." sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0," sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4478,13 +4627,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>57148</xdr:colOff>
+      <xdr:colOff>12324</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>38098</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>25679</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>585972</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>18598</xdr:rowOff>
     </xdr:to>
@@ -4514,13 +4663,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:colOff>14007</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>16156</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>587655</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>190050</xdr:rowOff>
     </xdr:to>
@@ -4884,14 +5033,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B41C610-527A-4758-9182-C399B9E67627}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="10" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="31">
+        <v>1</v>
+      </c>
+      <c r="C3" s="31">
+        <v>2</v>
+      </c>
+      <c r="D3" s="31">
+        <v>3</v>
+      </c>
+      <c r="E3" s="31">
+        <v>4</v>
+      </c>
+      <c r="F3" s="31">
+        <v>5</v>
+      </c>
+      <c r="G3" s="31">
+        <v>6</v>
+      </c>
+      <c r="H3" s="31">
+        <v>7</v>
+      </c>
+      <c r="I3" s="31">
+        <v>8</v>
+      </c>
+      <c r="J3" s="31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6">
+        <f>MAX($K$74)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>COUNT($C$7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="b">
+        <f>RGKudnyttelse&lt;=1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="b">
+        <f>RGKudnyttelse&gt;=0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f>{32767;32767;0.000001;0.01;FALSE;FALSE;TRUE;1;1;1;0.0001;TRUE}</f>
+        <v>32767</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f>{0;0;1;100;0;FALSE;TRUE;0.075;0;0;FALSE;30}</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5354189-028E-4B88-AC75-E88799B17CAC}">
   <dimension ref="A2:T72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J72" sqref="J72"/>
+      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -4903,8 +5164,8 @@
     <col min="7" max="7" width="2.85546875" customWidth="1"/>
     <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="19" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="18" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="18" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.28515625" customWidth="1"/>
     <col min="13" max="13" width="2.85546875" customWidth="1"/>
     <col min="14" max="14" width="29.7109375" style="7" customWidth="1"/>
@@ -4912,27 +5173,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="H2" s="25" t="s">
+      <c r="A2" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="H2" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="N2" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="6"/>
@@ -4941,11 +5211,11 @@
       <c r="F4" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
       <c r="L4" s="5"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -4955,8 +5225,8 @@
       <c r="B5" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="24">
-        <v>0.3699402127229045</v>
+      <c r="C5" s="23">
+        <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>141</v>
@@ -4964,23 +5234,23 @@
       <c r="H5" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="22" t="s">
+      <c r="I5" s="11"/>
+      <c r="J5" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="22" t="s">
+      <c r="K5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="O5" s="28" t="str">
+      <c r="O5" s="26" t="str">
         <f>J13</f>
         <v>Uden RGK</v>
       </c>
-      <c r="P5" s="28" t="str">
+      <c r="P5" s="26" t="str">
         <f>K13</f>
-        <v>Med 37% RGK</v>
+        <v>Med 100% RGK</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -4988,12 +5258,12 @@
       <c r="H6" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="19">
+      <c r="I6" s="11"/>
+      <c r="J6" s="18">
         <f>24*C$9</f>
         <v>744</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="18">
         <f>24*D$9</f>
         <v>744</v>
       </c>
@@ -5001,13 +5271,13 @@
         <f>H40</f>
         <v>Varmeproduktion Ovn2</v>
       </c>
-      <c r="O6" s="19">
+      <c r="O6" s="18">
         <f>J40</f>
         <v>7068</v>
       </c>
-      <c r="P6" s="19">
+      <c r="P6" s="18">
         <f>K40</f>
-        <v>6071.2528082144381</v>
+        <v>3850.78947368421</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -5018,33 +5288,33 @@
       <c r="I7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="22">
         <f>J6*C10</f>
         <v>7068</v>
       </c>
-      <c r="K7" s="23">
+      <c r="K7" s="22">
         <f>K6*D10</f>
         <v>16740</v>
       </c>
-      <c r="L7" s="18"/>
+      <c r="L7" s="17"/>
       <c r="N7" s="7" t="str">
         <f>H41</f>
         <v>Varmeproduktion Ovn3</v>
       </c>
-      <c r="O7" s="19">
+      <c r="O7" s="18">
         <f>J41</f>
         <v>16740</v>
       </c>
-      <c r="P7" s="19">
+      <c r="P7" s="18">
         <f>K41</f>
-        <v>18043.747191785562</v>
+        <v>20264.21052631579</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="6" t="s">
         <v>1</v>
       </c>
@@ -5054,34 +5324,34 @@
       <c r="E8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="6" t="s">
         <v>150</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="J8" s="23">
+      <c r="J8" s="22">
         <f>EtaRgkOvn2/EtaQNomOvn2*J7</f>
-        <v>550.47103653168188</v>
-      </c>
-      <c r="K8" s="23">
+        <v>1488</v>
+      </c>
+      <c r="K8" s="22">
         <f>EtaRgkOvn2/EtaQNomOvn2*K7</f>
-        <v>1303.7471917855623</v>
+        <v>3524.2105263157891</v>
       </c>
       <c r="N8" s="7" t="str">
         <f>H43</f>
         <v>Heraf RGK-varme</v>
       </c>
-      <c r="O8" s="19">
+      <c r="O8" s="18">
         <f>J43</f>
         <v>0</v>
       </c>
-      <c r="P8" s="19">
+      <c r="P8" s="18">
         <f>K43</f>
-        <v>2084.8085411386446</v>
+        <v>5142.2449555410485</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -5100,26 +5370,26 @@
       <c r="H9" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="23">
+      <c r="J9" s="22">
         <f>SUM(J7:J8)</f>
-        <v>7618.4710365316823</v>
-      </c>
-      <c r="K9" s="23">
+        <v>8556</v>
+      </c>
+      <c r="K9" s="22">
         <f>SUM(K7:K8)</f>
-        <v>18043.747191785562</v>
+        <v>20264.21052631579</v>
       </c>
       <c r="N9" s="7" t="str">
         <f>H34</f>
         <v>Bortkølet varme</v>
       </c>
-      <c r="O9" s="19">
+      <c r="O9" s="18">
         <f>J34</f>
         <v>0</v>
       </c>
-      <c r="P9" s="19">
+      <c r="P9" s="18">
         <f>K34</f>
         <v>0</v>
       </c>
@@ -5146,11 +5416,11 @@
       <c r="I10" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="18">
         <f>J7/EtaQNomOvn2</f>
         <v>8374.4075829383892</v>
       </c>
-      <c r="K10" s="19">
+      <c r="K10" s="18">
         <f>K7/EtaQNomOvn3</f>
         <v>25518.292682926829</v>
       </c>
@@ -5158,11 +5428,11 @@
         <f>H46</f>
         <v>Leveret varme</v>
       </c>
-      <c r="O10" s="19">
+      <c r="O10" s="18">
         <f>J46</f>
         <v>23808</v>
       </c>
-      <c r="P10" s="19">
+      <c r="P10" s="18">
         <f>K46</f>
         <v>24115</v>
       </c>
@@ -5183,14 +5453,14 @@
       <c r="H11" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="23">
+      <c r="J11" s="22">
         <f>J10*3.6/Htotal</f>
         <v>2955.6732645664906</v>
       </c>
-      <c r="K11" s="23">
+      <c r="K11" s="22">
         <f>K10/(Htotal/3.6)</f>
         <v>9006.456241033</v>
       </c>
@@ -5198,11 +5468,11 @@
         <f>H47</f>
         <v>Spidslastvarme</v>
       </c>
-      <c r="O11" s="19">
+      <c r="O11" s="18">
         <f>J47</f>
         <v>4307</v>
       </c>
-      <c r="P11" s="19">
+      <c r="P11" s="18">
         <f>K47</f>
         <v>4000</v>
       </c>
@@ -5218,8 +5488,8 @@
         <v>8</v>
       </c>
       <c r="H12" s="7"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -5234,26 +5504,26 @@
       <c r="H13" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="J13" s="22" t="s">
+      <c r="J13" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="K13" s="22" t="str">
+      <c r="K13" s="21" t="str">
         <f>"Med "&amp;TEXT(C5,"0%")&amp;" RGK"</f>
-        <v>Med 37% RGK</v>
+        <v>Med 100% RGK</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="N13" s="29" t="str">
+      <c r="N13" s="27" t="str">
         <f>"Varmemængder: "&amp;C22&amp;" ton affald, "&amp;D22&amp;" ton bioaffald"</f>
         <v>Varmemængder: 12000 ton affald, 0 ton bioaffald</v>
       </c>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -5271,17 +5541,17 @@
       <c r="I14" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J14" s="23">
+      <c r="J14" s="22">
         <f>MIN(Qdemand,K7,EtaQNomOvn3*Ftotal*Htotal/3.6)</f>
         <v>16740</v>
       </c>
-      <c r="K14" s="23">
+      <c r="K14" s="22">
         <f>MIN(Qdemand,K9,EtaQmaxOvn3*Ftotal*Htotal/3.6)</f>
-        <v>18043.747191785562</v>
-      </c>
-      <c r="L14" s="19">
+        <v>20264.21052631579</v>
+      </c>
+      <c r="L14" s="18">
         <f>K14-J14</f>
-        <v>1303.7471917855619</v>
+        <v>3524.21052631579</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -5290,11 +5560,11 @@
       </c>
       <c r="C15" s="4">
         <f>$C$5*C11/C10*C14</f>
-        <v>6.5732534639606613E-2</v>
+        <v>0.17768421052631578</v>
       </c>
       <c r="D15" s="4">
         <f>$C$5*D11/D10*D14</f>
-        <v>5.9321968333521768E-2</v>
+        <v>0.16035555555555556</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>66</v>
@@ -5302,17 +5572,17 @@
       <c r="I15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="19">
+      <c r="J15" s="18">
         <f>$J$14/EtaQNomOvn3/(Htotal/3.6)</f>
         <v>9006.456241033</v>
       </c>
-      <c r="K15" s="19">
+      <c r="K15" s="18">
         <f>$K$14/EtaQmaxOvn3/(Htotal/3.6)</f>
-        <v>8902.818092729658</v>
-      </c>
-      <c r="L15" s="19">
+        <v>8760.9795201777761</v>
+      </c>
+      <c r="L15" s="18">
         <f t="shared" ref="L15:L55" si="0">K15-J15</f>
-        <v>-103.63814830334195</v>
+        <v>-245.4767208552239</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -5321,11 +5591,11 @@
       </c>
       <c r="C16" s="4">
         <f>SUM(C14:C15)</f>
-        <v>0.90973253463960657</v>
+        <v>1.0216842105263158</v>
       </c>
       <c r="D16" s="4">
         <f>SUM(D14:D15)</f>
-        <v>0.7153219683335218</v>
+        <v>0.81635555555555561</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>64</v>
@@ -5333,17 +5603,17 @@
       <c r="I16" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J16" s="23">
+      <c r="J16" s="22">
         <f>Qdemand-J14</f>
         <v>11375</v>
       </c>
-      <c r="K16" s="23">
+      <c r="K16" s="22">
         <f>Qdemand-K14</f>
-        <v>10071.252808214438</v>
-      </c>
-      <c r="L16" s="19">
+        <v>7850.78947368421</v>
+      </c>
+      <c r="L16" s="18">
         <f t="shared" si="0"/>
-        <v>-1303.7471917855619</v>
+        <v>-3524.21052631579</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -5359,17 +5629,17 @@
       <c r="I17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="23">
+      <c r="J17" s="22">
         <f>Ftotal-J15</f>
         <v>2993.543758967</v>
       </c>
-      <c r="K17" s="23">
+      <c r="K17" s="22">
         <f>Ftotal-K15</f>
-        <v>3097.181907270342</v>
-      </c>
-      <c r="L17" s="19">
+        <v>3239.0204798222239</v>
+      </c>
+      <c r="L17" s="18">
         <f t="shared" si="0"/>
-        <v>103.63814830334195</v>
+        <v>245.4767208552239</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -5397,15 +5667,15 @@
       <c r="I18" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J18" s="23">
+      <c r="J18" s="22">
         <f>MIN(J16,NSvarme)</f>
         <v>4000</v>
       </c>
-      <c r="K18" s="23">
+      <c r="K18" s="22">
         <f>MIN(K16,NSvarme)</f>
         <v>4000</v>
       </c>
-      <c r="L18" s="19">
+      <c r="L18" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5418,17 +5688,17 @@
       <c r="I19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J19" s="23">
+      <c r="J19" s="22">
         <f>J16-J18</f>
         <v>7375</v>
       </c>
-      <c r="K19" s="23">
+      <c r="K19" s="22">
         <f>K16-K18</f>
-        <v>6071.2528082144381</v>
-      </c>
-      <c r="L19" s="19">
+        <v>3850.78947368421</v>
+      </c>
+      <c r="L19" s="18">
         <f t="shared" si="0"/>
-        <v>-1303.7471917855619</v>
+        <v>-3524.21052631579</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -5450,17 +5720,17 @@
       <c r="I20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J20" s="23">
+      <c r="J20" s="22">
         <f>MIN($J$19,J7,EtaQNomOvn2*(J17*Htotal)/3.6)</f>
         <v>7068</v>
       </c>
-      <c r="K20" s="23">
+      <c r="K20" s="22">
         <f>MIN($K$19,J9,EtaQmaxOvn2*(K17*Htotal)/3.6)</f>
-        <v>6071.2528082144381</v>
-      </c>
-      <c r="L20" s="19">
+        <v>3850.78947368421</v>
+      </c>
+      <c r="L20" s="18">
         <f t="shared" si="0"/>
-        <v>-996.74719178556188</v>
+        <v>-3217.21052631579</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -5485,17 +5755,17 @@
       <c r="I21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="23">
+      <c r="J21" s="22">
         <f>$J$20/EtaQNomOvn2/(Htotal/3.6)</f>
         <v>2955.6732645664906</v>
       </c>
-      <c r="K21" s="23">
+      <c r="K21" s="22">
         <f>$K$20/EtaQNomOvn2/(Htotal/3.6)</f>
-        <v>2538.8567639592025</v>
-      </c>
-      <c r="L21" s="19">
+        <v>1610.3106246240077</v>
+      </c>
+      <c r="L21" s="18">
         <f t="shared" si="0"/>
-        <v>-416.81650060728816</v>
+        <v>-1345.3626399424829</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -5520,15 +5790,15 @@
       <c r="I22" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J22" s="23">
+      <c r="J22" s="22">
         <f>J19-J20</f>
         <v>307</v>
       </c>
-      <c r="K22" s="23">
+      <c r="K22" s="22">
         <f>K19-K20</f>
         <v>0</v>
       </c>
-      <c r="L22" s="19">
+      <c r="L22" s="18">
         <f t="shared" si="0"/>
         <v>-307</v>
       </c>
@@ -5551,17 +5821,17 @@
       <c r="I23" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="23">
+      <c r="J23" s="22">
         <f>J17-J21</f>
         <v>37.870494400509415</v>
       </c>
-      <c r="K23" s="23">
+      <c r="K23" s="22">
         <f>K17-K21</f>
-        <v>558.32514331113953</v>
-      </c>
-      <c r="L23" s="19">
+        <v>1628.7098551982162</v>
+      </c>
+      <c r="L23" s="18">
         <f t="shared" si="0"/>
-        <v>520.45464891063011</v>
+        <v>1590.8393607977068</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -5587,15 +5857,15 @@
       <c r="I24" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J24" s="23">
+      <c r="J24" s="22">
         <f>J14+J20</f>
         <v>23808</v>
       </c>
-      <c r="K24" s="23">
+      <c r="K24" s="22">
         <f>K14+K20</f>
         <v>24115</v>
       </c>
-      <c r="L24" s="19">
+      <c r="L24" s="18">
         <f t="shared" si="0"/>
         <v>307</v>
       </c>
@@ -5622,15 +5892,15 @@
       <c r="I25" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J25" s="23">
+      <c r="J25" s="22">
         <f>J22</f>
         <v>307</v>
       </c>
-      <c r="K25" s="23">
+      <c r="K25" s="22">
         <f>K22</f>
         <v>0</v>
       </c>
-      <c r="L25" s="19">
+      <c r="L25" s="18">
         <f t="shared" si="0"/>
         <v>-307</v>
       </c>
@@ -5657,15 +5927,15 @@
       <c r="I26" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J26" s="19">
+      <c r="J26" s="18">
         <f>$J$7-$J$20</f>
         <v>0</v>
       </c>
-      <c r="K26" s="19">
+      <c r="K26" s="18">
         <f>J26</f>
         <v>0</v>
       </c>
-      <c r="L26" s="19">
+      <c r="L26" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5692,15 +5962,15 @@
       <c r="I27" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J27" s="19">
+      <c r="J27" s="18">
         <f>$K$7-$J$14</f>
         <v>0</v>
       </c>
-      <c r="K27" s="19">
+      <c r="K27" s="18">
         <f>J27</f>
         <v>0</v>
       </c>
-      <c r="L27" s="19">
+      <c r="L27" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5727,15 +5997,15 @@
       <c r="I28" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J28" s="19">
+      <c r="J28" s="18">
         <f>MIN(J27,EtaQNomOvn3*J23*Htotal/3.6,24*E9*KapQcool)</f>
         <v>0</v>
       </c>
-      <c r="K28" s="19">
+      <c r="K28" s="18">
         <f>MIN(K27,EtaQNomOvn3*K23*Htotal/3.6,24*E9*KapQcool)</f>
         <v>0</v>
       </c>
-      <c r="L28" s="19">
+      <c r="L28" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5750,15 +6020,15 @@
       <c r="I29" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J29" s="19">
+      <c r="J29" s="18">
         <f>J28/EtaQNomOvn3/(Htotal/3.6)</f>
         <v>0</v>
       </c>
-      <c r="K29" s="19">
+      <c r="K29" s="18">
         <f>K28/EtaQNomOvn3/(Htotal/3.6)</f>
         <v>0</v>
       </c>
-      <c r="L29" s="19">
+      <c r="L29" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5779,17 +6049,17 @@
       <c r="I30" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J30" s="19">
+      <c r="J30" s="18">
         <f>J23-J29</f>
         <v>37.870494400509415</v>
       </c>
-      <c r="K30" s="19">
+      <c r="K30" s="18">
         <f>K23-K29</f>
-        <v>558.32514331113953</v>
-      </c>
-      <c r="L30" s="19">
+        <v>1628.7098551982162</v>
+      </c>
+      <c r="L30" s="18">
         <f t="shared" si="0"/>
-        <v>520.45464891063011</v>
+        <v>1590.8393607977068</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -5808,15 +6078,15 @@
       <c r="I31" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J31" s="19">
+      <c r="J31" s="18">
         <f>MIN(J26,EtaQNomOvn3*J30*Htotal/3.6,24*E9*KapQcool-J28)</f>
         <v>0</v>
       </c>
-      <c r="K31" s="19">
+      <c r="K31" s="18">
         <f>MIN(K26,EtaQNomOvn3*K30*Htotal/3.6,24*E9*KapQcool-K28)</f>
         <v>0</v>
       </c>
-      <c r="L31" s="19">
+      <c r="L31" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5837,15 +6107,15 @@
       <c r="I32" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J32" s="19">
+      <c r="J32" s="18">
         <f>J31/EtaQNomOvn2/(Htotal/3.6)</f>
         <v>0</v>
       </c>
-      <c r="K32" s="19">
+      <c r="K32" s="18">
         <f>K31/EtaQNomOvn2/(Htotal/3.6)</f>
         <v>0</v>
       </c>
-      <c r="L32" s="19">
+      <c r="L32" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5866,17 +6136,17 @@
       <c r="I33" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="19">
+      <c r="J33" s="18">
         <f>J30-J32</f>
         <v>37.870494400509415</v>
       </c>
-      <c r="K33" s="19">
+      <c r="K33" s="18">
         <f>K30-K32</f>
-        <v>558.32514331113953</v>
-      </c>
-      <c r="L33" s="19">
+        <v>1628.7098551982162</v>
+      </c>
+      <c r="L33" s="18">
         <f t="shared" si="0"/>
-        <v>520.45464891063011</v>
+        <v>1590.8393607977068</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
@@ -5895,15 +6165,15 @@
       <c r="I34" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J34" s="19">
+      <c r="J34" s="18">
         <f>J28+J31</f>
         <v>0</v>
       </c>
-      <c r="K34" s="19">
+      <c r="K34" s="18">
         <f>K28+K31</f>
         <v>0</v>
       </c>
-      <c r="L34" s="19">
+      <c r="L34" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5924,28 +6194,28 @@
       <c r="I35" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J35" s="19">
+      <c r="J35" s="18">
         <f>SUM($C$22:$D$22)-J36</f>
         <v>11962.129505599491</v>
       </c>
-      <c r="K35" s="19">
+      <c r="K35" s="18">
         <f>SUM($C$22:$D$22)-K36</f>
-        <v>11441.67485668886</v>
-      </c>
-      <c r="L35" s="19">
+        <v>10371.290144801784</v>
+      </c>
+      <c r="L35" s="18">
         <f t="shared" si="0"/>
-        <v>-520.45464891063057</v>
-      </c>
-      <c r="N35" s="29" t="str">
+        <v>-1590.8393607977068</v>
+      </c>
+      <c r="N35" s="27" t="str">
         <f>"RGK ift. Nominel: "&amp;C22&amp;" ton affald, "&amp;D22&amp;" ton bioaffald"</f>
         <v>RGK ift. Nominel: 12000 ton affald, 0 ton bioaffald</v>
       </c>
-      <c r="O35" s="13"/>
-      <c r="P35" s="13"/>
-      <c r="Q35" s="13"/>
-      <c r="R35" s="13"/>
-      <c r="S35" s="13"/>
-      <c r="T35" s="13"/>
+      <c r="O35" s="12"/>
+      <c r="P35" s="12"/>
+      <c r="Q35" s="12"/>
+      <c r="R35" s="12"/>
+      <c r="S35" s="12"/>
+      <c r="T35" s="12"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
@@ -5963,17 +6233,17 @@
       <c r="I36" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J36" s="23">
+      <c r="J36" s="22">
         <f>J23</f>
         <v>37.870494400509415</v>
       </c>
-      <c r="K36" s="23">
+      <c r="K36" s="22">
         <f>K23</f>
-        <v>558.32514331113953</v>
-      </c>
-      <c r="L36" s="19">
+        <v>1628.7098551982162</v>
+      </c>
+      <c r="L36" s="18">
         <f t="shared" si="0"/>
-        <v>520.45464891063011</v>
+        <v>1590.8393607977068</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
@@ -5983,17 +6253,17 @@
       <c r="I37" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J37" s="19">
+      <c r="J37" s="18">
         <f>EtaE*(J15+J29)*Htotal/3.6</f>
         <v>5733.9603658536589</v>
       </c>
-      <c r="K37" s="19">
+      <c r="K37" s="18">
         <f>EtaE*(K15+K29)*Htotal/3.6</f>
-        <v>5667.9791387363366</v>
-      </c>
-      <c r="L37" s="19">
+        <v>5577.6776115211806</v>
+      </c>
+      <c r="L37" s="18">
         <f t="shared" si="0"/>
-        <v>-65.981227117322305</v>
+        <v>-156.28275433247836</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
@@ -6006,15 +6276,15 @@
       <c r="I38" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J38" s="19">
+      <c r="J38" s="18">
         <f>$D$9*$D$13</f>
         <v>775</v>
       </c>
-      <c r="K38" s="19">
+      <c r="K38" s="18">
         <f>$D$9*$D$13</f>
         <v>775</v>
       </c>
-      <c r="L38" s="19">
+      <c r="L38" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6035,17 +6305,17 @@
       <c r="I39" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J39" s="19">
+      <c r="J39" s="18">
         <f>J37-J38</f>
         <v>4958.9603658536589</v>
       </c>
-      <c r="K39" s="19">
+      <c r="K39" s="18">
         <f>K37-K38</f>
-        <v>4892.9791387363366</v>
-      </c>
-      <c r="L39" s="19">
+        <v>4802.6776115211806</v>
+      </c>
+      <c r="L39" s="18">
         <f t="shared" si="0"/>
-        <v>-65.981227117322305</v>
+        <v>-156.28275433247836</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
@@ -6055,7 +6325,7 @@
       <c r="B40" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="16">
+      <c r="C40" s="15">
         <f>SUM(C22:D22)</f>
         <v>12000</v>
       </c>
@@ -6065,17 +6335,17 @@
       <c r="I40" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J40" s="19">
+      <c r="J40" s="18">
         <f>J20+J31</f>
         <v>7068</v>
       </c>
-      <c r="K40" s="19">
+      <c r="K40" s="18">
         <f>K20+K31</f>
-        <v>6071.2528082144381</v>
-      </c>
-      <c r="L40" s="19">
+        <v>3850.78947368421</v>
+      </c>
+      <c r="L40" s="18">
         <f t="shared" si="0"/>
-        <v>-996.74719178556188</v>
+        <v>-3217.21052631579</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
@@ -6085,11 +6355,11 @@
       <c r="B41" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="17">
+      <c r="C41" s="16">
         <f>(C22*LHVaffald+D22*LHVbioaffald)/Ftotal</f>
         <v>10.199999999999999</v>
       </c>
-      <c r="D41" s="15">
+      <c r="D41" s="14">
         <f>Htotal/3.6</f>
         <v>2.833333333333333</v>
       </c>
@@ -6099,17 +6369,17 @@
       <c r="I41" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J41" s="19">
+      <c r="J41" s="18">
         <f>J14+J28</f>
         <v>16740</v>
       </c>
-      <c r="K41" s="19">
+      <c r="K41" s="18">
         <f>K14+K28</f>
-        <v>18043.747191785562</v>
-      </c>
-      <c r="L41" s="19">
+        <v>20264.21052631579</v>
+      </c>
+      <c r="L41" s="18">
         <f t="shared" si="0"/>
-        <v>1303.7471917855619</v>
+        <v>3524.21052631579</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
@@ -6120,15 +6390,15 @@
       <c r="I42" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J42" s="19">
+      <c r="J42" s="18">
         <f>SUM(J40:J41)</f>
         <v>23808</v>
       </c>
-      <c r="K42" s="19">
+      <c r="K42" s="18">
         <f>SUM(K40:K41)</f>
         <v>24115</v>
       </c>
-      <c r="L42" s="19">
+      <c r="L42" s="18">
         <f t="shared" si="0"/>
         <v>307</v>
       </c>
@@ -6140,32 +6410,32 @@
       <c r="I43" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J43" s="19">
-        <v>0</v>
-      </c>
-      <c r="K43" s="19">
+      <c r="J43" s="18">
+        <v>0</v>
+      </c>
+      <c r="K43" s="18">
         <f>(EtaRgkOvn2*K15+EtaRgkOvn3*K21)*Htotal/3.6</f>
-        <v>2084.8085411386446</v>
-      </c>
-      <c r="L43" s="19">
+        <v>5142.2449555410485</v>
+      </c>
+      <c r="L43" s="18">
         <f t="shared" si="0"/>
-        <v>2084.8085411386446</v>
+        <v>5142.2449555410485</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H44" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="J44" s="19">
+      <c r="J44" s="18">
         <v>0</v>
       </c>
       <c r="K44" s="2">
         <f>K43/K45</f>
-        <v>7.0000000047916663E-2</v>
-      </c>
-      <c r="L44" s="19">
+        <v>0.17318225802397103</v>
+      </c>
+      <c r="L44" s="18">
         <f t="shared" si="0"/>
-        <v>7.0000000047916663E-2</v>
+        <v>0.17318225802397103</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
@@ -6175,17 +6445,17 @@
       <c r="I45" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="J45" s="19">
+      <c r="J45" s="18">
         <f>J42+J37</f>
         <v>29541.960365853658</v>
       </c>
-      <c r="K45" s="19">
+      <c r="K45" s="18">
         <f>K42+K37</f>
-        <v>29782.979138736337</v>
-      </c>
-      <c r="L45" s="19">
+        <v>29692.67761152118</v>
+      </c>
+      <c r="L45" s="18">
         <f t="shared" si="0"/>
-        <v>241.0187728826786</v>
+        <v>150.71724566752164</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
@@ -6195,15 +6465,15 @@
       <c r="I46" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J46" s="19">
+      <c r="J46" s="18">
         <f>J42-J34</f>
         <v>23808</v>
       </c>
-      <c r="K46" s="19">
+      <c r="K46" s="18">
         <f>K42-K34</f>
         <v>24115</v>
       </c>
-      <c r="L46" s="19">
+      <c r="L46" s="18">
         <f t="shared" si="0"/>
         <v>307</v>
       </c>
@@ -6215,15 +6485,15 @@
       <c r="I47" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J47" s="19">
+      <c r="J47" s="18">
         <f>Qdemand-J46</f>
         <v>4307</v>
       </c>
-      <c r="K47" s="19">
+      <c r="K47" s="18">
         <f>Qdemand-K46</f>
         <v>4000</v>
       </c>
-      <c r="L47" s="19">
+      <c r="L47" s="18">
         <f t="shared" si="0"/>
         <v>-307</v>
       </c>
@@ -6232,7 +6502,7 @@
       <c r="H48" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="L48" s="19"/>
+      <c r="L48" s="18"/>
     </row>
     <row r="49" spans="8:20" x14ac:dyDescent="0.25">
       <c r="H49" t="s">
@@ -6241,17 +6511,17 @@
       <c r="I49" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="J49" s="19">
+      <c r="J49" s="18">
         <f>J$35*$C$23*LHVaffald/3.6</f>
         <v>33892.70026586522</v>
       </c>
-      <c r="K49" s="19">
+      <c r="K49" s="18">
         <f>K$35*$C$23*LHVaffald/3.6</f>
-        <v>32418.078760618431</v>
-      </c>
-      <c r="L49" s="19">
+        <v>29385.322076938384</v>
+      </c>
+      <c r="L49" s="18">
         <f t="shared" si="0"/>
-        <v>-1474.6215052467887</v>
+        <v>-4507.3781889268357</v>
       </c>
     </row>
     <row r="50" spans="8:20" x14ac:dyDescent="0.25">
@@ -6261,15 +6531,15 @@
       <c r="I50" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="J50" s="19">
+      <c r="J50" s="18">
         <f>J$35*AndelBioaffald*LHVbioaffald/3.6</f>
         <v>0</v>
       </c>
-      <c r="K50" s="19">
+      <c r="K50" s="18">
         <f>K$35*AndelBioaffald*LHVbioaffald/3.6</f>
         <v>0</v>
       </c>
-      <c r="L50" s="19">
+      <c r="L50" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6281,17 +6551,17 @@
       <c r="I51" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="J51" s="19">
+      <c r="J51" s="18">
         <f>J45/0.85 - J50</f>
         <v>34755.247489239599</v>
       </c>
-      <c r="K51" s="19">
+      <c r="K51" s="18">
         <f>K45/0.95 - K50</f>
-        <v>31350.504356564565</v>
-      </c>
-      <c r="L51" s="19">
+        <v>31255.450117390716</v>
+      </c>
+      <c r="L51" s="18">
         <f t="shared" si="0"/>
-        <v>-3404.7431326750338</v>
+        <v>-3499.7973718488829</v>
       </c>
     </row>
     <row r="52" spans="8:20" x14ac:dyDescent="0.25">
@@ -6301,15 +6571,15 @@
       <c r="I52" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J52" s="19">
+      <c r="J52" s="18">
         <f>J42*J51/(J51+J50)</f>
         <v>23808</v>
       </c>
-      <c r="K52" s="19">
+      <c r="K52" s="18">
         <f>K42*K51/(K51+K50)</f>
         <v>24115</v>
       </c>
-      <c r="L52" s="19">
+      <c r="L52" s="18">
         <f t="shared" si="0"/>
         <v>307</v>
       </c>
@@ -6321,17 +6591,17 @@
       <c r="I53" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J53" s="19">
+      <c r="J53" s="18">
         <f>J37*J51/(J51+J50)</f>
         <v>5733.9603658536589</v>
       </c>
-      <c r="K53" s="19">
+      <c r="K53" s="18">
         <f>K37*K51/(K51+K50)</f>
-        <v>5667.9791387363366</v>
-      </c>
-      <c r="L53" s="19">
+        <v>5577.6776115211806</v>
+      </c>
+      <c r="L53" s="18">
         <f t="shared" si="0"/>
-        <v>-65.981227117322305</v>
+        <v>-156.28275433247836</v>
       </c>
     </row>
     <row r="54" spans="8:20" x14ac:dyDescent="0.25">
@@ -6341,17 +6611,17 @@
       <c r="I54" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J54" s="19">
+      <c r="J54" s="18">
         <f>J52/1.2</f>
         <v>19840</v>
       </c>
-      <c r="K54" s="19">
+      <c r="K54" s="18">
         <f>(K52-0.1*(K52+K53))/1.2</f>
-        <v>17613.918405105305</v>
-      </c>
-      <c r="L54" s="19">
+        <v>17621.443532373236</v>
+      </c>
+      <c r="L54" s="18">
         <f t="shared" si="0"/>
-        <v>-2226.0815948946947</v>
+        <v>-2218.5564676267641</v>
       </c>
     </row>
     <row r="55" spans="8:20" x14ac:dyDescent="0.25">
@@ -6361,323 +6631,324 @@
       <c r="I55" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J55" s="19">
+      <c r="J55" s="18">
         <f>J54</f>
         <v>19840</v>
       </c>
-      <c r="K55" s="19">
+      <c r="K55" s="18">
         <f>K54</f>
-        <v>17613.918405105305</v>
-      </c>
-      <c r="L55" s="19">
+        <v>17621.443532373236</v>
+      </c>
+      <c r="L55" s="18">
         <f t="shared" si="0"/>
-        <v>-2226.0815948946947</v>
+        <v>-2218.5564676267641</v>
       </c>
     </row>
     <row r="56" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="N56" s="29" t="str">
+      <c r="N56" s="27" t="str">
         <f>"Økonomiske nøgletal: "&amp;C22&amp;" ton affald, "&amp;D22&amp;" ton bioaffald"</f>
         <v>Økonomiske nøgletal: 12000 ton affald, 0 ton bioaffald</v>
       </c>
-      <c r="O56" s="13"/>
-      <c r="P56" s="13"/>
-      <c r="Q56" s="13"/>
-      <c r="R56" s="13"/>
-      <c r="S56" s="13"/>
-      <c r="T56" s="13"/>
+      <c r="O56" s="12"/>
+      <c r="P56" s="12"/>
+      <c r="Q56" s="12"/>
+      <c r="R56" s="12"/>
+      <c r="S56" s="12"/>
+      <c r="T56" s="12"/>
     </row>
     <row r="57" spans="8:20" x14ac:dyDescent="0.25">
       <c r="H57" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="I57" s="12"/>
-      <c r="J57" s="22" t="str">
+      <c r="I57" s="11"/>
+      <c r="J57" s="21" t="str">
         <f>J13</f>
         <v>Uden RGK</v>
       </c>
-      <c r="K57" s="22" t="str">
+      <c r="K57" s="21" t="str">
         <f>K13</f>
-        <v>Med 37% RGK</v>
+        <v>Med 100% RGK</v>
       </c>
       <c r="L57" s="5" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="58" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H58" s="21" t="s">
+      <c r="H58" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="I58" s="21" t="s">
+      <c r="I58" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="J58" s="26">
+      <c r="J58" s="24">
         <f>Varmesalgspris*J46</f>
         <v>7404288</v>
       </c>
-      <c r="K58" s="26">
+      <c r="K58" s="24">
         <f>Varmesalgspris*K46</f>
         <v>7499765</v>
       </c>
-      <c r="L58" s="27">
+      <c r="L58" s="25">
         <f>K58-J58</f>
         <v>95477</v>
       </c>
     </row>
     <row r="59" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H59" s="21" t="s">
+      <c r="H59" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="I59" s="21" t="s">
+      <c r="I59" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="J59" s="26">
+      <c r="J59" s="24">
         <f>(Elpris-ElprodTarif)*J39</f>
         <v>3947332.4512195126</v>
       </c>
-      <c r="K59" s="26">
+      <c r="K59" s="24">
         <f>(Elpris-ElprodTarif)*K39</f>
-        <v>3894811.3944341238</v>
-      </c>
-      <c r="L59" s="27">
+        <v>3822931.3787708599</v>
+      </c>
+      <c r="L59" s="25">
         <f t="shared" ref="L59:L72" si="1">K59-J59</f>
-        <v>-52521.05678538885</v>
+        <v>-124401.0724486527</v>
       </c>
     </row>
     <row r="60" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H60" s="21" t="s">
+      <c r="H60" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="I60" s="21" t="s">
+      <c r="I60" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="J60" s="26">
-        <v>0</v>
-      </c>
-      <c r="K60" s="26">
+      <c r="J60" s="24">
+        <v>0</v>
+      </c>
+      <c r="K60" s="24">
         <f>IF(K43&lt;7%*K45,0,10%)*K66</f>
-        <v>201644.13790164556</v>
-      </c>
-      <c r="L60" s="27">
+        <v>201730.28555860883</v>
+      </c>
+      <c r="L60" s="25">
         <f t="shared" si="1"/>
-        <v>201644.13790164556</v>
+        <v>201730.28555860883</v>
       </c>
     </row>
     <row r="61" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H61" s="21" t="s">
+      <c r="H61" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="I61" s="21" t="s">
+      <c r="I61" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="J61" s="26">
+      <c r="J61" s="24">
         <f>$C$24*($C$22-J36*$C$23)</f>
         <v>6280117.9904397326</v>
       </c>
-      <c r="K61" s="26">
+      <c r="K61" s="24">
         <f>$C$24*($C$22-K36*$C$23)</f>
-        <v>6006879.2997616511</v>
-      </c>
-      <c r="L61" s="27">
+        <v>5444927.3260209365</v>
+      </c>
+      <c r="L61" s="25">
         <f t="shared" si="1"/>
-        <v>-273238.69067808148</v>
+        <v>-835190.66441879608</v>
       </c>
     </row>
     <row r="62" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="I62" s="21"/>
-      <c r="J62" s="27"/>
-      <c r="K62" s="27"/>
-      <c r="L62" s="27"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="25"/>
+      <c r="K62" s="25"/>
+      <c r="L62" s="25"/>
     </row>
     <row r="63" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H63" s="21" t="s">
+      <c r="H63" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="I63" s="21" t="s">
+      <c r="I63" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="J63" s="27">
+      <c r="J63" s="25">
         <f>$D$24*($D$22-J36*AndelBioaffald)</f>
         <v>0</v>
       </c>
-      <c r="K63" s="27">
+      <c r="K63" s="25">
         <f>$D$24*($D$22-K36*AndelBioaffald)</f>
         <v>0</v>
       </c>
-      <c r="L63" s="27">
+      <c r="L63" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H64" s="21" t="s">
+      <c r="H64" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="I64" s="21" t="s">
+      <c r="I64" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="J64" s="26">
+      <c r="J64" s="24">
         <f>$C$18*J40+$D$18*J41+$E$18*J34</f>
         <v>1049040</v>
       </c>
-      <c r="K64" s="26">
+      <c r="K64" s="24">
         <f>J64+$F$18*$K$43</f>
-        <v>1069888.0854113866</v>
-      </c>
-      <c r="L64" s="27">
+        <v>1100462.4495554105</v>
+      </c>
+      <c r="L64" s="25">
         <f t="shared" si="1"/>
-        <v>20848.085411386564</v>
+        <v>51422.449555410538</v>
       </c>
     </row>
     <row r="65" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H65" s="21" t="s">
+      <c r="H65" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="I65" s="21" t="s">
+      <c r="I65" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="J65" s="26">
+      <c r="J65" s="24">
         <f>AFV*3.6*J46</f>
         <v>2211287.04</v>
       </c>
-      <c r="K65" s="26">
+      <c r="K65" s="24">
         <f>AFV*3.6*K46</f>
         <v>2239801.2000000002</v>
       </c>
-      <c r="L65" s="27">
+      <c r="L65" s="25">
         <f t="shared" si="1"/>
         <v>28514.160000000149</v>
       </c>
     </row>
     <row r="66" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H66" s="21" t="s">
+      <c r="H66" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="I66" s="21" t="s">
+      <c r="I66" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="J66" s="27">
+      <c r="J66" s="25">
         <f>ATL*3.6*J54</f>
         <v>2271283.2000000002</v>
       </c>
-      <c r="K66" s="27">
+      <c r="K66" s="25">
         <f>ATL*3.6*K54</f>
-        <v>2016441.3790164555</v>
-      </c>
-      <c r="L66" s="27">
+        <v>2017302.855586088</v>
+      </c>
+      <c r="L66" s="25">
         <f t="shared" si="1"/>
-        <v>-254841.82098354469</v>
+        <v>-253980.34441391216</v>
       </c>
     </row>
     <row r="67" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H67" s="21" t="s">
+      <c r="H67" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="I67" s="21" t="s">
+      <c r="I67" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="J67" s="27">
+      <c r="J67" s="25">
         <f>CO2afgift*$C$26 /1000 *3.6*J54</f>
         <v>471719.80799999996</v>
       </c>
-      <c r="K67" s="27">
+      <c r="K67" s="25">
         <f>CO2afgift*$C$26 /1000 *3.6*K54</f>
-        <v>418792.04678346473</v>
-      </c>
-      <c r="L67" s="27">
+        <v>418970.96571441251</v>
+      </c>
+      <c r="L67" s="25">
         <f t="shared" si="1"/>
-        <v>-52927.761216535233</v>
+        <v>-52748.842285587452</v>
       </c>
     </row>
     <row r="68" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H68" s="21" t="s">
+      <c r="H68" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="I68" s="21" t="s">
+      <c r="I68" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="J68" s="27">
+      <c r="J68" s="25">
         <f>Kvotepris*$C$27/1000*C28*J35</f>
         <v>2209465.1303317542</v>
       </c>
-      <c r="K68" s="27">
+      <c r="K68" s="25">
         <f>Kvotepris*$C$27/1000*10.6*K35</f>
-        <v>2113334.554404716</v>
-      </c>
-      <c r="L68" s="27">
+        <v>1915629.1461956135</v>
+      </c>
+      <c r="L68" s="25">
         <f t="shared" si="1"/>
-        <v>-96130.575927038211</v>
+        <v>-293835.98413614067</v>
       </c>
     </row>
     <row r="69" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="I69" s="21"/>
-      <c r="J69" s="27"/>
-      <c r="K69" s="27"/>
-      <c r="L69" s="27"/>
+      <c r="I69" s="20"/>
+      <c r="J69" s="25"/>
+      <c r="K69" s="25"/>
+      <c r="L69" s="25"/>
     </row>
     <row r="70" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H70" s="21" t="s">
+      <c r="H70" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="I70" s="21" t="s">
+      <c r="I70" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="J70" s="27">
+      <c r="J70" s="25">
         <f>SUM(J58:J61)</f>
         <v>17631738.441659246</v>
       </c>
-      <c r="K70" s="27">
+      <c r="K70" s="25">
         <f>SUM(K58:K61)</f>
-        <v>17603099.832097419</v>
-      </c>
-      <c r="L70" s="27">
+        <v>16969353.990350407</v>
+      </c>
+      <c r="L70" s="25">
         <f t="shared" si="1"/>
-        <v>-28638.609561827034</v>
+        <v>-662384.45130883902</v>
       </c>
     </row>
     <row r="71" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H71" s="21" t="s">
+      <c r="H71" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="I71" s="21" t="s">
+      <c r="I71" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="J71" s="27">
+      <c r="J71" s="25">
         <f>SUM(J63:J68)</f>
         <v>8212795.1783317551</v>
       </c>
-      <c r="K71" s="27">
+      <c r="K71" s="25">
         <f>SUM(K63:K68)</f>
-        <v>7858257.265616023</v>
-      </c>
-      <c r="L71" s="27">
+        <v>7692166.617051525</v>
+      </c>
+      <c r="L71" s="25">
         <f t="shared" si="1"/>
-        <v>-354537.91271573212</v>
+        <v>-520628.56128023006</v>
       </c>
     </row>
     <row r="72" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H72" s="21" t="s">
+      <c r="H72" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="I72" s="21" t="s">
+      <c r="I72" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="J72" s="27">
+      <c r="J72" s="25">
         <f>J70-J71</f>
         <v>9418943.2633274905</v>
       </c>
-      <c r="K72" s="27">
+      <c r="K72" s="25">
         <f>K70-K71</f>
-        <v>9744842.5664813966</v>
-      </c>
-      <c r="L72" s="27">
+        <v>9277187.3732988816</v>
+      </c>
+      <c r="L72" s="25">
         <f t="shared" si="1"/>
-        <v>325899.30315390602</v>
+        <v>-141755.89002860896</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="H2:L2"/>
+    <mergeCell ref="N2:T2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6686,7 +6957,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B38EAE2D-0C92-4631-B92C-FB0A81AF4228}">
   <dimension ref="C2:P30"/>
   <sheetViews>
@@ -6739,29 +7010,29 @@
       <c r="C4" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="18">
         <v>11400.2114002</v>
       </c>
       <c r="F4" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="18">
         <v>1382.27949725194</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="18">
         <v>2526.36441138806</v>
       </c>
       <c r="J4" t="s">
         <v>77</v>
       </c>
-      <c r="K4" s="20">
+      <c r="K4" s="19">
         <v>10.5</v>
       </c>
-      <c r="M4" s="19">
+      <c r="M4" s="18">
         <f>G4*$K4/3.6</f>
         <v>4031.6485336514916</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="18">
         <f>H4*$K4/3.6</f>
         <v>7368.5628665485083</v>
       </c>
@@ -6770,29 +7041,29 @@
       <c r="C5" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="18">
         <v>0</v>
       </c>
       <c r="F5" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="19">
-        <v>0</v>
-      </c>
-      <c r="H5" s="19">
+      <c r="G5" s="18">
+        <v>0</v>
+      </c>
+      <c r="H5" s="18">
         <v>0</v>
       </c>
       <c r="J5" t="s">
         <v>78</v>
       </c>
-      <c r="K5" s="20">
+      <c r="K5" s="19">
         <v>10.5</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="18">
         <f t="shared" ref="M5:M24" si="0">G5*$K5/3.6</f>
         <v>0</v>
       </c>
-      <c r="N5" s="19">
+      <c r="N5" s="18">
         <f t="shared" ref="N5:N24" si="1">H5*$K5/3.6</f>
         <v>0</v>
       </c>
@@ -6801,29 +7072,29 @@
       <c r="C6" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="18">
         <v>0</v>
       </c>
       <c r="F6" t="s">
         <v>79</v>
       </c>
-      <c r="G6" s="19">
-        <v>0</v>
-      </c>
-      <c r="H6" s="19">
+      <c r="G6" s="18">
+        <v>0</v>
+      </c>
+      <c r="H6" s="18">
         <v>0</v>
       </c>
       <c r="J6" t="s">
         <v>79</v>
       </c>
-      <c r="K6" s="20">
+      <c r="K6" s="19">
         <v>10.5</v>
       </c>
-      <c r="M6" s="19">
+      <c r="M6" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N6" s="19">
+      <c r="N6" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6832,29 +7103,29 @@
       <c r="C7" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="18">
         <v>6154.3428210033298</v>
       </c>
       <c r="F7" t="s">
         <v>80</v>
       </c>
-      <c r="G7" s="19">
-        <v>0</v>
-      </c>
-      <c r="H7" s="19">
+      <c r="G7" s="18">
+        <v>0</v>
+      </c>
+      <c r="H7" s="18">
         <v>2356.9823569800001</v>
       </c>
       <c r="J7" t="s">
         <v>80</v>
       </c>
-      <c r="K7" s="20">
+      <c r="K7" s="19">
         <v>9.4</v>
       </c>
-      <c r="M7" s="19">
+      <c r="M7" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N7" s="19">
+      <c r="N7" s="18">
         <f t="shared" si="1"/>
         <v>6154.3428210033335</v>
       </c>
@@ -6863,29 +7134,29 @@
       <c r="C8" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="18">
         <v>1276.2179428833299</v>
       </c>
       <c r="F8" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="18">
         <v>437.56043756000003</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="18">
         <v>0</v>
       </c>
       <c r="J8" t="s">
         <v>81</v>
       </c>
-      <c r="K8" s="20">
+      <c r="K8" s="19">
         <v>10.5</v>
       </c>
-      <c r="M8" s="19">
+      <c r="M8" s="18">
         <f t="shared" si="0"/>
         <v>1276.2179428833335</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6894,29 +7165,29 @@
       <c r="C9" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="18">
         <v>0</v>
       </c>
       <c r="F9" t="s">
         <v>82</v>
       </c>
-      <c r="G9" s="19">
-        <v>0</v>
-      </c>
-      <c r="H9" s="19">
+      <c r="G9" s="18">
+        <v>0</v>
+      </c>
+      <c r="H9" s="18">
         <v>0</v>
       </c>
       <c r="J9" t="s">
         <v>82</v>
       </c>
-      <c r="K9" s="20">
+      <c r="K9" s="19">
         <v>14.5</v>
       </c>
-      <c r="M9" s="19">
+      <c r="M9" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N9" s="19">
+      <c r="N9" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6925,29 +7196,29 @@
       <c r="C10" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="18">
         <v>972.20097220000002</v>
       </c>
       <c r="F10" t="s">
         <v>83</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="18">
         <v>291.66029165999998</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="18">
         <v>0</v>
       </c>
       <c r="J10" t="s">
         <v>83</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K10" s="19">
         <v>12</v>
       </c>
-      <c r="M10" s="19">
+      <c r="M10" s="18">
         <f t="shared" si="0"/>
         <v>972.20097219999991</v>
       </c>
-      <c r="N10" s="19">
+      <c r="N10" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6956,29 +7227,29 @@
       <c r="C11" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="18">
         <v>15.375015375</v>
       </c>
       <c r="F11" t="s">
         <v>84</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="18">
         <v>6.1500061500000003</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="18">
         <v>0</v>
       </c>
       <c r="J11" t="s">
         <v>84</v>
       </c>
-      <c r="K11" s="20">
+      <c r="K11" s="19">
         <v>9</v>
       </c>
-      <c r="M11" s="19">
+      <c r="M11" s="18">
         <f t="shared" si="0"/>
         <v>15.375015375</v>
       </c>
-      <c r="N11" s="19">
+      <c r="N11" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6987,29 +7258,29 @@
       <c r="C12" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="18">
         <v>785.27856305555599</v>
       </c>
       <c r="F12" t="s">
         <v>85</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="18">
         <v>257.00025699999998</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="18">
         <v>0</v>
       </c>
       <c r="J12" t="s">
         <v>85</v>
       </c>
-      <c r="K12" s="20">
+      <c r="K12" s="19">
         <v>11</v>
       </c>
-      <c r="M12" s="19">
+      <c r="M12" s="18">
         <f t="shared" si="0"/>
         <v>785.27856305555542</v>
       </c>
-      <c r="N12" s="19">
+      <c r="N12" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7018,29 +7289,29 @@
       <c r="C13" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="18">
         <v>60.1667268333333</v>
       </c>
       <c r="F13" t="s">
         <v>86</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="18">
         <v>22.800022800000001</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="18">
         <v>0</v>
       </c>
       <c r="J13" t="s">
         <v>86</v>
       </c>
-      <c r="K13" s="20">
+      <c r="K13" s="19">
         <v>9.5</v>
       </c>
-      <c r="M13" s="19">
+      <c r="M13" s="18">
         <f t="shared" si="0"/>
         <v>60.166726833333335</v>
       </c>
-      <c r="N13" s="19">
+      <c r="N13" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7049,29 +7320,29 @@
       <c r="C14" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="18">
         <v>2540.00254</v>
       </c>
       <c r="F14" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="19">
-        <v>0</v>
-      </c>
-      <c r="H14" s="19">
+      <c r="G14" s="18">
+        <v>0</v>
+      </c>
+      <c r="H14" s="18">
         <v>1016.001016</v>
       </c>
       <c r="J14" t="s">
         <v>87</v>
       </c>
-      <c r="K14" s="20">
+      <c r="K14" s="19">
         <v>9</v>
       </c>
-      <c r="M14" s="19">
+      <c r="M14" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N14" s="19">
+      <c r="N14" s="18">
         <f t="shared" si="1"/>
         <v>2540.00254</v>
       </c>
@@ -7080,29 +7351,29 @@
       <c r="C15" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="18">
         <v>45.100045100000003</v>
       </c>
       <c r="F15" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="19">
-        <v>0</v>
-      </c>
-      <c r="H15" s="19">
+      <c r="G15" s="18">
+        <v>0</v>
+      </c>
+      <c r="H15" s="18">
         <v>13.53001353</v>
       </c>
       <c r="J15" t="s">
         <v>88</v>
       </c>
-      <c r="K15" s="20">
+      <c r="K15" s="19">
         <v>12</v>
       </c>
-      <c r="M15" s="19">
+      <c r="M15" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N15" s="19">
+      <c r="N15" s="18">
         <f t="shared" si="1"/>
         <v>45.100045100000003</v>
       </c>
@@ -7111,29 +7382,29 @@
       <c r="C16" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="18">
         <v>18.861129972222201</v>
       </c>
       <c r="F16" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="18">
         <v>6.7900067899999996</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="18">
         <v>0</v>
       </c>
       <c r="J16" t="s">
         <v>89</v>
       </c>
-      <c r="K16" s="20">
+      <c r="K16" s="19">
         <v>10</v>
       </c>
-      <c r="M16" s="19">
+      <c r="M16" s="18">
         <f t="shared" si="0"/>
         <v>18.861129972222219</v>
       </c>
-      <c r="N16" s="19">
+      <c r="N16" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7142,29 +7413,29 @@
       <c r="C17" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="18">
         <v>0</v>
       </c>
       <c r="F17" t="s">
         <v>90</v>
       </c>
-      <c r="G17" s="19">
-        <v>0</v>
-      </c>
-      <c r="H17" s="19">
+      <c r="G17" s="18">
+        <v>0</v>
+      </c>
+      <c r="H17" s="18">
         <v>0</v>
       </c>
       <c r="J17" t="s">
         <v>90</v>
       </c>
-      <c r="K17" s="20">
+      <c r="K17" s="19">
         <v>11</v>
       </c>
-      <c r="M17" s="19">
+      <c r="M17" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N17" s="19">
+      <c r="N17" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7173,29 +7444,29 @@
       <c r="C18" t="s">
         <v>91</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="18">
         <v>9410.2844102750005</v>
       </c>
       <c r="F18" t="s">
         <v>91</v>
       </c>
-      <c r="G18" s="19">
-        <v>0</v>
-      </c>
-      <c r="H18" s="19">
+      <c r="G18" s="18">
+        <v>0</v>
+      </c>
+      <c r="H18" s="18">
         <v>3226.38322638</v>
       </c>
       <c r="J18" t="s">
         <v>91</v>
       </c>
-      <c r="K18" s="20">
+      <c r="K18" s="19">
         <v>10.5</v>
       </c>
-      <c r="M18" s="19">
+      <c r="M18" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N18" s="19">
+      <c r="N18" s="18">
         <f t="shared" si="1"/>
         <v>9410.2844102750005</v>
       </c>
@@ -7204,29 +7475,29 @@
       <c r="C19" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="18">
         <v>0</v>
       </c>
       <c r="F19" t="s">
         <v>92</v>
       </c>
-      <c r="G19" s="19">
-        <v>0</v>
-      </c>
-      <c r="H19" s="19">
+      <c r="G19" s="18">
+        <v>0</v>
+      </c>
+      <c r="H19" s="18">
         <v>0</v>
       </c>
       <c r="J19" t="s">
         <v>92</v>
       </c>
-      <c r="K19" s="20">
+      <c r="K19" s="19">
         <v>10.5</v>
       </c>
-      <c r="M19" s="19">
+      <c r="M19" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N19" s="19">
+      <c r="N19" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7235,29 +7506,29 @@
       <c r="C20" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="18">
         <v>0</v>
       </c>
       <c r="F20" t="s">
         <v>93</v>
       </c>
-      <c r="G20" s="19">
-        <v>0</v>
-      </c>
-      <c r="H20" s="19">
+      <c r="G20" s="18">
+        <v>0</v>
+      </c>
+      <c r="H20" s="18">
         <v>0</v>
       </c>
       <c r="J20" t="s">
         <v>93</v>
       </c>
-      <c r="K20" s="20">
+      <c r="K20" s="19">
         <v>13</v>
       </c>
-      <c r="M20" s="19">
+      <c r="M20" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N20" s="19">
+      <c r="N20" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7266,29 +7537,29 @@
       <c r="C21" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="18">
         <v>231.59745381944401</v>
       </c>
       <c r="F21" t="s">
         <v>94</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="18">
         <v>57.500057499999997</v>
       </c>
-      <c r="H21" s="19">
+      <c r="H21" s="18">
         <v>0</v>
       </c>
       <c r="J21" t="s">
         <v>94</v>
       </c>
-      <c r="K21" s="20">
+      <c r="K21" s="19">
         <v>14.5</v>
       </c>
-      <c r="M21" s="19">
+      <c r="M21" s="18">
         <f t="shared" si="0"/>
         <v>231.59745381944444</v>
       </c>
-      <c r="N21" s="19">
+      <c r="N21" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7297,29 +7568,29 @@
       <c r="C22" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="18">
         <v>0</v>
       </c>
       <c r="F22" t="s">
         <v>95</v>
       </c>
-      <c r="G22" s="19">
-        <v>0</v>
-      </c>
-      <c r="H22" s="19">
+      <c r="G22" s="18">
+        <v>0</v>
+      </c>
+      <c r="H22" s="18">
         <v>0</v>
       </c>
       <c r="J22" t="s">
         <v>95</v>
       </c>
-      <c r="K22" s="20">
+      <c r="K22" s="19">
         <v>14.7</v>
       </c>
-      <c r="M22" s="19">
+      <c r="M22" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N22" s="19">
+      <c r="N22" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7328,29 +7599,29 @@
       <c r="C23" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="18">
         <v>41.300041299999997</v>
       </c>
       <c r="F23" t="s">
         <v>96</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="18">
         <v>10.62001062</v>
       </c>
-      <c r="H23" s="19">
+      <c r="H23" s="18">
         <v>0</v>
       </c>
       <c r="J23" t="s">
         <v>96</v>
       </c>
-      <c r="K23" s="20">
+      <c r="K23" s="19">
         <v>14</v>
       </c>
-      <c r="M23" s="19">
+      <c r="M23" s="18">
         <f t="shared" si="0"/>
         <v>41.300041299999997</v>
       </c>
-      <c r="N23" s="19">
+      <c r="N23" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7359,47 +7630,47 @@
       <c r="C24" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="18">
         <v>37.975037974999999</v>
       </c>
       <c r="F24" t="s">
         <v>97</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="18">
         <v>15.19001519</v>
       </c>
-      <c r="H24" s="19">
+      <c r="H24" s="18">
         <v>0</v>
       </c>
       <c r="J24" t="s">
         <v>97</v>
       </c>
-      <c r="K24" s="20">
+      <c r="K24" s="19">
         <v>9</v>
       </c>
-      <c r="M24" s="19">
+      <c r="M24" s="18">
         <f t="shared" si="0"/>
         <v>37.975037974999999</v>
       </c>
-      <c r="N24" s="19">
+      <c r="N24" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D25" s="19">
+      <c r="D25" s="18">
         <f>SUM(D4:D24)</f>
         <v>32988.914099992209</v>
       </c>
-      <c r="K25" s="19"/>
+      <c r="K25" s="18"/>
       <c r="L25" t="s">
         <v>102</v>
       </c>
-      <c r="M25" s="19">
+      <c r="M25" s="18">
         <f>SUM(M4:M24)</f>
         <v>7470.6214170653802</v>
       </c>
-      <c r="N25" s="19">
+      <c r="N25" s="18">
         <f>SUM(N4:N24)</f>
         <v>25518.29268292684</v>
       </c>
@@ -7415,17 +7686,17 @@
       <c r="L27" t="s">
         <v>101</v>
       </c>
-      <c r="M27" s="19">
+      <c r="M27" s="18">
         <f>M25*0.844</f>
         <v>6305.2044760031804</v>
       </c>
-      <c r="N27" s="19">
+      <c r="N27" s="18">
         <f>N25*0.656</f>
         <v>16740.000000000007</v>
       </c>
     </row>
     <row r="28" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D28" s="19">
+      <c r="D28" s="18">
         <f>SUMPRODUCT(G4:G24,K4:K24)+SUMPRODUCT(H4:H24,K4:K24)</f>
         <v>118760.09075997199</v>
       </c>
@@ -7434,7 +7705,7 @@
       </c>
     </row>
     <row r="29" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D29" s="15">
+      <c r="D29" s="14">
         <f>D28/SUM(G4:H24)</f>
         <v>10.214329996215641</v>
       </c>
@@ -7458,16 +7729,16 @@
       <c r="L30" t="s">
         <v>76</v>
       </c>
-      <c r="M30" s="19">
+      <c r="M30" s="18">
         <v>6305.2044760031904</v>
       </c>
-      <c r="N30" s="19">
+      <c r="N30" s="18">
         <v>16740</v>
       </c>
-      <c r="O30" s="19">
+      <c r="O30" s="18">
         <v>4000</v>
       </c>
-      <c r="P30" s="19">
+      <c r="P30" s="18">
         <v>1069</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Diverse udbygninger, diskret RGK-aktivering
</commit_message>
<xml_diff>
--- a/REFA Forenklet VPO-model.xlsx
+++ b/REFA Forenklet VPO-model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\REFA Affald\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47F7748-BA8C-4E37-967C-FA2B05C7595F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7573BE0-FFB7-4B94-AF83-B320621F2EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{858EECC8-30FB-4D42-A70B-DA5455FDD71D}"/>
   </bookViews>
@@ -22,6 +22,8 @@
     <definedName name="AndelAffald">Model!$C$23</definedName>
     <definedName name="AndelBioaffald">Model!$D$23</definedName>
     <definedName name="ATL">Model!$C$35</definedName>
+    <definedName name="BioAffaldTonnage">Model!$C$22</definedName>
+    <definedName name="BioTonnage">Model!$D$22</definedName>
     <definedName name="CO2afgift">Model!$C$36</definedName>
     <definedName name="CO2indholdAfgift">Model!$C$26</definedName>
     <definedName name="CO2indholdKvote">Model!$C$27</definedName>
@@ -349,8 +351,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="157">
   <si>
     <t>INPUT</t>
   </si>
@@ -833,7 +857,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0,"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -876,6 +900,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -938,7 +969,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -956,9 +987,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -987,12 +1015,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1002,6 +1024,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -1383,7 +1418,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6280117.9904397326</c:v>
+                  <c:v>4648141.7507472299</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1401,16 +1436,16 @@
                   <c:v>471719.80799999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2209465.1303317542</c:v>
+                  <c:v>2093987.8587116271</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17631738.441659246</c:v>
+                  <c:v>15999762.201966742</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8212795.1783317551</c:v>
+                  <c:v>8097317.9067116277</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9418943.2633274905</c:v>
+                  <c:v>7902444.2952551143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1559,13 +1594,13 @@
                   <c:v>7499765</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3822931.3787708599</c:v>
+                  <c:v>3822931.378770859</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>201730.28555860883</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5444927.3260209365</c:v>
+                  <c:v>4029987.0276944069</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1583,16 +1618,16 @@
                   <c:v>418970.96571441251</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1915629.1461956135</c:v>
+                  <c:v>1815509.1559763304</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16969353.990350407</c:v>
+                  <c:v>15554413.692023873</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7692166.617051525</c:v>
+                  <c:v>7592046.6268322412</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9277187.3732988816</c:v>
+                  <c:v>7962367.0651916321</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2195,7 +2230,7 @@
                   <c:v>20264.21052631579</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5142.2449555410485</c:v>
+                  <c:v>5142.2449555410476</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2633,13 +2668,13 @@
                   <c:v>95477</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-124401.0724486527</c:v>
+                  <c:v>-124401.07244865363</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>201730.28555860883</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-835190.66441879608</c:v>
+                  <c:v>-618154.72305282298</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2657,16 +2692,16 @@
                   <c:v>-52748.842285587452</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-293835.98413614067</c:v>
+                  <c:v>-278478.70273529668</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-662384.45130883902</c:v>
+                  <c:v>-445348.50994286872</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-520628.56128023006</c:v>
+                  <c:v>-505271.27987938654</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-141755.89002860896</c:v>
+                  <c:v>59922.769936517812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5056,31 +5091,31 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="31">
+      <c r="B3" s="28">
         <v>1</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="28">
         <v>2</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="28">
         <v>3</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="28">
         <v>4</v>
       </c>
-      <c r="F3" s="31">
+      <c r="F3" s="28">
         <v>5</v>
       </c>
-      <c r="G3" s="31">
+      <c r="G3" s="28">
         <v>6</v>
       </c>
-      <c r="H3" s="31">
+      <c r="H3" s="28">
         <v>7</v>
       </c>
-      <c r="I3" s="31">
+      <c r="I3" s="28">
         <v>8</v>
       </c>
-      <c r="J3" s="31">
+      <c r="J3" s="28">
         <v>9</v>
       </c>
     </row>
@@ -5093,10 +5128,10 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="27" t="s">
         <v>155</v>
       </c>
     </row>
@@ -5152,7 +5187,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -5164,8 +5199,8 @@
     <col min="7" max="7" width="2.85546875" customWidth="1"/>
     <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="18" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="17" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="17" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.28515625" customWidth="1"/>
     <col min="13" max="13" width="2.85546875" customWidth="1"/>
     <col min="14" max="14" width="29.7109375" style="7" customWidth="1"/>
@@ -5173,36 +5208,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="H2" s="29" t="s">
+      <c r="A2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="H2" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="N2" s="29" t="s">
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="N2" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O3" t="e" cm="1">
+        <f t="array" ref="O3">db</f>
+        <v>#NAME?</v>
+      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="6"/>
@@ -5211,11 +5252,11 @@
       <c r="F4" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
       <c r="L4" s="5"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -5225,7 +5266,7 @@
       <c r="B5" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="22">
         <v>1</v>
       </c>
       <c r="F5" t="s">
@@ -5234,21 +5275,21 @@
       <c r="H5" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="21" t="s">
+      <c r="I5" s="10"/>
+      <c r="J5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="21" t="s">
+      <c r="K5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="N5" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="O5" s="26" t="str">
+      <c r="O5" s="25" t="str">
         <f>J13</f>
         <v>Uden RGK</v>
       </c>
-      <c r="P5" s="26" t="str">
+      <c r="P5" s="25" t="str">
         <f>K13</f>
         <v>Med 100% RGK</v>
       </c>
@@ -5258,12 +5299,12 @@
       <c r="H6" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="11"/>
-      <c r="J6" s="18">
+      <c r="I6" s="10"/>
+      <c r="J6" s="17">
         <f>24*C$9</f>
         <v>744</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="17">
         <f>24*D$9</f>
         <v>744</v>
       </c>
@@ -5271,11 +5312,11 @@
         <f>H40</f>
         <v>Varmeproduktion Ovn2</v>
       </c>
-      <c r="O6" s="18">
+      <c r="O6" s="17">
         <f>J40</f>
         <v>7068</v>
       </c>
-      <c r="P6" s="18">
+      <c r="P6" s="17">
         <f>K40</f>
         <v>3850.78947368421</v>
       </c>
@@ -5288,24 +5329,24 @@
       <c r="I7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="21">
         <f>J6*C10</f>
         <v>7068</v>
       </c>
-      <c r="K7" s="22">
+      <c r="K7" s="21">
         <f>K6*D10</f>
         <v>16740</v>
       </c>
-      <c r="L7" s="17"/>
+      <c r="L7" s="16"/>
       <c r="N7" s="7" t="str">
         <f>H41</f>
         <v>Varmeproduktion Ovn3</v>
       </c>
-      <c r="O7" s="18">
+      <c r="O7" s="17">
         <f>J41</f>
         <v>16740</v>
       </c>
-      <c r="P7" s="18">
+      <c r="P7" s="17">
         <f>K41</f>
         <v>20264.21052631579</v>
       </c>
@@ -5314,7 +5355,7 @@
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="11"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="6" t="s">
         <v>1</v>
       </c>
@@ -5330,14 +5371,14 @@
       <c r="H8" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8" s="21">
         <f>EtaRgkOvn2/EtaQNomOvn2*J7</f>
         <v>1488</v>
       </c>
-      <c r="K8" s="22">
+      <c r="K8" s="21">
         <f>EtaRgkOvn2/EtaQNomOvn2*K7</f>
         <v>3524.2105263157891</v>
       </c>
@@ -5345,13 +5386,13 @@
         <f>H43</f>
         <v>Heraf RGK-varme</v>
       </c>
-      <c r="O8" s="18">
+      <c r="O8" s="17">
         <f>J43</f>
         <v>0</v>
       </c>
-      <c r="P8" s="18">
+      <c r="P8" s="17">
         <f>K43</f>
-        <v>5142.2449555410485</v>
+        <v>5142.2449555410476</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -5370,14 +5411,14 @@
       <c r="H9" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="I9" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="22">
+      <c r="J9" s="21">
         <f>SUM(J7:J8)</f>
         <v>8556</v>
       </c>
-      <c r="K9" s="22">
+      <c r="K9" s="21">
         <f>SUM(K7:K8)</f>
         <v>20264.21052631579</v>
       </c>
@@ -5385,11 +5426,11 @@
         <f>H34</f>
         <v>Bortkølet varme</v>
       </c>
-      <c r="O9" s="18">
+      <c r="O9" s="17">
         <f>J34</f>
         <v>0</v>
       </c>
-      <c r="P9" s="18">
+      <c r="P9" s="17">
         <f>K34</f>
         <v>0</v>
       </c>
@@ -5416,11 +5457,11 @@
       <c r="I10" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="17">
         <f>J7/EtaQNomOvn2</f>
         <v>8374.4075829383892</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="17">
         <f>K7/EtaQNomOvn3</f>
         <v>25518.292682926829</v>
       </c>
@@ -5428,11 +5469,11 @@
         <f>H46</f>
         <v>Leveret varme</v>
       </c>
-      <c r="O10" s="18">
+      <c r="O10" s="17">
         <f>J46</f>
         <v>23808</v>
       </c>
-      <c r="P10" s="18">
+      <c r="P10" s="17">
         <f>K46</f>
         <v>24115</v>
       </c>
@@ -5453,26 +5494,26 @@
       <c r="H11" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="22">
+      <c r="J11" s="21">
         <f>J10*3.6/Htotal</f>
-        <v>2955.6732645664906</v>
-      </c>
-      <c r="K11" s="22">
+        <v>2871.2254570074479</v>
+      </c>
+      <c r="K11" s="21">
         <f>K10/(Htotal/3.6)</f>
-        <v>9006.456241033</v>
+        <v>8749.1289198606282</v>
       </c>
       <c r="N11" s="7" t="str">
         <f>H47</f>
         <v>Spidslastvarme</v>
       </c>
-      <c r="O11" s="18">
+      <c r="O11" s="17">
         <f>J47</f>
         <v>4307</v>
       </c>
-      <c r="P11" s="18">
+      <c r="P11" s="17">
         <f>K47</f>
         <v>4000</v>
       </c>
@@ -5488,8 +5529,19 @@
         <v>8</v>
       </c>
       <c r="H12" s="7"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="N12" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="O12" s="24">
+        <f>DBudenRGK</f>
+        <v>7902444.2952551143</v>
+      </c>
+      <c r="P12" s="24">
+        <f>DBmedRGK</f>
+        <v>7962367.0651916321</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -5504,26 +5556,26 @@
       <c r="H13" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="J13" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="K13" s="21" t="str">
+      <c r="K13" s="20" t="str">
         <f>"Med "&amp;TEXT(C5,"0%")&amp;" RGK"</f>
         <v>Med 100% RGK</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="N13" s="27" t="str">
+      <c r="N13" s="26" t="str">
         <f>"Varmemængder: "&amp;C22&amp;" ton affald, "&amp;D22&amp;" ton bioaffald"</f>
         <v>Varmemængder: 12000 ton affald, 0 ton bioaffald</v>
       </c>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -5541,15 +5593,15 @@
       <c r="I14" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J14" s="22">
+      <c r="J14" s="21">
         <f>MIN(Qdemand,K7,EtaQNomOvn3*Ftotal*Htotal/3.6)</f>
         <v>16740</v>
       </c>
-      <c r="K14" s="22">
+      <c r="K14" s="21">
         <f>MIN(Qdemand,K9,EtaQmaxOvn3*Ftotal*Htotal/3.6)</f>
         <v>20264.21052631579</v>
       </c>
-      <c r="L14" s="18">
+      <c r="L14" s="17">
         <f>K14-J14</f>
         <v>3524.21052631579</v>
       </c>
@@ -5572,17 +5624,17 @@
       <c r="I15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="17">
         <f>$J$14/EtaQNomOvn3/(Htotal/3.6)</f>
-        <v>9006.456241033</v>
-      </c>
-      <c r="K15" s="18">
+        <v>8749.1289198606282</v>
+      </c>
+      <c r="K15" s="17">
         <f>$K$14/EtaQmaxOvn3/(Htotal/3.6)</f>
-        <v>8760.9795201777761</v>
-      </c>
-      <c r="L15" s="18">
+        <v>8510.6658196012668</v>
+      </c>
+      <c r="L15" s="17">
         <f t="shared" ref="L15:L55" si="0">K15-J15</f>
-        <v>-245.4767208552239</v>
+        <v>-238.46310025936145</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -5603,15 +5655,15 @@
       <c r="I16" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J16" s="22">
+      <c r="J16" s="21">
         <f>Qdemand-J14</f>
         <v>11375</v>
       </c>
-      <c r="K16" s="22">
+      <c r="K16" s="21">
         <f>Qdemand-K14</f>
         <v>7850.78947368421</v>
       </c>
-      <c r="L16" s="18">
+      <c r="L16" s="17">
         <f t="shared" si="0"/>
         <v>-3524.21052631579</v>
       </c>
@@ -5629,17 +5681,17 @@
       <c r="I17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="22">
+      <c r="J17" s="21">
         <f>Ftotal-J15</f>
-        <v>2993.543758967</v>
-      </c>
-      <c r="K17" s="22">
+        <v>3250.8710801393718</v>
+      </c>
+      <c r="K17" s="21">
         <f>Ftotal-K15</f>
-        <v>3239.0204798222239</v>
-      </c>
-      <c r="L17" s="18">
+        <v>3489.3341803987332</v>
+      </c>
+      <c r="L17" s="17">
         <f t="shared" si="0"/>
-        <v>245.4767208552239</v>
+        <v>238.46310025936145</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -5667,15 +5719,15 @@
       <c r="I18" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J18" s="22">
+      <c r="J18" s="21">
         <f>MIN(J16,NSvarme)</f>
         <v>4000</v>
       </c>
-      <c r="K18" s="22">
+      <c r="K18" s="21">
         <f>MIN(K16,NSvarme)</f>
         <v>4000</v>
       </c>
-      <c r="L18" s="18">
+      <c r="L18" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5688,15 +5740,15 @@
       <c r="I19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J19" s="22">
+      <c r="J19" s="21">
         <f>J16-J18</f>
         <v>7375</v>
       </c>
-      <c r="K19" s="22">
+      <c r="K19" s="21">
         <f>K16-K18</f>
         <v>3850.78947368421</v>
       </c>
-      <c r="L19" s="18">
+      <c r="L19" s="17">
         <f t="shared" si="0"/>
         <v>-3524.21052631579</v>
       </c>
@@ -5720,33 +5772,33 @@
       <c r="I20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J20" s="22">
+      <c r="J20" s="21">
         <f>MIN($J$19,J7,EtaQNomOvn2*(J17*Htotal)/3.6)</f>
         <v>7068</v>
       </c>
-      <c r="K20" s="22">
+      <c r="K20" s="21">
         <f>MIN($K$19,J9,EtaQmaxOvn2*(K17*Htotal)/3.6)</f>
         <v>3850.78947368421</v>
       </c>
-      <c r="L20" s="18">
+      <c r="L20" s="17">
         <f t="shared" si="0"/>
         <v>-3217.21052631579</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="33">
         <v>1</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="33">
         <v>1</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="34">
         <v>1</v>
       </c>
       <c r="H21" s="7" t="s">
@@ -5755,17 +5807,17 @@
       <c r="I21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="22">
+      <c r="J21" s="21">
         <f>$J$20/EtaQNomOvn2/(Htotal/3.6)</f>
-        <v>2955.6732645664906</v>
-      </c>
-      <c r="K21" s="22">
+        <v>2871.2254570074479</v>
+      </c>
+      <c r="K21" s="21">
         <f>$K$20/EtaQNomOvn2/(Htotal/3.6)</f>
-        <v>1610.3106246240077</v>
-      </c>
-      <c r="L21" s="18">
+        <v>1564.3017496347502</v>
+      </c>
+      <c r="L21" s="17">
         <f t="shared" si="0"/>
-        <v>-1345.3626399424829</v>
+        <v>-1306.9237073726977</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -5775,7 +5827,8 @@
       <c r="B22" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="14">
+        <f>F22-BioTonnage</f>
         <v>12000</v>
       </c>
       <c r="D22">
@@ -5784,21 +5837,24 @@
       <c r="E22">
         <v>4000</v>
       </c>
+      <c r="F22">
+        <v>12000</v>
+      </c>
       <c r="H22" s="7" t="s">
         <v>64</v>
       </c>
       <c r="I22" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J22" s="22">
+      <c r="J22" s="21">
         <f>J19-J20</f>
         <v>307</v>
       </c>
-      <c r="K22" s="22">
+      <c r="K22" s="21">
         <f>K19-K20</f>
         <v>0</v>
       </c>
-      <c r="L22" s="18">
+      <c r="L22" s="17">
         <f t="shared" si="0"/>
         <v>-307</v>
       </c>
@@ -5821,17 +5877,17 @@
       <c r="I23" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="22">
+      <c r="J23" s="21">
         <f>J17-J21</f>
-        <v>37.870494400509415</v>
-      </c>
-      <c r="K23" s="22">
+        <v>379.64562313192391</v>
+      </c>
+      <c r="K23" s="21">
         <f>K17-K21</f>
-        <v>1628.7098551982162</v>
-      </c>
-      <c r="L23" s="18">
+        <v>1925.032430763983</v>
+      </c>
+      <c r="L23" s="17">
         <f t="shared" si="0"/>
-        <v>1590.8393607977068</v>
+        <v>1545.3868076320591</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -5842,7 +5898,7 @@
         <v>29</v>
       </c>
       <c r="C24">
-        <v>525</v>
+        <v>400</v>
       </c>
       <c r="D24">
         <f>-6.5*3.6</f>
@@ -5857,15 +5913,15 @@
       <c r="I24" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J24" s="22">
+      <c r="J24" s="21">
         <f>J14+J20</f>
         <v>23808</v>
       </c>
-      <c r="K24" s="22">
+      <c r="K24" s="21">
         <f>K14+K20</f>
         <v>24115</v>
       </c>
-      <c r="L24" s="18">
+      <c r="L24" s="17">
         <f t="shared" si="0"/>
         <v>307</v>
       </c>
@@ -5878,7 +5934,7 @@
         <v>35</v>
       </c>
       <c r="C25">
-        <v>10.199999999999999</v>
+        <v>10.5</v>
       </c>
       <c r="D25">
         <v>14</v>
@@ -5892,15 +5948,15 @@
       <c r="I25" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J25" s="22">
+      <c r="J25" s="21">
         <f>J22</f>
         <v>307</v>
       </c>
-      <c r="K25" s="22">
+      <c r="K25" s="21">
         <f>K22</f>
         <v>0</v>
       </c>
-      <c r="L25" s="18">
+      <c r="L25" s="17">
         <f t="shared" si="0"/>
         <v>-307</v>
       </c>
@@ -5927,15 +5983,15 @@
       <c r="I26" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J26" s="18">
+      <c r="J26" s="17">
         <f>$J$7-$J$20</f>
         <v>0</v>
       </c>
-      <c r="K26" s="18">
+      <c r="K26" s="17">
         <f>J26</f>
         <v>0</v>
       </c>
-      <c r="L26" s="18">
+      <c r="L26" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5962,15 +6018,15 @@
       <c r="I27" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J27" s="18">
+      <c r="J27" s="17">
         <f>$K$7-$J$14</f>
         <v>0</v>
       </c>
-      <c r="K27" s="18">
+      <c r="K27" s="17">
         <f>J27</f>
         <v>0</v>
       </c>
-      <c r="L27" s="18">
+      <c r="L27" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5997,15 +6053,15 @@
       <c r="I28" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J28" s="18">
+      <c r="J28" s="17">
         <f>MIN(J27,EtaQNomOvn3*J23*Htotal/3.6,24*E9*KapQcool)</f>
         <v>0</v>
       </c>
-      <c r="K28" s="18">
+      <c r="K28" s="17">
         <f>MIN(K27,EtaQNomOvn3*K23*Htotal/3.6,24*E9*KapQcool)</f>
         <v>0</v>
       </c>
-      <c r="L28" s="18">
+      <c r="L28" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6020,15 +6076,15 @@
       <c r="I29" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J29" s="18">
+      <c r="J29" s="17">
         <f>J28/EtaQNomOvn3/(Htotal/3.6)</f>
         <v>0</v>
       </c>
-      <c r="K29" s="18">
+      <c r="K29" s="17">
         <f>K28/EtaQNomOvn3/(Htotal/3.6)</f>
         <v>0</v>
       </c>
-      <c r="L29" s="18">
+      <c r="L29" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6049,17 +6105,17 @@
       <c r="I30" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J30" s="18">
+      <c r="J30" s="17">
         <f>J23-J29</f>
-        <v>37.870494400509415</v>
-      </c>
-      <c r="K30" s="18">
+        <v>379.64562313192391</v>
+      </c>
+      <c r="K30" s="17">
         <f>K23-K29</f>
-        <v>1628.7098551982162</v>
-      </c>
-      <c r="L30" s="18">
+        <v>1925.032430763983</v>
+      </c>
+      <c r="L30" s="17">
         <f t="shared" si="0"/>
-        <v>1590.8393607977068</v>
+        <v>1545.3868076320591</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -6078,15 +6134,15 @@
       <c r="I31" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J31" s="18">
+      <c r="J31" s="17">
         <f>MIN(J26,EtaQNomOvn3*J30*Htotal/3.6,24*E9*KapQcool-J28)</f>
         <v>0</v>
       </c>
-      <c r="K31" s="18">
+      <c r="K31" s="17">
         <f>MIN(K26,EtaQNomOvn3*K30*Htotal/3.6,24*E9*KapQcool-K28)</f>
         <v>0</v>
       </c>
-      <c r="L31" s="18">
+      <c r="L31" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6107,15 +6163,15 @@
       <c r="I32" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J32" s="18">
+      <c r="J32" s="17">
         <f>J31/EtaQNomOvn2/(Htotal/3.6)</f>
         <v>0</v>
       </c>
-      <c r="K32" s="18">
+      <c r="K32" s="17">
         <f>K31/EtaQNomOvn2/(Htotal/3.6)</f>
         <v>0</v>
       </c>
-      <c r="L32" s="18">
+      <c r="L32" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6128,7 +6184,7 @@
         <v>44</v>
       </c>
       <c r="C33">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>65</v>
@@ -6136,17 +6192,17 @@
       <c r="I33" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="18">
+      <c r="J33" s="17">
         <f>J30-J32</f>
-        <v>37.870494400509415</v>
-      </c>
-      <c r="K33" s="18">
+        <v>379.64562313192391</v>
+      </c>
+      <c r="K33" s="17">
         <f>K30-K32</f>
-        <v>1628.7098551982162</v>
-      </c>
-      <c r="L33" s="18">
+        <v>1925.032430763983</v>
+      </c>
+      <c r="L33" s="17">
         <f t="shared" si="0"/>
-        <v>1590.8393607977068</v>
+        <v>1545.3868076320591</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
@@ -6165,15 +6221,15 @@
       <c r="I34" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J34" s="18">
+      <c r="J34" s="17">
         <f>J28+J31</f>
         <v>0</v>
       </c>
-      <c r="K34" s="18">
+      <c r="K34" s="17">
         <f>K28+K31</f>
         <v>0</v>
       </c>
-      <c r="L34" s="18">
+      <c r="L34" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6194,28 +6250,28 @@
       <c r="I35" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J35" s="18">
+      <c r="J35" s="17">
         <f>SUM($C$22:$D$22)-J36</f>
-        <v>11962.129505599491</v>
-      </c>
-      <c r="K35" s="18">
+        <v>11620.354376868076</v>
+      </c>
+      <c r="K35" s="17">
         <f>SUM($C$22:$D$22)-K36</f>
-        <v>10371.290144801784</v>
-      </c>
-      <c r="L35" s="18">
+        <v>10074.967569236018</v>
+      </c>
+      <c r="L35" s="17">
         <f t="shared" si="0"/>
-        <v>-1590.8393607977068</v>
-      </c>
-      <c r="N35" s="27" t="str">
+        <v>-1545.3868076320578</v>
+      </c>
+      <c r="N35" s="26" t="str">
         <f>"RGK ift. Nominel: "&amp;C22&amp;" ton affald, "&amp;D22&amp;" ton bioaffald"</f>
         <v>RGK ift. Nominel: 12000 ton affald, 0 ton bioaffald</v>
       </c>
-      <c r="O35" s="12"/>
-      <c r="P35" s="12"/>
-      <c r="Q35" s="12"/>
-      <c r="R35" s="12"/>
-      <c r="S35" s="12"/>
-      <c r="T35" s="12"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+      <c r="T35" s="11"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
@@ -6233,17 +6289,17 @@
       <c r="I36" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J36" s="22">
+      <c r="J36" s="21">
         <f>J23</f>
-        <v>37.870494400509415</v>
-      </c>
-      <c r="K36" s="22">
+        <v>379.64562313192391</v>
+      </c>
+      <c r="K36" s="21">
         <f>K23</f>
-        <v>1628.7098551982162</v>
-      </c>
-      <c r="L36" s="18">
+        <v>1925.032430763983</v>
+      </c>
+      <c r="L36" s="17">
         <f t="shared" si="0"/>
-        <v>1590.8393607977068</v>
+        <v>1545.3868076320591</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
@@ -6253,17 +6309,17 @@
       <c r="I37" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J37" s="18">
+      <c r="J37" s="17">
         <f>EtaE*(J15+J29)*Htotal/3.6</f>
         <v>5733.9603658536589</v>
       </c>
-      <c r="K37" s="18">
+      <c r="K37" s="17">
         <f>EtaE*(K15+K29)*Htotal/3.6</f>
-        <v>5577.6776115211806</v>
-      </c>
-      <c r="L37" s="18">
+        <v>5577.6776115211796</v>
+      </c>
+      <c r="L37" s="17">
         <f t="shared" si="0"/>
-        <v>-156.28275433247836</v>
+        <v>-156.28275433247927</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
@@ -6276,15 +6332,15 @@
       <c r="I38" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J38" s="18">
+      <c r="J38" s="17">
         <f>$D$9*$D$13</f>
         <v>775</v>
       </c>
-      <c r="K38" s="18">
+      <c r="K38" s="17">
         <f>$D$9*$D$13</f>
         <v>775</v>
       </c>
-      <c r="L38" s="18">
+      <c r="L38" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6305,17 +6361,17 @@
       <c r="I39" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J39" s="18">
+      <c r="J39" s="17">
         <f>J37-J38</f>
         <v>4958.9603658536589</v>
       </c>
-      <c r="K39" s="18">
+      <c r="K39" s="17">
         <f>K37-K38</f>
-        <v>4802.6776115211806</v>
-      </c>
-      <c r="L39" s="18">
+        <v>4802.6776115211796</v>
+      </c>
+      <c r="L39" s="17">
         <f t="shared" si="0"/>
-        <v>-156.28275433247836</v>
+        <v>-156.28275433247927</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
@@ -6325,7 +6381,7 @@
       <c r="B40" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="15">
+      <c r="C40" s="14">
         <f>SUM(C22:D22)</f>
         <v>12000</v>
       </c>
@@ -6335,15 +6391,15 @@
       <c r="I40" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J40" s="18">
+      <c r="J40" s="17">
         <f>J20+J31</f>
         <v>7068</v>
       </c>
-      <c r="K40" s="18">
+      <c r="K40" s="17">
         <f>K20+K31</f>
         <v>3850.78947368421</v>
       </c>
-      <c r="L40" s="18">
+      <c r="L40" s="17">
         <f t="shared" si="0"/>
         <v>-3217.21052631579</v>
       </c>
@@ -6355,13 +6411,13 @@
       <c r="B41" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="16">
+      <c r="C41" s="15">
         <f>(C22*LHVaffald+D22*LHVbioaffald)/Ftotal</f>
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D41" s="14">
+        <v>10.5</v>
+      </c>
+      <c r="D41" s="13">
         <f>Htotal/3.6</f>
-        <v>2.833333333333333</v>
+        <v>2.9166666666666665</v>
       </c>
       <c r="H41" t="s">
         <v>121</v>
@@ -6369,15 +6425,15 @@
       <c r="I41" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J41" s="18">
+      <c r="J41" s="17">
         <f>J14+J28</f>
         <v>16740</v>
       </c>
-      <c r="K41" s="18">
+      <c r="K41" s="17">
         <f>K14+K28</f>
         <v>20264.21052631579</v>
       </c>
-      <c r="L41" s="18">
+      <c r="L41" s="17">
         <f t="shared" si="0"/>
         <v>3524.21052631579</v>
       </c>
@@ -6390,15 +6446,15 @@
       <c r="I42" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J42" s="18">
+      <c r="J42" s="17">
         <f>SUM(J40:J41)</f>
         <v>23808</v>
       </c>
-      <c r="K42" s="18">
+      <c r="K42" s="17">
         <f>SUM(K40:K41)</f>
         <v>24115</v>
       </c>
-      <c r="L42" s="18">
+      <c r="L42" s="17">
         <f t="shared" si="0"/>
         <v>307</v>
       </c>
@@ -6410,32 +6466,32 @@
       <c r="I43" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J43" s="18">
-        <v>0</v>
-      </c>
-      <c r="K43" s="18">
+      <c r="J43" s="17">
+        <v>0</v>
+      </c>
+      <c r="K43" s="17">
         <f>(EtaRgkOvn2*K15+EtaRgkOvn3*K21)*Htotal/3.6</f>
-        <v>5142.2449555410485</v>
-      </c>
-      <c r="L43" s="18">
+        <v>5142.2449555410476</v>
+      </c>
+      <c r="L43" s="17">
         <f t="shared" si="0"/>
-        <v>5142.2449555410485</v>
+        <v>5142.2449555410476</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H44" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="J44" s="18">
+      <c r="J44" s="17">
         <v>0</v>
       </c>
       <c r="K44" s="2">
         <f>K43/K45</f>
-        <v>0.17318225802397103</v>
-      </c>
-      <c r="L44" s="18">
+        <v>0.173182258023971</v>
+      </c>
+      <c r="L44" s="17">
         <f t="shared" si="0"/>
-        <v>0.17318225802397103</v>
+        <v>0.173182258023971</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
@@ -6445,15 +6501,15 @@
       <c r="I45" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="J45" s="18">
+      <c r="J45" s="17">
         <f>J42+J37</f>
         <v>29541.960365853658</v>
       </c>
-      <c r="K45" s="18">
+      <c r="K45" s="17">
         <f>K42+K37</f>
         <v>29692.67761152118</v>
       </c>
-      <c r="L45" s="18">
+      <c r="L45" s="17">
         <f t="shared" si="0"/>
         <v>150.71724566752164</v>
       </c>
@@ -6465,15 +6521,15 @@
       <c r="I46" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J46" s="18">
+      <c r="J46" s="17">
         <f>J42-J34</f>
         <v>23808</v>
       </c>
-      <c r="K46" s="18">
+      <c r="K46" s="17">
         <f>K42-K34</f>
         <v>24115</v>
       </c>
-      <c r="L46" s="18">
+      <c r="L46" s="17">
         <f t="shared" si="0"/>
         <v>307</v>
       </c>
@@ -6485,15 +6541,15 @@
       <c r="I47" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J47" s="18">
+      <c r="J47" s="17">
         <f>Qdemand-J46</f>
         <v>4307</v>
       </c>
-      <c r="K47" s="18">
+      <c r="K47" s="17">
         <f>Qdemand-K46</f>
         <v>4000</v>
       </c>
-      <c r="L47" s="18">
+      <c r="L47" s="17">
         <f t="shared" si="0"/>
         <v>-307</v>
       </c>
@@ -6502,7 +6558,7 @@
       <c r="H48" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="L48" s="18"/>
+      <c r="L48" s="17"/>
     </row>
     <row r="49" spans="8:20" x14ac:dyDescent="0.25">
       <c r="H49" t="s">
@@ -6511,15 +6567,15 @@
       <c r="I49" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="J49" s="18">
+      <c r="J49" s="17">
         <f>J$35*$C$23*LHVaffald/3.6</f>
         <v>33892.70026586522</v>
       </c>
-      <c r="K49" s="18">
+      <c r="K49" s="17">
         <f>K$35*$C$23*LHVaffald/3.6</f>
         <v>29385.322076938384</v>
       </c>
-      <c r="L49" s="18">
+      <c r="L49" s="17">
         <f t="shared" si="0"/>
         <v>-4507.3781889268357</v>
       </c>
@@ -6531,15 +6587,15 @@
       <c r="I50" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="J50" s="18">
+      <c r="J50" s="17">
         <f>J$35*AndelBioaffald*LHVbioaffald/3.6</f>
         <v>0</v>
       </c>
-      <c r="K50" s="18">
+      <c r="K50" s="17">
         <f>K$35*AndelBioaffald*LHVbioaffald/3.6</f>
         <v>0</v>
       </c>
-      <c r="L50" s="18">
+      <c r="L50" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6551,15 +6607,15 @@
       <c r="I51" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="J51" s="18">
+      <c r="J51" s="17">
         <f>J45/0.85 - J50</f>
         <v>34755.247489239599</v>
       </c>
-      <c r="K51" s="18">
+      <c r="K51" s="17">
         <f>K45/0.95 - K50</f>
         <v>31255.450117390716</v>
       </c>
-      <c r="L51" s="18">
+      <c r="L51" s="17">
         <f t="shared" si="0"/>
         <v>-3499.7973718488829</v>
       </c>
@@ -6571,15 +6627,15 @@
       <c r="I52" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J52" s="18">
+      <c r="J52" s="17">
         <f>J42*J51/(J51+J50)</f>
         <v>23808</v>
       </c>
-      <c r="K52" s="18">
+      <c r="K52" s="17">
         <f>K42*K51/(K51+K50)</f>
         <v>24115</v>
       </c>
-      <c r="L52" s="18">
+      <c r="L52" s="17">
         <f t="shared" si="0"/>
         <v>307</v>
       </c>
@@ -6591,17 +6647,17 @@
       <c r="I53" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J53" s="18">
+      <c r="J53" s="17">
         <f>J37*J51/(J51+J50)</f>
         <v>5733.9603658536589</v>
       </c>
-      <c r="K53" s="18">
+      <c r="K53" s="17">
         <f>K37*K51/(K51+K50)</f>
-        <v>5577.6776115211806</v>
-      </c>
-      <c r="L53" s="18">
+        <v>5577.6776115211796</v>
+      </c>
+      <c r="L53" s="17">
         <f t="shared" si="0"/>
-        <v>-156.28275433247836</v>
+        <v>-156.28275433247927</v>
       </c>
     </row>
     <row r="54" spans="8:20" x14ac:dyDescent="0.25">
@@ -6611,15 +6667,15 @@
       <c r="I54" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J54" s="18">
+      <c r="J54" s="17">
         <f>J52/1.2</f>
         <v>19840</v>
       </c>
-      <c r="K54" s="18">
+      <c r="K54" s="17">
         <f>(K52-0.1*(K52+K53))/1.2</f>
         <v>17621.443532373236</v>
       </c>
-      <c r="L54" s="18">
+      <c r="L54" s="17">
         <f t="shared" si="0"/>
         <v>-2218.5564676267641</v>
       </c>
@@ -6631,41 +6687,41 @@
       <c r="I55" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J55" s="18">
+      <c r="J55" s="17">
         <f>J54</f>
         <v>19840</v>
       </c>
-      <c r="K55" s="18">
+      <c r="K55" s="17">
         <f>K54</f>
         <v>17621.443532373236</v>
       </c>
-      <c r="L55" s="18">
+      <c r="L55" s="17">
         <f t="shared" si="0"/>
         <v>-2218.5564676267641</v>
       </c>
     </row>
     <row r="56" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="N56" s="27" t="str">
+      <c r="N56" s="26" t="str">
         <f>"Økonomiske nøgletal: "&amp;C22&amp;" ton affald, "&amp;D22&amp;" ton bioaffald"</f>
         <v>Økonomiske nøgletal: 12000 ton affald, 0 ton bioaffald</v>
       </c>
-      <c r="O56" s="12"/>
-      <c r="P56" s="12"/>
-      <c r="Q56" s="12"/>
-      <c r="R56" s="12"/>
-      <c r="S56" s="12"/>
-      <c r="T56" s="12"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="11"/>
+      <c r="R56" s="11"/>
+      <c r="S56" s="11"/>
+      <c r="T56" s="11"/>
     </row>
     <row r="57" spans="8:20" x14ac:dyDescent="0.25">
       <c r="H57" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="I57" s="11"/>
-      <c r="J57" s="21" t="str">
+      <c r="I57" s="10"/>
+      <c r="J57" s="20" t="str">
         <f>J13</f>
         <v>Uden RGK</v>
       </c>
-      <c r="K57" s="21" t="str">
+      <c r="K57" s="20" t="str">
         <f>K13</f>
         <v>Med 100% RGK</v>
       </c>
@@ -6674,274 +6730,274 @@
       </c>
     </row>
     <row r="58" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H58" s="20" t="s">
+      <c r="H58" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="I58" s="20" t="s">
+      <c r="I58" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="J58" s="24">
+      <c r="J58" s="23">
         <f>Varmesalgspris*J46</f>
         <v>7404288</v>
       </c>
-      <c r="K58" s="24">
+      <c r="K58" s="23">
         <f>Varmesalgspris*K46</f>
         <v>7499765</v>
       </c>
-      <c r="L58" s="25">
+      <c r="L58" s="24">
         <f>K58-J58</f>
         <v>95477</v>
       </c>
     </row>
     <row r="59" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H59" s="20" t="s">
+      <c r="H59" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="I59" s="20" t="s">
+      <c r="I59" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="J59" s="24">
+      <c r="J59" s="23">
         <f>(Elpris-ElprodTarif)*J39</f>
         <v>3947332.4512195126</v>
       </c>
-      <c r="K59" s="24">
+      <c r="K59" s="23">
         <f>(Elpris-ElprodTarif)*K39</f>
-        <v>3822931.3787708599</v>
-      </c>
-      <c r="L59" s="25">
+        <v>3822931.378770859</v>
+      </c>
+      <c r="L59" s="24">
         <f t="shared" ref="L59:L72" si="1">K59-J59</f>
-        <v>-124401.0724486527</v>
+        <v>-124401.07244865363</v>
       </c>
     </row>
     <row r="60" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H60" s="20" t="s">
+      <c r="H60" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="I60" s="20" t="s">
+      <c r="I60" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="J60" s="24">
-        <v>0</v>
-      </c>
-      <c r="K60" s="24">
+      <c r="J60" s="23">
+        <v>0</v>
+      </c>
+      <c r="K60" s="23">
         <f>IF(K43&lt;7%*K45,0,10%)*K66</f>
         <v>201730.28555860883</v>
       </c>
-      <c r="L60" s="25">
+      <c r="L60" s="24">
         <f t="shared" si="1"/>
         <v>201730.28555860883</v>
       </c>
     </row>
     <row r="61" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H61" s="20" t="s">
+      <c r="H61" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="I61" s="20" t="s">
+      <c r="I61" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="J61" s="24">
+      <c r="J61" s="23">
         <f>$C$24*($C$22-J36*$C$23)</f>
-        <v>6280117.9904397326</v>
-      </c>
-      <c r="K61" s="24">
+        <v>4648141.7507472299</v>
+      </c>
+      <c r="K61" s="23">
         <f>$C$24*($C$22-K36*$C$23)</f>
-        <v>5444927.3260209365</v>
-      </c>
-      <c r="L61" s="25">
+        <v>4029987.0276944069</v>
+      </c>
+      <c r="L61" s="24">
         <f t="shared" si="1"/>
-        <v>-835190.66441879608</v>
+        <v>-618154.72305282298</v>
       </c>
     </row>
     <row r="62" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="I62" s="20"/>
-      <c r="J62" s="25"/>
-      <c r="K62" s="25"/>
-      <c r="L62" s="25"/>
+      <c r="I62" s="19"/>
+      <c r="J62" s="24"/>
+      <c r="K62" s="24"/>
+      <c r="L62" s="24"/>
     </row>
     <row r="63" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H63" s="20" t="s">
+      <c r="H63" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="I63" s="20" t="s">
+      <c r="I63" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="J63" s="25">
+      <c r="J63" s="24">
         <f>$D$24*($D$22-J36*AndelBioaffald)</f>
         <v>0</v>
       </c>
-      <c r="K63" s="25">
+      <c r="K63" s="24">
         <f>$D$24*($D$22-K36*AndelBioaffald)</f>
         <v>0</v>
       </c>
-      <c r="L63" s="25">
+      <c r="L63" s="24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H64" s="20" t="s">
+      <c r="H64" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="I64" s="20" t="s">
+      <c r="I64" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="J64" s="24">
+      <c r="J64" s="23">
         <f>$C$18*J40+$D$18*J41+$E$18*J34</f>
         <v>1049040</v>
       </c>
-      <c r="K64" s="24">
+      <c r="K64" s="23">
         <f>J64+$F$18*$K$43</f>
         <v>1100462.4495554105</v>
       </c>
-      <c r="L64" s="25">
+      <c r="L64" s="24">
         <f t="shared" si="1"/>
         <v>51422.449555410538</v>
       </c>
     </row>
     <row r="65" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H65" s="20" t="s">
+      <c r="H65" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="I65" s="20" t="s">
+      <c r="I65" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="J65" s="24">
+      <c r="J65" s="23">
         <f>AFV*3.6*J46</f>
         <v>2211287.04</v>
       </c>
-      <c r="K65" s="24">
+      <c r="K65" s="23">
         <f>AFV*3.6*K46</f>
         <v>2239801.2000000002</v>
       </c>
-      <c r="L65" s="25">
+      <c r="L65" s="24">
         <f t="shared" si="1"/>
         <v>28514.160000000149</v>
       </c>
     </row>
     <row r="66" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H66" s="20" t="s">
+      <c r="H66" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="I66" s="20" t="s">
+      <c r="I66" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="J66" s="25">
+      <c r="J66" s="24">
         <f>ATL*3.6*J54</f>
         <v>2271283.2000000002</v>
       </c>
-      <c r="K66" s="25">
+      <c r="K66" s="24">
         <f>ATL*3.6*K54</f>
         <v>2017302.855586088</v>
       </c>
-      <c r="L66" s="25">
+      <c r="L66" s="24">
         <f t="shared" si="1"/>
         <v>-253980.34441391216</v>
       </c>
     </row>
     <row r="67" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H67" s="20" t="s">
+      <c r="H67" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="I67" s="20" t="s">
+      <c r="I67" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="J67" s="25">
+      <c r="J67" s="24">
         <f>CO2afgift*$C$26 /1000 *3.6*J54</f>
         <v>471719.80799999996</v>
       </c>
-      <c r="K67" s="25">
+      <c r="K67" s="24">
         <f>CO2afgift*$C$26 /1000 *3.6*K54</f>
         <v>418970.96571441251</v>
       </c>
-      <c r="L67" s="25">
+      <c r="L67" s="24">
         <f t="shared" si="1"/>
         <v>-52748.842285587452</v>
       </c>
     </row>
     <row r="68" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H68" s="20" t="s">
+      <c r="H68" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="I68" s="20" t="s">
+      <c r="I68" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="J68" s="25">
+      <c r="J68" s="24">
         <f>Kvotepris*$C$27/1000*C28*J35</f>
-        <v>2209465.1303317542</v>
-      </c>
-      <c r="K68" s="25">
+        <v>2093987.8587116271</v>
+      </c>
+      <c r="K68" s="24">
         <f>Kvotepris*$C$27/1000*10.6*K35</f>
-        <v>1915629.1461956135</v>
-      </c>
-      <c r="L68" s="25">
+        <v>1815509.1559763304</v>
+      </c>
+      <c r="L68" s="24">
         <f t="shared" si="1"/>
-        <v>-293835.98413614067</v>
+        <v>-278478.70273529668</v>
       </c>
     </row>
     <row r="69" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="I69" s="20"/>
-      <c r="J69" s="25"/>
-      <c r="K69" s="25"/>
-      <c r="L69" s="25"/>
+      <c r="I69" s="19"/>
+      <c r="J69" s="24"/>
+      <c r="K69" s="24"/>
+      <c r="L69" s="24"/>
     </row>
     <row r="70" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H70" s="20" t="s">
+      <c r="H70" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="I70" s="20" t="s">
+      <c r="I70" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="J70" s="25">
+      <c r="J70" s="24">
         <f>SUM(J58:J61)</f>
-        <v>17631738.441659246</v>
-      </c>
-      <c r="K70" s="25">
+        <v>15999762.201966742</v>
+      </c>
+      <c r="K70" s="24">
         <f>SUM(K58:K61)</f>
-        <v>16969353.990350407</v>
-      </c>
-      <c r="L70" s="25">
+        <v>15554413.692023873</v>
+      </c>
+      <c r="L70" s="24">
         <f t="shared" si="1"/>
-        <v>-662384.45130883902</v>
+        <v>-445348.50994286872</v>
       </c>
     </row>
     <row r="71" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H71" s="20" t="s">
+      <c r="H71" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="I71" s="20" t="s">
+      <c r="I71" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="J71" s="25">
+      <c r="J71" s="24">
         <f>SUM(J63:J68)</f>
-        <v>8212795.1783317551</v>
-      </c>
-      <c r="K71" s="25">
+        <v>8097317.9067116277</v>
+      </c>
+      <c r="K71" s="24">
         <f>SUM(K63:K68)</f>
-        <v>7692166.617051525</v>
-      </c>
-      <c r="L71" s="25">
+        <v>7592046.6268322412</v>
+      </c>
+      <c r="L71" s="24">
         <f t="shared" si="1"/>
-        <v>-520628.56128023006</v>
+        <v>-505271.27987938654</v>
       </c>
     </row>
     <row r="72" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H72" s="20" t="s">
+      <c r="H72" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="I72" s="20" t="s">
+      <c r="I72" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="J72" s="25">
+      <c r="J72" s="24">
         <f>J70-J71</f>
-        <v>9418943.2633274905</v>
-      </c>
-      <c r="K72" s="25">
+        <v>7902444.2952551143</v>
+      </c>
+      <c r="K72" s="24">
         <f>K70-K71</f>
-        <v>9277187.3732988816</v>
-      </c>
-      <c r="L72" s="25">
+        <v>7962367.0651916321</v>
+      </c>
+      <c r="L72" s="24">
         <f t="shared" si="1"/>
-        <v>-141755.89002860896</v>
+        <v>59922.769936517812</v>
       </c>
     </row>
   </sheetData>
@@ -7010,29 +7066,29 @@
       <c r="C4" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <v>11400.2114002</v>
       </c>
       <c r="F4" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="17">
         <v>1382.27949725194</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="17">
         <v>2526.36441138806</v>
       </c>
       <c r="J4" t="s">
         <v>77</v>
       </c>
-      <c r="K4" s="19">
+      <c r="K4" s="18">
         <v>10.5</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="17">
         <f>G4*$K4/3.6</f>
         <v>4031.6485336514916</v>
       </c>
-      <c r="N4" s="18">
+      <c r="N4" s="17">
         <f>H4*$K4/3.6</f>
         <v>7368.5628665485083</v>
       </c>
@@ -7041,29 +7097,29 @@
       <c r="C5" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <v>0</v>
       </c>
       <c r="F5" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="18">
-        <v>0</v>
-      </c>
-      <c r="H5" s="18">
+      <c r="G5" s="17">
+        <v>0</v>
+      </c>
+      <c r="H5" s="17">
         <v>0</v>
       </c>
       <c r="J5" t="s">
         <v>78</v>
       </c>
-      <c r="K5" s="19">
+      <c r="K5" s="18">
         <v>10.5</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="17">
         <f t="shared" ref="M5:M24" si="0">G5*$K5/3.6</f>
         <v>0</v>
       </c>
-      <c r="N5" s="18">
+      <c r="N5" s="17">
         <f t="shared" ref="N5:N24" si="1">H5*$K5/3.6</f>
         <v>0</v>
       </c>
@@ -7072,29 +7128,29 @@
       <c r="C6" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <v>0</v>
       </c>
       <c r="F6" t="s">
         <v>79</v>
       </c>
-      <c r="G6" s="18">
-        <v>0</v>
-      </c>
-      <c r="H6" s="18">
+      <c r="G6" s="17">
+        <v>0</v>
+      </c>
+      <c r="H6" s="17">
         <v>0</v>
       </c>
       <c r="J6" t="s">
         <v>79</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="18">
         <v>10.5</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N6" s="18">
+      <c r="N6" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7103,29 +7159,29 @@
       <c r="C7" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <v>6154.3428210033298</v>
       </c>
       <c r="F7" t="s">
         <v>80</v>
       </c>
-      <c r="G7" s="18">
-        <v>0</v>
-      </c>
-      <c r="H7" s="18">
+      <c r="G7" s="17">
+        <v>0</v>
+      </c>
+      <c r="H7" s="17">
         <v>2356.9823569800001</v>
       </c>
       <c r="J7" t="s">
         <v>80</v>
       </c>
-      <c r="K7" s="19">
+      <c r="K7" s="18">
         <v>9.4</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="17">
         <f t="shared" si="1"/>
         <v>6154.3428210033335</v>
       </c>
@@ -7134,29 +7190,29 @@
       <c r="C8" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <v>1276.2179428833299</v>
       </c>
       <c r="F8" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="17">
         <v>437.56043756000003</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="17">
         <v>0</v>
       </c>
       <c r="J8" t="s">
         <v>81</v>
       </c>
-      <c r="K8" s="19">
+      <c r="K8" s="18">
         <v>10.5</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="17">
         <f t="shared" si="0"/>
         <v>1276.2179428833335</v>
       </c>
-      <c r="N8" s="18">
+      <c r="N8" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7165,29 +7221,29 @@
       <c r="C9" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <v>0</v>
       </c>
       <c r="F9" t="s">
         <v>82</v>
       </c>
-      <c r="G9" s="18">
-        <v>0</v>
-      </c>
-      <c r="H9" s="18">
+      <c r="G9" s="17">
+        <v>0</v>
+      </c>
+      <c r="H9" s="17">
         <v>0</v>
       </c>
       <c r="J9" t="s">
         <v>82</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="18">
         <v>14.5</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N9" s="18">
+      <c r="N9" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7196,29 +7252,29 @@
       <c r="C10" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="17">
         <v>972.20097220000002</v>
       </c>
       <c r="F10" t="s">
         <v>83</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="17">
         <v>291.66029165999998</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="17">
         <v>0</v>
       </c>
       <c r="J10" t="s">
         <v>83</v>
       </c>
-      <c r="K10" s="19">
+      <c r="K10" s="18">
         <v>12</v>
       </c>
-      <c r="M10" s="18">
+      <c r="M10" s="17">
         <f t="shared" si="0"/>
         <v>972.20097219999991</v>
       </c>
-      <c r="N10" s="18">
+      <c r="N10" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7227,29 +7283,29 @@
       <c r="C11" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="17">
         <v>15.375015375</v>
       </c>
       <c r="F11" t="s">
         <v>84</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="17">
         <v>6.1500061500000003</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="17">
         <v>0</v>
       </c>
       <c r="J11" t="s">
         <v>84</v>
       </c>
-      <c r="K11" s="19">
+      <c r="K11" s="18">
         <v>9</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="17">
         <f t="shared" si="0"/>
         <v>15.375015375</v>
       </c>
-      <c r="N11" s="18">
+      <c r="N11" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7258,29 +7314,29 @@
       <c r="C12" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="17">
         <v>785.27856305555599</v>
       </c>
       <c r="F12" t="s">
         <v>85</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="17">
         <v>257.00025699999998</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="17">
         <v>0</v>
       </c>
       <c r="J12" t="s">
         <v>85</v>
       </c>
-      <c r="K12" s="19">
+      <c r="K12" s="18">
         <v>11</v>
       </c>
-      <c r="M12" s="18">
+      <c r="M12" s="17">
         <f t="shared" si="0"/>
         <v>785.27856305555542</v>
       </c>
-      <c r="N12" s="18">
+      <c r="N12" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7289,29 +7345,29 @@
       <c r="C13" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="17">
         <v>60.1667268333333</v>
       </c>
       <c r="F13" t="s">
         <v>86</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="17">
         <v>22.800022800000001</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="17">
         <v>0</v>
       </c>
       <c r="J13" t="s">
         <v>86</v>
       </c>
-      <c r="K13" s="19">
+      <c r="K13" s="18">
         <v>9.5</v>
       </c>
-      <c r="M13" s="18">
+      <c r="M13" s="17">
         <f t="shared" si="0"/>
         <v>60.166726833333335</v>
       </c>
-      <c r="N13" s="18">
+      <c r="N13" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7320,29 +7376,29 @@
       <c r="C14" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="17">
         <v>2540.00254</v>
       </c>
       <c r="F14" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="18">
-        <v>0</v>
-      </c>
-      <c r="H14" s="18">
+      <c r="G14" s="17">
+        <v>0</v>
+      </c>
+      <c r="H14" s="17">
         <v>1016.001016</v>
       </c>
       <c r="J14" t="s">
         <v>87</v>
       </c>
-      <c r="K14" s="19">
+      <c r="K14" s="18">
         <v>9</v>
       </c>
-      <c r="M14" s="18">
+      <c r="M14" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N14" s="18">
+      <c r="N14" s="17">
         <f t="shared" si="1"/>
         <v>2540.00254</v>
       </c>
@@ -7351,29 +7407,29 @@
       <c r="C15" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="17">
         <v>45.100045100000003</v>
       </c>
       <c r="F15" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="18">
-        <v>0</v>
-      </c>
-      <c r="H15" s="18">
+      <c r="G15" s="17">
+        <v>0</v>
+      </c>
+      <c r="H15" s="17">
         <v>13.53001353</v>
       </c>
       <c r="J15" t="s">
         <v>88</v>
       </c>
-      <c r="K15" s="19">
+      <c r="K15" s="18">
         <v>12</v>
       </c>
-      <c r="M15" s="18">
+      <c r="M15" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N15" s="18">
+      <c r="N15" s="17">
         <f t="shared" si="1"/>
         <v>45.100045100000003</v>
       </c>
@@ -7382,29 +7438,29 @@
       <c r="C16" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="17">
         <v>18.861129972222201</v>
       </c>
       <c r="F16" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="17">
         <v>6.7900067899999996</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="17">
         <v>0</v>
       </c>
       <c r="J16" t="s">
         <v>89</v>
       </c>
-      <c r="K16" s="19">
+      <c r="K16" s="18">
         <v>10</v>
       </c>
-      <c r="M16" s="18">
+      <c r="M16" s="17">
         <f t="shared" si="0"/>
         <v>18.861129972222219</v>
       </c>
-      <c r="N16" s="18">
+      <c r="N16" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7413,29 +7469,29 @@
       <c r="C17" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="17">
         <v>0</v>
       </c>
       <c r="F17" t="s">
         <v>90</v>
       </c>
-      <c r="G17" s="18">
-        <v>0</v>
-      </c>
-      <c r="H17" s="18">
+      <c r="G17" s="17">
+        <v>0</v>
+      </c>
+      <c r="H17" s="17">
         <v>0</v>
       </c>
       <c r="J17" t="s">
         <v>90</v>
       </c>
-      <c r="K17" s="19">
+      <c r="K17" s="18">
         <v>11</v>
       </c>
-      <c r="M17" s="18">
+      <c r="M17" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N17" s="18">
+      <c r="N17" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7444,29 +7500,29 @@
       <c r="C18" t="s">
         <v>91</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="17">
         <v>9410.2844102750005</v>
       </c>
       <c r="F18" t="s">
         <v>91</v>
       </c>
-      <c r="G18" s="18">
-        <v>0</v>
-      </c>
-      <c r="H18" s="18">
+      <c r="G18" s="17">
+        <v>0</v>
+      </c>
+      <c r="H18" s="17">
         <v>3226.38322638</v>
       </c>
       <c r="J18" t="s">
         <v>91</v>
       </c>
-      <c r="K18" s="19">
+      <c r="K18" s="18">
         <v>10.5</v>
       </c>
-      <c r="M18" s="18">
+      <c r="M18" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N18" s="18">
+      <c r="N18" s="17">
         <f t="shared" si="1"/>
         <v>9410.2844102750005</v>
       </c>
@@ -7475,29 +7531,29 @@
       <c r="C19" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="17">
         <v>0</v>
       </c>
       <c r="F19" t="s">
         <v>92</v>
       </c>
-      <c r="G19" s="18">
-        <v>0</v>
-      </c>
-      <c r="H19" s="18">
+      <c r="G19" s="17">
+        <v>0</v>
+      </c>
+      <c r="H19" s="17">
         <v>0</v>
       </c>
       <c r="J19" t="s">
         <v>92</v>
       </c>
-      <c r="K19" s="19">
+      <c r="K19" s="18">
         <v>10.5</v>
       </c>
-      <c r="M19" s="18">
+      <c r="M19" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N19" s="18">
+      <c r="N19" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7506,29 +7562,29 @@
       <c r="C20" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="17">
         <v>0</v>
       </c>
       <c r="F20" t="s">
         <v>93</v>
       </c>
-      <c r="G20" s="18">
-        <v>0</v>
-      </c>
-      <c r="H20" s="18">
+      <c r="G20" s="17">
+        <v>0</v>
+      </c>
+      <c r="H20" s="17">
         <v>0</v>
       </c>
       <c r="J20" t="s">
         <v>93</v>
       </c>
-      <c r="K20" s="19">
+      <c r="K20" s="18">
         <v>13</v>
       </c>
-      <c r="M20" s="18">
+      <c r="M20" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N20" s="18">
+      <c r="N20" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7537,29 +7593,29 @@
       <c r="C21" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="17">
         <v>231.59745381944401</v>
       </c>
       <c r="F21" t="s">
         <v>94</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="17">
         <v>57.500057499999997</v>
       </c>
-      <c r="H21" s="18">
+      <c r="H21" s="17">
         <v>0</v>
       </c>
       <c r="J21" t="s">
         <v>94</v>
       </c>
-      <c r="K21" s="19">
+      <c r="K21" s="18">
         <v>14.5</v>
       </c>
-      <c r="M21" s="18">
+      <c r="M21" s="17">
         <f t="shared" si="0"/>
         <v>231.59745381944444</v>
       </c>
-      <c r="N21" s="18">
+      <c r="N21" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7568,29 +7624,29 @@
       <c r="C22" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="17">
         <v>0</v>
       </c>
       <c r="F22" t="s">
         <v>95</v>
       </c>
-      <c r="G22" s="18">
-        <v>0</v>
-      </c>
-      <c r="H22" s="18">
+      <c r="G22" s="17">
+        <v>0</v>
+      </c>
+      <c r="H22" s="17">
         <v>0</v>
       </c>
       <c r="J22" t="s">
         <v>95</v>
       </c>
-      <c r="K22" s="19">
+      <c r="K22" s="18">
         <v>14.7</v>
       </c>
-      <c r="M22" s="18">
+      <c r="M22" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N22" s="18">
+      <c r="N22" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7599,29 +7655,29 @@
       <c r="C23" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="17">
         <v>41.300041299999997</v>
       </c>
       <c r="F23" t="s">
         <v>96</v>
       </c>
-      <c r="G23" s="18">
+      <c r="G23" s="17">
         <v>10.62001062</v>
       </c>
-      <c r="H23" s="18">
+      <c r="H23" s="17">
         <v>0</v>
       </c>
       <c r="J23" t="s">
         <v>96</v>
       </c>
-      <c r="K23" s="19">
+      <c r="K23" s="18">
         <v>14</v>
       </c>
-      <c r="M23" s="18">
+      <c r="M23" s="17">
         <f t="shared" si="0"/>
         <v>41.300041299999997</v>
       </c>
-      <c r="N23" s="18">
+      <c r="N23" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7630,47 +7686,47 @@
       <c r="C24" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="17">
         <v>37.975037974999999</v>
       </c>
       <c r="F24" t="s">
         <v>97</v>
       </c>
-      <c r="G24" s="18">
+      <c r="G24" s="17">
         <v>15.19001519</v>
       </c>
-      <c r="H24" s="18">
+      <c r="H24" s="17">
         <v>0</v>
       </c>
       <c r="J24" t="s">
         <v>97</v>
       </c>
-      <c r="K24" s="19">
+      <c r="K24" s="18">
         <v>9</v>
       </c>
-      <c r="M24" s="18">
+      <c r="M24" s="17">
         <f t="shared" si="0"/>
         <v>37.975037974999999</v>
       </c>
-      <c r="N24" s="18">
+      <c r="N24" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D25" s="18">
+      <c r="D25" s="17">
         <f>SUM(D4:D24)</f>
         <v>32988.914099992209</v>
       </c>
-      <c r="K25" s="18"/>
+      <c r="K25" s="17"/>
       <c r="L25" t="s">
         <v>102</v>
       </c>
-      <c r="M25" s="18">
+      <c r="M25" s="17">
         <f>SUM(M4:M24)</f>
         <v>7470.6214170653802</v>
       </c>
-      <c r="N25" s="18">
+      <c r="N25" s="17">
         <f>SUM(N4:N24)</f>
         <v>25518.29268292684</v>
       </c>
@@ -7686,17 +7742,17 @@
       <c r="L27" t="s">
         <v>101</v>
       </c>
-      <c r="M27" s="18">
+      <c r="M27" s="17">
         <f>M25*0.844</f>
         <v>6305.2044760031804</v>
       </c>
-      <c r="N27" s="18">
+      <c r="N27" s="17">
         <f>N25*0.656</f>
         <v>16740.000000000007</v>
       </c>
     </row>
     <row r="28" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D28" s="18">
+      <c r="D28" s="17">
         <f>SUMPRODUCT(G4:G24,K4:K24)+SUMPRODUCT(H4:H24,K4:K24)</f>
         <v>118760.09075997199</v>
       </c>
@@ -7705,7 +7761,7 @@
       </c>
     </row>
     <row r="29" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D29" s="14">
+      <c r="D29" s="13">
         <f>D28/SUM(G4:H24)</f>
         <v>10.214329996215641</v>
       </c>
@@ -7729,16 +7785,16 @@
       <c r="L30" t="s">
         <v>76</v>
       </c>
-      <c r="M30" s="18">
+      <c r="M30" s="17">
         <v>6305.2044760031904</v>
       </c>
-      <c r="N30" s="18">
+      <c r="N30" s="17">
         <v>16740</v>
       </c>
-      <c r="O30" s="18">
+      <c r="O30" s="17">
         <v>4000</v>
       </c>
-      <c r="P30" s="18">
+      <c r="P30" s="17">
         <v>1069</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Indsat kolonner med mellemregninger
</commit_message>
<xml_diff>
--- a/REFA Forenklet VPO-model.xlsx
+++ b/REFA Forenklet VPO-model.xlsx
@@ -8,9 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\REFA Affald\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7573BE0-FFB7-4B94-AF83-B320621F2EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C52EC4-B121-471A-9242-22A4A41DA308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{858EECC8-30FB-4D42-A70B-DA5455FDD71D}"/>
+    <workbookView xWindow="-15" yWindow="0" windowWidth="14550" windowHeight="15510" activeTab="1" xr2:uid="{16E12CA9-1556-4394-AFAE-8F484516E35F}"/>
   </bookViews>
   <sheets>
     <sheet name="SolverRepos" sheetId="3" r:id="rId1"/>
@@ -351,30 +352,8 @@
 </comments>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="169">
   <si>
     <t>INPUT</t>
   </si>
@@ -845,6 +824,42 @@
   </si>
   <si>
     <t>Restriktioner</t>
+  </si>
+  <si>
+    <t>MELLEMREGNINGER</t>
+  </si>
+  <si>
+    <t>Affaldsforbrug Ovn3</t>
+  </si>
+  <si>
+    <t>Nordic Sugar varme</t>
+  </si>
+  <si>
+    <t>Affaldsforbrug Ovn2</t>
+  </si>
+  <si>
+    <t>Ikke-udnyttet affald</t>
+  </si>
+  <si>
+    <t>Udnyttet affald</t>
+  </si>
+  <si>
+    <t>Brændselsmængder</t>
+  </si>
+  <si>
+    <t>Kapacitetsudnyttelse</t>
+  </si>
+  <si>
+    <t>Ovn3 tonnage</t>
+  </si>
+  <si>
+    <t>Ovn2 tonnage</t>
+  </si>
+  <si>
+    <t>Bortkøleanlæg varme</t>
+  </si>
+  <si>
+    <t>SUM</t>
   </si>
 </sst>
 </file>
@@ -909,7 +924,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -936,6 +951,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -969,7 +990,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -996,7 +1017,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2"/>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1009,9 +1029,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1024,12 +1041,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1037,13 +1048,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1078,11 +1109,11 @@
     <c:title>
       <c:tx>
         <c:strRef>
-          <c:f>Model!$N$56</c:f>
+          <c:f>Model!$T$47</c:f>
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Økonomiske nøgletal: 12000 ton affald, 0 ton bioaffald</c:v>
+              <c:v>Økonomiske nøgletal: 15000 ton affald, 0 ton bioaffald</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -1591,43 +1622,43 @@
                 <c:formatCode>#,##0,</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>7499765</c:v>
+                  <c:v>9139668</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3822931.378770859</c:v>
+                  <c:v>3947332.4512195126</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>201730.28555860883</c:v>
+                  <c:v>246855.16981097564</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4029987.0276944069</c:v>
+                  <c:v>4648141.7507472299</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1100462.4495554105</c:v>
+                  <c:v>1107810.8046975606</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2239801.2000000002</c:v>
+                  <c:v>2729557.4400000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2017302.855586088</c:v>
+                  <c:v>2468551.6981097562</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>418970.96571441251</c:v>
+                  <c:v>512690.2418291159</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1815509.1559763304</c:v>
+                  <c:v>2093987.8587116271</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15554413.692023873</c:v>
+                  <c:v>17981997.371777717</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7592046.6268322412</c:v>
+                  <c:v>8912598.0433480591</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7962367.0651916321</c:v>
+                  <c:v>9069399.328429658</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1925,11 +1956,11 @@
     <c:title>
       <c:tx>
         <c:strRef>
-          <c:f>Model!$N$13</c:f>
+          <c:f>Model!$T$4</c:f>
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Varmemængder: 12000 ton affald, 0 ton bioaffald</c:v>
+              <c:v>Varmemængder: 15000 ton affald, 0 ton bioaffald</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -1975,12 +2006,9 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Model!$O$5</c:f>
+              <c:f>Model!$P$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Uden RGK</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -2053,7 +2081,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Model!$N$6:$N$11</c:f>
+              <c:f>Model!$N$22:$N$27</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2079,7 +2107,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Model!$O$6:$O$11</c:f>
+              <c:f>Model!$P$22:$P$27</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2099,7 +2127,7 @@
                   <c:v>23808</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4307</c:v>
+                  <c:v>11192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2115,12 +2143,9 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Model!$P$5</c:f>
+              <c:f>Model!$Q$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Med 100% RGK</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -2193,7 +2218,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Model!$N$6:$N$11</c:f>
+              <c:f>Model!$N$22:$N$27</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2219,27 +2244,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Model!$P$6:$P$11</c:f>
+              <c:f>Model!$Q$22:$Q$27</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3850.78947368421</c:v>
+                  <c:v>8556</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20264.21052631579</c:v>
+                  <c:v>20832</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5142.2449555410476</c:v>
+                  <c:v>5877.080469756057</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24115</c:v>
+                  <c:v>29388</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4000</c:v>
+                  <c:v>5612</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2474,11 +2499,11 @@
     <c:title>
       <c:tx>
         <c:strRef>
-          <c:f>Model!$N$35</c:f>
+          <c:f>Model!$T$26</c:f>
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>RGK ift. Nominel: 12000 ton affald, 0 ton bioaffald</c:v>
+              <c:v>RGK ift. Nominel: 15000 ton affald, 0 ton bioaffald</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -2665,43 +2690,43 @@
                 <c:formatCode>#,##0,</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>95477</c:v>
+                  <c:v>1735380</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-124401.07244865363</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>201730.28555860883</c:v>
+                  <c:v>246855.16981097564</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-618154.72305282298</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51422.449555410538</c:v>
+                  <c:v>58770.804697560612</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28514.160000000149</c:v>
+                  <c:v>518270.40000000037</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-253980.34441391216</c:v>
+                  <c:v>197268.49810975604</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-52748.842285587452</c:v>
+                  <c:v>40970.433829115937</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-278478.70273529668</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-445348.50994286872</c:v>
+                  <c:v>1982235.169810975</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-505271.27987938654</c:v>
+                  <c:v>815280.13663643133</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>59922.769936517812</c:v>
+                  <c:v>1166955.0331745436</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4590,13 +4615,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>525413</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>151778</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>34</xdr:col>
       <xdr:colOff>99958</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>132728</xdr:rowOff>
@@ -4661,15 +4686,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>12324</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>38098</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>585972</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>18598</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4697,15 +4722,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>14007</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>587655</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>190050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4733,15 +4758,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>11206</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>22412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>584854</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>2912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5074,6 +5099,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5091,31 +5117,31 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="28">
+      <c r="B3" s="26">
         <v>1</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="26">
         <v>2</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="26">
         <v>3</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="26">
         <v>4</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="26">
         <v>5</v>
       </c>
-      <c r="G3" s="28">
+      <c r="G3" s="26">
         <v>6</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="26">
         <v>7</v>
       </c>
-      <c r="I3" s="28">
+      <c r="I3" s="26">
         <v>8</v>
       </c>
-      <c r="J3" s="28">
+      <c r="J3" s="26">
         <v>9</v>
       </c>
     </row>
@@ -5128,10 +5154,10 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="25" t="s">
         <v>155</v>
       </c>
     </row>
@@ -5181,13 +5207,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5354189-028E-4B88-AC75-E88799B17CAC}">
-  <dimension ref="A2:T72"/>
+  <dimension ref="A2:Z72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -5197,49 +5223,56 @@
     <col min="3" max="5" width="9.140625" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="2.85546875" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="17" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="2.85546875" customWidth="1"/>
-    <col min="14" max="14" width="29.7109375" style="7" customWidth="1"/>
-    <col min="15" max="16" width="13" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="11" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="13.28515625" style="16" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="14.42578125" style="16" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="2.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.140625" customWidth="1"/>
+    <col min="20" max="20" width="29.7109375" style="7" customWidth="1"/>
+    <col min="21" max="22" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="H2" s="31" t="s">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="H2" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="N2" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="N2" s="31" t="s">
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="T2" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="O3" t="e" cm="1">
-        <f t="array" ref="O3">db</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>139</v>
       </c>
@@ -5255,18 +5288,46 @@
       <c r="I4" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
       <c r="L4" s="5"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N4" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" s="19" t="str">
+        <f>J57</f>
+        <v>Uden RGK</v>
+      </c>
+      <c r="Q4" s="19" t="str">
+        <f t="shared" ref="Q4:R4" si="0">K57</f>
+        <v>Med 100% RGK</v>
+      </c>
+      <c r="R4" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>RGK ift. nominel</v>
+      </c>
+      <c r="T4" s="24" t="str">
+        <f>"Varmemængder: "&amp;C22&amp;" ton affald, "&amp;D22&amp;" ton bioaffald"</f>
+        <v>Varmemængder: 15000 ton affald, 0 ton bioaffald</v>
+      </c>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>138</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="21">
         <v>1</v>
       </c>
       <c r="F5" t="s">
@@ -5276,52 +5337,72 @@
         <v>144</v>
       </c>
       <c r="I5" s="10"/>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="K5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="O5" s="25" t="str">
-        <f>J13</f>
-        <v>Uden RGK</v>
-      </c>
-      <c r="P5" s="25" t="str">
-        <f>K13</f>
-        <v>Med 100% RGK</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L5" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="N5" s="18" t="str">
+        <f>H70</f>
+        <v>Indtægter total</v>
+      </c>
+      <c r="O5" s="18" t="str">
+        <f>I70</f>
+        <v>tkr</v>
+      </c>
+      <c r="P5" s="23">
+        <f>J70</f>
+        <v>15999762.201966742</v>
+      </c>
+      <c r="Q5" s="23">
+        <f>K70</f>
+        <v>17981997.371777717</v>
+      </c>
+      <c r="R5" s="23">
+        <f>L70</f>
+        <v>1982235.169810975</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="H6" s="8" t="s">
         <v>57</v>
       </c>
       <c r="I6" s="10"/>
-      <c r="J6" s="17">
+      <c r="J6" s="16">
         <f>24*C$9</f>
         <v>744</v>
       </c>
-      <c r="K6" s="17">
+      <c r="K6" s="16">
         <f>24*D$9</f>
         <v>744</v>
       </c>
-      <c r="N6" s="7" t="str">
-        <f>H40</f>
-        <v>Varmeproduktion Ovn2</v>
-      </c>
-      <c r="O6" s="17">
-        <f>J40</f>
-        <v>7068</v>
-      </c>
-      <c r="P6" s="17">
-        <f>K40</f>
-        <v>3850.78947368421</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N6" s="18" t="str">
+        <f>H71</f>
+        <v>Omkostninger total</v>
+      </c>
+      <c r="O6" s="18" t="str">
+        <f>I71</f>
+        <v>tkr</v>
+      </c>
+      <c r="P6" s="23">
+        <f>J71</f>
+        <v>8097317.9067116277</v>
+      </c>
+      <c r="Q6" s="23">
+        <f>K71</f>
+        <v>8912598.0433480591</v>
+      </c>
+      <c r="R6" s="23">
+        <f>L71</f>
+        <v>815280.13663643133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="H7" s="8" t="s">
         <v>58</v>
@@ -5329,29 +5410,40 @@
       <c r="I7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="21">
+      <c r="J7" s="20">
         <f>J6*C10</f>
         <v>7068</v>
       </c>
-      <c r="K7" s="21">
+      <c r="K7" s="20">
         <f>K6*D10</f>
         <v>16740</v>
       </c>
-      <c r="L7" s="16"/>
-      <c r="N7" s="7" t="str">
-        <f>H41</f>
-        <v>Varmeproduktion Ovn3</v>
-      </c>
-      <c r="O7" s="17">
-        <f>J41</f>
-        <v>16740</v>
-      </c>
-      <c r="P7" s="17">
-        <f>K41</f>
-        <v>20264.21052631579</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L7" s="20">
+        <f>SUM(J7:K7)</f>
+        <v>23808</v>
+      </c>
+      <c r="N7" s="18" t="str">
+        <f>H72</f>
+        <v>Dækningsbidrag</v>
+      </c>
+      <c r="O7" s="18" t="str">
+        <f>I72</f>
+        <v>tkr</v>
+      </c>
+      <c r="P7" s="23">
+        <f>J72</f>
+        <v>7902444.2952551143</v>
+      </c>
+      <c r="Q7" s="23">
+        <f>K72</f>
+        <v>9069399.328429658</v>
+      </c>
+      <c r="R7" s="23">
+        <f>L72</f>
+        <v>1166955.0331745436</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -5371,31 +5463,28 @@
       <c r="H8" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="20">
         <f>EtaRgkOvn2/EtaQNomOvn2*J7</f>
         <v>1488</v>
       </c>
-      <c r="K8" s="21">
-        <f>EtaRgkOvn2/EtaQNomOvn2*K7</f>
-        <v>3524.2105263157891</v>
-      </c>
-      <c r="N8" s="7" t="str">
-        <f>H43</f>
-        <v>Heraf RGK-varme</v>
-      </c>
-      <c r="O8" s="17">
-        <f>J43</f>
-        <v>0</v>
-      </c>
-      <c r="P8" s="17">
-        <f>K43</f>
-        <v>5142.2449555410476</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K8" s="20">
+        <f>EtaRgkOvn3/EtaQNomOvn3*K7</f>
+        <v>4092</v>
+      </c>
+      <c r="L8" s="20">
+        <f t="shared" ref="L8:L11" si="1">SUM(J8:K8)</f>
+        <v>5580</v>
+      </c>
+      <c r="N8" s="5"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -5411,31 +5500,43 @@
       <c r="H9" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="20">
         <f>SUM(J7:J8)</f>
         <v>8556</v>
       </c>
-      <c r="K9" s="21">
+      <c r="K9" s="20">
         <f>SUM(K7:K8)</f>
-        <v>20264.21052631579</v>
-      </c>
-      <c r="N9" s="7" t="str">
-        <f>H34</f>
-        <v>Bortkølet varme</v>
-      </c>
-      <c r="O9" s="17">
-        <f>J34</f>
-        <v>0</v>
-      </c>
-      <c r="P9" s="17">
-        <f>K34</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+        <v>20832</v>
+      </c>
+      <c r="L9" s="20">
+        <f t="shared" si="1"/>
+        <v>29388</v>
+      </c>
+      <c r="N9" s="18" t="str">
+        <f>H58</f>
+        <v>Varmesalg</v>
+      </c>
+      <c r="O9" s="18" t="str">
+        <f t="shared" ref="O9:R12" si="2">I58</f>
+        <v>tkr</v>
+      </c>
+      <c r="P9" s="22">
+        <f t="shared" si="2"/>
+        <v>7404288</v>
+      </c>
+      <c r="Q9" s="22">
+        <f t="shared" si="2"/>
+        <v>9139668</v>
+      </c>
+      <c r="R9" s="23">
+        <f t="shared" si="2"/>
+        <v>1735380</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
@@ -5457,28 +5558,40 @@
       <c r="I10" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="16">
         <f>J7/EtaQNomOvn2</f>
         <v>8374.4075829383892</v>
       </c>
-      <c r="K10" s="17">
+      <c r="K10" s="16">
         <f>K7/EtaQNomOvn3</f>
         <v>25518.292682926829</v>
       </c>
-      <c r="N10" s="7" t="str">
-        <f>H46</f>
-        <v>Leveret varme</v>
-      </c>
-      <c r="O10" s="17">
-        <f>J46</f>
-        <v>23808</v>
-      </c>
-      <c r="P10" s="17">
-        <f>K46</f>
-        <v>24115</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L10" s="20">
+        <f t="shared" si="1"/>
+        <v>33892.70026586522</v>
+      </c>
+      <c r="N10" s="18" t="str">
+        <f>H59</f>
+        <v>Elsalg</v>
+      </c>
+      <c r="O10" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>tkr</v>
+      </c>
+      <c r="P10" s="22">
+        <f t="shared" si="2"/>
+        <v>3947332.4512195126</v>
+      </c>
+      <c r="Q10" s="22">
+        <f t="shared" si="2"/>
+        <v>3947332.4512195126</v>
+      </c>
+      <c r="R10" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
@@ -5494,31 +5607,43 @@
       <c r="H11" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="20">
         <f>J10*3.6/Htotal</f>
         <v>2871.2254570074479</v>
       </c>
-      <c r="K11" s="21">
+      <c r="K11" s="20">
         <f>K10/(Htotal/3.6)</f>
         <v>8749.1289198606282</v>
       </c>
-      <c r="N11" s="7" t="str">
-        <f>H47</f>
-        <v>Spidslastvarme</v>
-      </c>
-      <c r="O11" s="17">
-        <f>J47</f>
-        <v>4307</v>
-      </c>
-      <c r="P11" s="17">
-        <f>K47</f>
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L11" s="20">
+        <f t="shared" si="1"/>
+        <v>11620.354376868076</v>
+      </c>
+      <c r="N11" s="18" t="str">
+        <f>H60</f>
+        <v>RGK-rabat</v>
+      </c>
+      <c r="O11" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>tkr</v>
+      </c>
+      <c r="P11" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="22">
+        <f t="shared" si="2"/>
+        <v>246855.16981097564</v>
+      </c>
+      <c r="R11" s="23">
+        <f t="shared" si="2"/>
+        <v>246855.16981097564</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>5</v>
       </c>
@@ -5529,21 +5654,30 @@
         <v>8</v>
       </c>
       <c r="H12" s="7"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="N12" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="O12" s="24">
-        <f>DBudenRGK</f>
-        <v>7902444.2952551143</v>
-      </c>
-      <c r="P12" s="24">
-        <f>DBmedRGK</f>
-        <v>7962367.0651916321</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="N12" s="18" t="str">
+        <f>H61</f>
+        <v>Modtagebetaling affald</v>
+      </c>
+      <c r="O12" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v>tkr</v>
+      </c>
+      <c r="P12" s="22">
+        <f t="shared" si="2"/>
+        <v>4648141.7507472299</v>
+      </c>
+      <c r="Q12" s="22">
+        <f t="shared" si="2"/>
+        <v>4648141.7507472299</v>
+      </c>
+      <c r="R12" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>7</v>
       </c>
@@ -5556,28 +5690,23 @@
       <c r="H13" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="J13" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="K13" s="20" t="str">
-        <f>"Med "&amp;TEXT(C5,"0%")&amp;" RGK"</f>
+      <c r="K13" s="19" t="str">
+        <f>"Med "&amp;TEXT(RGKudnyttelse,"0%")&amp;" RGK"</f>
         <v>Med 100% RGK</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="N13" s="26" t="str">
-        <f>"Varmemængder: "&amp;C22&amp;" ton affald, "&amp;D22&amp;" ton bioaffald"</f>
-        <v>Varmemængder: 12000 ton affald, 0 ton bioaffald</v>
-      </c>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>10</v>
       </c>
@@ -5593,20 +5722,40 @@
       <c r="I14" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J14" s="21">
+      <c r="J14" s="20">
         <f>MIN(Qdemand,K7,EtaQNomOvn3*Ftotal*Htotal/3.6)</f>
         <v>16740</v>
       </c>
-      <c r="K14" s="21">
+      <c r="K14" s="20">
         <f>MIN(Qdemand,K9,EtaQmaxOvn3*Ftotal*Htotal/3.6)</f>
-        <v>20264.21052631579</v>
-      </c>
-      <c r="L14" s="17">
+        <v>20832</v>
+      </c>
+      <c r="L14" s="16">
         <f>K14-J14</f>
-        <v>3524.21052631579</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+        <v>4092</v>
+      </c>
+      <c r="N14" s="18" t="str">
+        <f>H63</f>
+        <v>Betaling bioaffald</v>
+      </c>
+      <c r="O14" s="18" t="str">
+        <f t="shared" ref="O14:O19" si="3">I63</f>
+        <v>tkr</v>
+      </c>
+      <c r="P14" s="23">
+        <f t="shared" ref="P14:P19" si="4">J63</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="23">
+        <f t="shared" ref="Q14:Q19" si="5">K63</f>
+        <v>0</v>
+      </c>
+      <c r="R14" s="23">
+        <f t="shared" ref="R14:R19" si="6">L63</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>11</v>
       </c>
@@ -5624,20 +5773,40 @@
       <c r="I15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="17">
+      <c r="J15" s="16">
         <f>$J$14/EtaQNomOvn3/(Htotal/3.6)</f>
         <v>8749.1289198606282</v>
       </c>
-      <c r="K15" s="17">
+      <c r="K15" s="16">
         <f>$K$14/EtaQmaxOvn3/(Htotal/3.6)</f>
-        <v>8510.6658196012668</v>
-      </c>
-      <c r="L15" s="17">
-        <f t="shared" ref="L15:L55" si="0">K15-J15</f>
-        <v>-238.46310025936145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+        <v>8749.1289198606282</v>
+      </c>
+      <c r="L15" s="16">
+        <f t="shared" ref="L15:L55" si="7">K15-J15</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="18" t="str">
+        <f>H64</f>
+        <v>DV-omkostninger</v>
+      </c>
+      <c r="O15" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>tkr</v>
+      </c>
+      <c r="P15" s="22">
+        <f t="shared" si="4"/>
+        <v>1049040</v>
+      </c>
+      <c r="Q15" s="22">
+        <f t="shared" si="5"/>
+        <v>1107810.8046975606</v>
+      </c>
+      <c r="R15" s="23">
+        <f t="shared" si="6"/>
+        <v>58770.804697560612</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>75</v>
       </c>
@@ -5655,20 +5824,40 @@
       <c r="I16" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J16" s="21">
+      <c r="J16" s="20">
         <f>Qdemand-J14</f>
-        <v>11375</v>
-      </c>
-      <c r="K16" s="21">
+        <v>18260</v>
+      </c>
+      <c r="K16" s="20">
         <f>Qdemand-K14</f>
-        <v>7850.78947368421</v>
-      </c>
-      <c r="L16" s="17">
-        <f t="shared" si="0"/>
-        <v>-3524.21052631579</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>14168</v>
+      </c>
+      <c r="L16" s="16">
+        <f t="shared" si="7"/>
+        <v>-4092</v>
+      </c>
+      <c r="N16" s="18" t="str">
+        <f>H65</f>
+        <v>Affaldvarme-afgift</v>
+      </c>
+      <c r="O16" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>tkr</v>
+      </c>
+      <c r="P16" s="22">
+        <f t="shared" si="4"/>
+        <v>2211287.04</v>
+      </c>
+      <c r="Q16" s="22">
+        <f t="shared" si="5"/>
+        <v>2729557.4400000004</v>
+      </c>
+      <c r="R16" s="23">
+        <f t="shared" si="6"/>
+        <v>518270.40000000037</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>12</v>
       </c>
@@ -5681,20 +5870,40 @@
       <c r="I17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="21">
+      <c r="J17" s="20">
         <f>Ftotal-J15</f>
-        <v>3250.8710801393718</v>
-      </c>
-      <c r="K17" s="21">
+        <v>6250.8710801393718</v>
+      </c>
+      <c r="K17" s="20">
         <f>Ftotal-K15</f>
-        <v>3489.3341803987332</v>
-      </c>
-      <c r="L17" s="17">
-        <f t="shared" si="0"/>
-        <v>238.46310025936145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>6250.8710801393718</v>
+      </c>
+      <c r="L17" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="18" t="str">
+        <f>H66</f>
+        <v>Tillægsafgift</v>
+      </c>
+      <c r="O17" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>tkr</v>
+      </c>
+      <c r="P17" s="23">
+        <f t="shared" si="4"/>
+        <v>2271283.2000000002</v>
+      </c>
+      <c r="Q17" s="23">
+        <f t="shared" si="5"/>
+        <v>2468551.6981097562</v>
+      </c>
+      <c r="R17" s="23">
+        <f t="shared" si="6"/>
+        <v>197268.49810975604</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>23</v>
       </c>
@@ -5719,20 +5928,40 @@
       <c r="I18" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J18" s="21">
+      <c r="J18" s="20">
         <f>MIN(J16,NSvarme)</f>
         <v>4000</v>
       </c>
-      <c r="K18" s="21">
+      <c r="K18" s="20">
         <f>MIN(K16,NSvarme)</f>
         <v>4000</v>
       </c>
-      <c r="L18" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L18" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="18" t="str">
+        <f>H67</f>
+        <v>CO2-afgift</v>
+      </c>
+      <c r="O18" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>tkr</v>
+      </c>
+      <c r="P18" s="23">
+        <f t="shared" si="4"/>
+        <v>471719.80799999996</v>
+      </c>
+      <c r="Q18" s="23">
+        <f t="shared" si="5"/>
+        <v>512690.2418291159</v>
+      </c>
+      <c r="R18" s="23">
+        <f t="shared" si="6"/>
+        <v>40970.433829115937</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="H19" s="7" t="s">
         <v>64</v>
@@ -5740,20 +5969,40 @@
       <c r="I19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J19" s="21">
+      <c r="J19" s="20">
         <f>J16-J18</f>
-        <v>7375</v>
-      </c>
-      <c r="K19" s="21">
+        <v>14260</v>
+      </c>
+      <c r="K19" s="20">
         <f>K16-K18</f>
-        <v>3850.78947368421</v>
-      </c>
-      <c r="L19" s="17">
-        <f t="shared" si="0"/>
-        <v>-3524.21052631579</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>10168</v>
+      </c>
+      <c r="L19" s="16">
+        <f t="shared" si="7"/>
+        <v>-4092</v>
+      </c>
+      <c r="N19" s="18" t="str">
+        <f>H68</f>
+        <v>Kvote-omkostning</v>
+      </c>
+      <c r="O19" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>tkr</v>
+      </c>
+      <c r="P19" s="23">
+        <f t="shared" si="4"/>
+        <v>2093987.8587116271</v>
+      </c>
+      <c r="Q19" s="23">
+        <f t="shared" si="5"/>
+        <v>2093987.8587116271</v>
+      </c>
+      <c r="R19" s="23">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>16</v>
       </c>
@@ -5772,33 +6021,38 @@
       <c r="I20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J20" s="21">
+      <c r="J20" s="20">
         <f>MIN($J$19,J7,EtaQNomOvn2*(J17*Htotal)/3.6)</f>
         <v>7068</v>
       </c>
-      <c r="K20" s="21">
+      <c r="K20" s="20">
         <f>MIN($K$19,J9,EtaQmaxOvn2*(K17*Htotal)/3.6)</f>
-        <v>3850.78947368421</v>
-      </c>
-      <c r="L20" s="17">
-        <f t="shared" si="0"/>
-        <v>-3217.21052631579</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
+        <v>8556</v>
+      </c>
+      <c r="L20" s="16">
+        <f t="shared" si="7"/>
+        <v>1488</v>
+      </c>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="33">
+      <c r="C21" s="29">
         <v>1</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21" s="29">
         <v>1</v>
       </c>
-      <c r="E21" s="34">
+      <c r="E21" s="30">
         <v>1</v>
       </c>
       <c r="H21" s="7" t="s">
@@ -5807,20 +6061,26 @@
       <c r="I21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="21">
+      <c r="J21" s="20">
         <f>$J$20/EtaQNomOvn2/(Htotal/3.6)</f>
         <v>2871.2254570074479</v>
       </c>
-      <c r="K21" s="21">
-        <f>$K$20/EtaQNomOvn2/(Htotal/3.6)</f>
-        <v>1564.3017496347502</v>
-      </c>
-      <c r="L21" s="17">
-        <f t="shared" si="0"/>
-        <v>-1306.9237073726977</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K21" s="20">
+        <f>$K$20/EtaQmaxOvn2/(Htotal/3.6)</f>
+        <v>2871.2254570074479</v>
+      </c>
+      <c r="L21" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="16"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>20</v>
       </c>
@@ -5829,7 +6089,7 @@
       </c>
       <c r="C22" s="14">
         <f>F22-BioTonnage</f>
-        <v>12000</v>
+        <v>15000</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -5838,7 +6098,7 @@
         <v>4000</v>
       </c>
       <c r="F22">
-        <v>12000</v>
+        <v>15000</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>64</v>
@@ -5846,20 +6106,39 @@
       <c r="I22" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J22" s="21">
+      <c r="J22" s="20">
         <f>J19-J20</f>
-        <v>307</v>
-      </c>
-      <c r="K22" s="21">
+        <v>7192</v>
+      </c>
+      <c r="K22" s="20">
         <f>K19-K20</f>
-        <v>0</v>
-      </c>
-      <c r="L22" s="17">
-        <f t="shared" si="0"/>
-        <v>-307</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1612</v>
+      </c>
+      <c r="L22" s="16">
+        <f t="shared" si="7"/>
+        <v>-5580</v>
+      </c>
+      <c r="N22" s="7" t="str">
+        <f>H40</f>
+        <v>Varmeproduktion Ovn2</v>
+      </c>
+      <c r="O22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="P22" s="16">
+        <f>J40</f>
+        <v>7068</v>
+      </c>
+      <c r="Q22" s="16">
+        <f>K40</f>
+        <v>8556</v>
+      </c>
+      <c r="R22" s="16">
+        <f>Q22-P22</f>
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>62</v>
       </c>
@@ -5877,20 +6156,39 @@
       <c r="I23" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="21">
+      <c r="J23" s="20">
         <f>J17-J21</f>
-        <v>379.64562313192391</v>
-      </c>
-      <c r="K23" s="21">
+        <v>3379.6456231319239</v>
+      </c>
+      <c r="K23" s="20">
         <f>K17-K21</f>
-        <v>1925.032430763983</v>
-      </c>
-      <c r="L23" s="17">
-        <f t="shared" si="0"/>
-        <v>1545.3868076320591</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3379.6456231319239</v>
+      </c>
+      <c r="L23" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="7" t="str">
+        <f>H41</f>
+        <v>Varmeproduktion Ovn3</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="P23" s="16">
+        <f>J41</f>
+        <v>16740</v>
+      </c>
+      <c r="Q23" s="16">
+        <f>K41</f>
+        <v>20832</v>
+      </c>
+      <c r="R23" s="16">
+        <f t="shared" ref="R23:R27" si="8">Q23-P23</f>
+        <v>4092</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>45</v>
       </c>
@@ -5913,20 +6211,39 @@
       <c r="I24" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J24" s="21">
+      <c r="J24" s="20">
         <f>J14+J20</f>
         <v>23808</v>
       </c>
-      <c r="K24" s="21">
+      <c r="K24" s="20">
         <f>K14+K20</f>
-        <v>24115</v>
-      </c>
-      <c r="L24" s="17">
-        <f t="shared" si="0"/>
-        <v>307</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>29388</v>
+      </c>
+      <c r="L24" s="16">
+        <f t="shared" si="7"/>
+        <v>5580</v>
+      </c>
+      <c r="N24" s="7" t="str">
+        <f>H43</f>
+        <v>Heraf RGK-varme</v>
+      </c>
+      <c r="O24" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="P24" s="16">
+        <f>J43</f>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="16">
+        <f>K43</f>
+        <v>5877.080469756057</v>
+      </c>
+      <c r="R24" s="16">
+        <f t="shared" si="8"/>
+        <v>5877.080469756057</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>34</v>
       </c>
@@ -5948,20 +6265,39 @@
       <c r="I25" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J25" s="21">
+      <c r="J25" s="20">
         <f>J22</f>
-        <v>307</v>
-      </c>
-      <c r="K25" s="21">
+        <v>7192</v>
+      </c>
+      <c r="K25" s="20">
         <f>K22</f>
-        <v>0</v>
-      </c>
-      <c r="L25" s="17">
-        <f t="shared" si="0"/>
-        <v>-307</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1612</v>
+      </c>
+      <c r="L25" s="16">
+        <f t="shared" si="7"/>
+        <v>-5580</v>
+      </c>
+      <c r="N25" s="7" t="str">
+        <f>H34</f>
+        <v>Bortkølet varme</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="P25" s="16">
+        <f>J34</f>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="16">
+        <f>K34</f>
+        <v>0</v>
+      </c>
+      <c r="R25" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>42</v>
       </c>
@@ -5983,20 +6319,49 @@
       <c r="I26" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J26" s="17">
+      <c r="J26" s="16">
         <f>$J$7-$J$20</f>
         <v>0</v>
       </c>
-      <c r="K26" s="17">
+      <c r="K26" s="16">
         <f>J26</f>
         <v>0</v>
       </c>
-      <c r="L26" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L26" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="7" t="str">
+        <f>H46</f>
+        <v>Leveret varme</v>
+      </c>
+      <c r="O26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="P26" s="16">
+        <f>J46</f>
+        <v>23808</v>
+      </c>
+      <c r="Q26" s="16">
+        <f>K46</f>
+        <v>29388</v>
+      </c>
+      <c r="R26" s="16">
+        <f t="shared" si="8"/>
+        <v>5580</v>
+      </c>
+      <c r="T26" s="24" t="str">
+        <f>"RGK ift. Nominel: "&amp;C22&amp;" ton affald, "&amp;D22&amp;" ton bioaffald"</f>
+        <v>RGK ift. Nominel: 15000 ton affald, 0 ton bioaffald</v>
+      </c>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+      <c r="X26" s="11"/>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="11"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>43</v>
       </c>
@@ -6018,20 +6383,39 @@
       <c r="I27" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J27" s="17">
+      <c r="J27" s="16">
         <f>$K$7-$J$14</f>
         <v>0</v>
       </c>
-      <c r="K27" s="17">
+      <c r="K27" s="16">
         <f>J27</f>
         <v>0</v>
       </c>
-      <c r="L27" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L27" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="7" t="str">
+        <f>H47</f>
+        <v>Spidslastvarme</v>
+      </c>
+      <c r="O27" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="P27" s="16">
+        <f>J47</f>
+        <v>11192</v>
+      </c>
+      <c r="Q27" s="16">
+        <f>K47</f>
+        <v>5612</v>
+      </c>
+      <c r="R27" s="16">
+        <f t="shared" si="8"/>
+        <v>-5580</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>146</v>
       </c>
@@ -6053,20 +6437,24 @@
       <c r="I28" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J28" s="17">
+      <c r="J28" s="16">
         <f>MIN(J27,EtaQNomOvn3*J23*Htotal/3.6,24*E9*KapQcool)</f>
         <v>0</v>
       </c>
-      <c r="K28" s="17">
+      <c r="K28" s="16">
         <f>MIN(K27,EtaQNomOvn3*K23*Htotal/3.6,24*E9*KapQcool)</f>
         <v>0</v>
       </c>
-      <c r="L28" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L28" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N28" s="7"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="16"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>26</v>
       </c>
@@ -6076,20 +6464,24 @@
       <c r="I29" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J29" s="17">
+      <c r="J29" s="16">
         <f>J28/EtaQNomOvn3/(Htotal/3.6)</f>
         <v>0</v>
       </c>
-      <c r="K29" s="17">
+      <c r="K29" s="16">
         <f>K28/EtaQNomOvn3/(Htotal/3.6)</f>
         <v>0</v>
       </c>
-      <c r="L29" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L29" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="R29" s="16"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>33</v>
       </c>
@@ -6105,20 +6497,38 @@
       <c r="I30" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J30" s="17">
+      <c r="J30" s="16">
         <f>J23-J29</f>
-        <v>379.64562313192391</v>
-      </c>
-      <c r="K30" s="17">
+        <v>3379.6456231319239</v>
+      </c>
+      <c r="K30" s="16">
         <f>K23-K29</f>
-        <v>1925.032430763983</v>
-      </c>
-      <c r="L30" s="17">
-        <f t="shared" si="0"/>
-        <v>1545.3868076320591</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3379.6456231319239</v>
+      </c>
+      <c r="L30" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P30" s="16">
+        <f>J15</f>
+        <v>8749.1289198606282</v>
+      </c>
+      <c r="Q30" s="16">
+        <f>K15</f>
+        <v>8749.1289198606282</v>
+      </c>
+      <c r="R30" s="16">
+        <f>Q30-P30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>30</v>
       </c>
@@ -6134,20 +6544,38 @@
       <c r="I31" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J31" s="17">
+      <c r="J31" s="16">
         <f>MIN(J26,EtaQNomOvn3*J30*Htotal/3.6,24*E9*KapQcool-J28)</f>
         <v>0</v>
       </c>
-      <c r="K31" s="17">
+      <c r="K31" s="16">
         <f>MIN(K26,EtaQNomOvn3*K30*Htotal/3.6,24*E9*KapQcool-K28)</f>
         <v>0</v>
       </c>
-      <c r="L31" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L31" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="O31" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="P31" s="16">
+        <f>J18</f>
+        <v>4000</v>
+      </c>
+      <c r="Q31" s="16">
+        <f>K18</f>
+        <v>4000</v>
+      </c>
+      <c r="R31" s="16">
+        <f t="shared" ref="R31:R36" si="9">Q31-P31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>46</v>
       </c>
@@ -6163,20 +6591,38 @@
       <c r="I32" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J32" s="17">
+      <c r="J32" s="16">
         <f>J31/EtaQNomOvn2/(Htotal/3.6)</f>
         <v>0</v>
       </c>
-      <c r="K32" s="17">
+      <c r="K32" s="16">
         <f>K31/EtaQNomOvn2/(Htotal/3.6)</f>
         <v>0</v>
       </c>
-      <c r="L32" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L32" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N32" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="O32" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P32" s="16">
+        <f>J21</f>
+        <v>2871.2254570074479</v>
+      </c>
+      <c r="Q32" s="16">
+        <f>K21</f>
+        <v>2871.2254570074479</v>
+      </c>
+      <c r="R32" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>32</v>
       </c>
@@ -6192,20 +6638,38 @@
       <c r="I33" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="17">
+      <c r="J33" s="16">
         <f>J30-J32</f>
-        <v>379.64562313192391</v>
-      </c>
-      <c r="K33" s="17">
+        <v>3379.6456231319239</v>
+      </c>
+      <c r="K33" s="16">
         <f>K30-K32</f>
-        <v>1925.032430763983</v>
-      </c>
-      <c r="L33" s="17">
-        <f t="shared" si="0"/>
-        <v>1545.3868076320591</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+        <v>3379.6456231319239</v>
+      </c>
+      <c r="L33" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N33" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="O33" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P33" s="16">
+        <f>J29</f>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="16">
+        <f>K29</f>
+        <v>0</v>
+      </c>
+      <c r="R33" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>36</v>
       </c>
@@ -6221,20 +6685,38 @@
       <c r="I34" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J34" s="17">
+      <c r="J34" s="16">
         <f>J28+J31</f>
         <v>0</v>
       </c>
-      <c r="K34" s="17">
+      <c r="K34" s="16">
         <f>K28+K31</f>
         <v>0</v>
       </c>
-      <c r="L34" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L34" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N34" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="O34" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P34" s="16">
+        <f>J32</f>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="16">
+        <f>K32</f>
+        <v>0</v>
+      </c>
+      <c r="R34" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>37</v>
       </c>
@@ -6250,30 +6732,38 @@
       <c r="I35" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J35" s="17">
+      <c r="J35" s="16">
         <f>SUM($C$22:$D$22)-J36</f>
         <v>11620.354376868076</v>
       </c>
-      <c r="K35" s="17">
+      <c r="K35" s="16">
         <f>SUM($C$22:$D$22)-K36</f>
-        <v>10074.967569236018</v>
-      </c>
-      <c r="L35" s="17">
-        <f t="shared" si="0"/>
-        <v>-1545.3868076320578</v>
-      </c>
-      <c r="N35" s="26" t="str">
-        <f>"RGK ift. Nominel: "&amp;C22&amp;" ton affald, "&amp;D22&amp;" ton bioaffald"</f>
-        <v>RGK ift. Nominel: 12000 ton affald, 0 ton bioaffald</v>
-      </c>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="11"/>
-      <c r="S35" s="11"/>
-      <c r="T35" s="11"/>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+        <v>11620.354376868076</v>
+      </c>
+      <c r="L35" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N35" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="O35" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P35" s="16">
+        <f>P30+SUM(P32:P34)</f>
+        <v>11620.354376868076</v>
+      </c>
+      <c r="Q35" s="16">
+        <f>Q30+SUM(Q32:Q34)</f>
+        <v>11620.354376868076</v>
+      </c>
+      <c r="R35" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>38</v>
       </c>
@@ -6289,40 +6779,59 @@
       <c r="I36" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J36" s="21">
+      <c r="J36" s="20">
         <f>J23</f>
-        <v>379.64562313192391</v>
-      </c>
-      <c r="K36" s="21">
+        <v>3379.6456231319239</v>
+      </c>
+      <c r="K36" s="20">
         <f>K23</f>
-        <v>1925.032430763983</v>
-      </c>
-      <c r="L36" s="17">
-        <f t="shared" si="0"/>
-        <v>1545.3868076320591</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+        <v>3379.6456231319239</v>
+      </c>
+      <c r="L36" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N36" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="O36" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P36" s="20">
+        <f>J36</f>
+        <v>3379.6456231319239</v>
+      </c>
+      <c r="Q36" s="20">
+        <f>K36</f>
+        <v>3379.6456231319239</v>
+      </c>
+      <c r="R36" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H37" t="s">
         <v>53</v>
       </c>
       <c r="I37" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J37" s="17">
+      <c r="J37" s="16">
         <f>EtaE*(J15+J29)*Htotal/3.6</f>
         <v>5733.9603658536589</v>
       </c>
-      <c r="K37" s="17">
+      <c r="K37" s="16">
         <f>EtaE*(K15+K29)*Htotal/3.6</f>
-        <v>5577.6776115211796</v>
-      </c>
-      <c r="L37" s="17">
-        <f t="shared" si="0"/>
-        <v>-156.28275433247927</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+        <v>5733.9603658536589</v>
+      </c>
+      <c r="L37" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R37" s="16"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>39</v>
       </c>
@@ -6332,20 +6841,24 @@
       <c r="I38" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J38" s="17">
+      <c r="J38" s="16">
         <f>$D$9*$D$13</f>
         <v>775</v>
       </c>
-      <c r="K38" s="17">
+      <c r="K38" s="16">
         <f>$D$9*$D$13</f>
         <v>775</v>
       </c>
-      <c r="L38" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L38" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N38" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="R38" s="16"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>47</v>
       </c>
@@ -6353,7 +6866,7 @@
         <v>48</v>
       </c>
       <c r="C39">
-        <v>28115</v>
+        <v>35000</v>
       </c>
       <c r="H39" t="s">
         <v>54</v>
@@ -6361,20 +6874,35 @@
       <c r="I39" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J39" s="17">
+      <c r="J39" s="16">
         <f>J37-J38</f>
         <v>4958.9603658536589</v>
       </c>
-      <c r="K39" s="17">
+      <c r="K39" s="16">
         <f>K37-K38</f>
-        <v>4802.6776115211796</v>
-      </c>
-      <c r="L39" s="17">
-        <f t="shared" si="0"/>
-        <v>-156.28275433247927</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+        <v>4958.9603658536589</v>
+      </c>
+      <c r="L39" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N39" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="P39" s="2">
+        <f>(P30+P33)/$K$11</f>
+        <v>1</v>
+      </c>
+      <c r="Q39" s="2">
+        <f>(Q30+Q33)/$K$11</f>
+        <v>1</v>
+      </c>
+      <c r="R39" s="2">
+        <f>Q39-P39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>68</v>
       </c>
@@ -6383,7 +6911,7 @@
       </c>
       <c r="C40" s="14">
         <f>SUM(C22:D22)</f>
-        <v>12000</v>
+        <v>15000</v>
       </c>
       <c r="H40" t="s">
         <v>120</v>
@@ -6391,20 +6919,35 @@
       <c r="I40" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J40" s="17">
+      <c r="J40" s="16">
         <f>J20+J31</f>
         <v>7068</v>
       </c>
-      <c r="K40" s="17">
+      <c r="K40" s="16">
         <f>K20+K31</f>
-        <v>3850.78947368421</v>
-      </c>
-      <c r="L40" s="17">
-        <f t="shared" si="0"/>
-        <v>-3217.21052631579</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+        <v>8556</v>
+      </c>
+      <c r="L40" s="16">
+        <f t="shared" si="7"/>
+        <v>1488</v>
+      </c>
+      <c r="N40" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="P40" s="2">
+        <f>(P32+P34)/$J$11</f>
+        <v>1</v>
+      </c>
+      <c r="Q40" s="2">
+        <f>(Q32+Q34)/$J$11</f>
+        <v>1</v>
+      </c>
+      <c r="R40" s="2">
+        <f t="shared" ref="R40:R41" si="10">Q40-P40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>67</v>
       </c>
@@ -6425,20 +6968,35 @@
       <c r="I41" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J41" s="17">
+      <c r="J41" s="16">
         <f>J14+J28</f>
         <v>16740</v>
       </c>
-      <c r="K41" s="17">
+      <c r="K41" s="16">
         <f>K14+K28</f>
-        <v>20264.21052631579</v>
-      </c>
-      <c r="L41" s="17">
-        <f t="shared" si="0"/>
-        <v>3524.21052631579</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+        <v>20832</v>
+      </c>
+      <c r="L41" s="16">
+        <f t="shared" si="7"/>
+        <v>4092</v>
+      </c>
+      <c r="N41" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="P41" s="2">
+        <f>P25/(24*$E$9*KapQcool)</f>
+        <v>0</v>
+      </c>
+      <c r="Q41" s="2">
+        <f>Q25/(24*$E$9*KapQcool)</f>
+        <v>0</v>
+      </c>
+      <c r="R41" s="2">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="H42" t="s">
         <v>116</v>
@@ -6446,566 +7004,666 @@
       <c r="I42" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J42" s="17">
+      <c r="J42" s="16">
         <f>SUM(J40:J41)</f>
         <v>23808</v>
       </c>
-      <c r="K42" s="17">
+      <c r="K42" s="16">
         <f>SUM(K40:K41)</f>
-        <v>24115</v>
-      </c>
-      <c r="L42" s="17">
-        <f t="shared" si="0"/>
-        <v>307</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+        <v>29388</v>
+      </c>
+      <c r="L42" s="16">
+        <f t="shared" si="7"/>
+        <v>5580</v>
+      </c>
+      <c r="R42" s="16"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H43" s="7" t="s">
         <v>122</v>
       </c>
       <c r="I43" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J43" s="17">
-        <v>0</v>
-      </c>
-      <c r="K43" s="17">
+      <c r="J43" s="16">
+        <v>0</v>
+      </c>
+      <c r="K43" s="16">
         <f>(EtaRgkOvn2*K15+EtaRgkOvn3*K21)*Htotal/3.6</f>
-        <v>5142.2449555410476</v>
-      </c>
-      <c r="L43" s="17">
-        <f t="shared" si="0"/>
-        <v>5142.2449555410476</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+        <v>5877.080469756057</v>
+      </c>
+      <c r="L43" s="16">
+        <f t="shared" si="7"/>
+        <v>5877.080469756057</v>
+      </c>
+      <c r="N43" s="7"/>
+      <c r="R43" s="16"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H44" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="J44" s="17">
+      <c r="J44" s="16">
         <v>0</v>
       </c>
       <c r="K44" s="2">
         <f>K43/K45</f>
-        <v>0.173182258023971</v>
-      </c>
-      <c r="L44" s="17">
-        <f t="shared" si="0"/>
-        <v>0.173182258023971</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+        <v>0.16733349757634497</v>
+      </c>
+      <c r="L44" s="16">
+        <f t="shared" si="7"/>
+        <v>0.16733349757634497</v>
+      </c>
+      <c r="N44" s="7"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="16"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H45" t="s">
         <v>114</v>
       </c>
       <c r="I45" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="J45" s="17">
+      <c r="J45" s="16">
         <f>J42+J37</f>
         <v>29541.960365853658</v>
       </c>
-      <c r="K45" s="17">
+      <c r="K45" s="16">
         <f>K42+K37</f>
-        <v>29692.67761152118</v>
-      </c>
-      <c r="L45" s="17">
-        <f t="shared" si="0"/>
-        <v>150.71724566752164</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+        <v>35121.960365853658</v>
+      </c>
+      <c r="L45" s="16">
+        <f t="shared" si="7"/>
+        <v>5580</v>
+      </c>
+      <c r="R45" s="16"/>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H46" t="s">
         <v>117</v>
       </c>
       <c r="I46" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J46" s="17">
+      <c r="J46" s="16">
         <f>J42-J34</f>
         <v>23808</v>
       </c>
-      <c r="K46" s="17">
+      <c r="K46" s="16">
         <f>K42-K34</f>
-        <v>24115</v>
-      </c>
-      <c r="L46" s="17">
-        <f t="shared" si="0"/>
-        <v>307</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+        <v>29388</v>
+      </c>
+      <c r="L46" s="16">
+        <f t="shared" si="7"/>
+        <v>5580</v>
+      </c>
+      <c r="R46" s="16"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H47" t="s">
         <v>142</v>
       </c>
       <c r="I47" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J47" s="17">
+      <c r="J47" s="16">
         <f>Qdemand-J46</f>
-        <v>4307</v>
-      </c>
-      <c r="K47" s="17">
+        <v>11192</v>
+      </c>
+      <c r="K47" s="16">
         <f>Qdemand-K46</f>
-        <v>4000</v>
-      </c>
-      <c r="L47" s="17">
-        <f t="shared" si="0"/>
-        <v>-307</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+        <v>5612</v>
+      </c>
+      <c r="L47" s="16">
+        <f t="shared" si="7"/>
+        <v>-5580</v>
+      </c>
+      <c r="R47" s="16"/>
+      <c r="T47" s="24" t="str">
+        <f>"Økonomiske nøgletal: "&amp;C22&amp;" ton affald, "&amp;D22&amp;" ton bioaffald"</f>
+        <v>Økonomiske nøgletal: 15000 ton affald, 0 ton bioaffald</v>
+      </c>
+      <c r="U47" s="11"/>
+      <c r="V47" s="11"/>
+      <c r="W47" s="11"/>
+      <c r="X47" s="11"/>
+      <c r="Y47" s="11"/>
+      <c r="Z47" s="11"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H48" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="L48" s="17"/>
-    </row>
-    <row r="49" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="L48" s="16"/>
+      <c r="N48" s="5"/>
+      <c r="R48" s="16"/>
+    </row>
+    <row r="49" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H49" t="s">
         <v>131</v>
       </c>
       <c r="I49" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="J49" s="17">
+      <c r="J49" s="16">
         <f>J$35*$C$23*LHVaffald/3.6</f>
         <v>33892.70026586522</v>
       </c>
-      <c r="K49" s="17">
+      <c r="K49" s="16">
         <f>K$35*$C$23*LHVaffald/3.6</f>
-        <v>29385.322076938384</v>
-      </c>
-      <c r="L49" s="17">
-        <f t="shared" si="0"/>
-        <v>-4507.3781889268357</v>
-      </c>
-    </row>
-    <row r="50" spans="8:20" x14ac:dyDescent="0.25">
+        <v>33892.70026586522</v>
+      </c>
+      <c r="L49" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R49" s="16"/>
+    </row>
+    <row r="50" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H50" t="s">
         <v>132</v>
       </c>
       <c r="I50" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="J50" s="17">
+      <c r="J50" s="16">
         <f>J$35*AndelBioaffald*LHVbioaffald/3.6</f>
         <v>0</v>
       </c>
-      <c r="K50" s="17">
+      <c r="K50" s="16">
         <f>K$35*AndelBioaffald*LHVbioaffald/3.6</f>
         <v>0</v>
       </c>
-      <c r="L50" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="L50" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R50" s="16"/>
+    </row>
+    <row r="51" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H51" t="s">
         <v>130</v>
       </c>
       <c r="I51" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="J51" s="17">
+      <c r="J51" s="16">
         <f>J45/0.85 - J50</f>
         <v>34755.247489239599</v>
       </c>
-      <c r="K51" s="17">
+      <c r="K51" s="16">
         <f>K45/0.95 - K50</f>
-        <v>31255.450117390716</v>
-      </c>
-      <c r="L51" s="17">
-        <f t="shared" si="0"/>
-        <v>-3499.7973718488829</v>
-      </c>
-    </row>
-    <row r="52" spans="8:20" x14ac:dyDescent="0.25">
+        <v>36970.484595635433</v>
+      </c>
+      <c r="L51" s="16">
+        <f t="shared" si="7"/>
+        <v>2215.2371063958344</v>
+      </c>
+      <c r="R51" s="16"/>
+    </row>
+    <row r="52" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H52" t="s">
         <v>136</v>
       </c>
       <c r="I52" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J52" s="17">
+      <c r="J52" s="16">
         <f>J42*J51/(J51+J50)</f>
         <v>23808</v>
       </c>
-      <c r="K52" s="17">
+      <c r="K52" s="16">
         <f>K42*K51/(K51+K50)</f>
-        <v>24115</v>
-      </c>
-      <c r="L52" s="17">
-        <f t="shared" si="0"/>
-        <v>307</v>
-      </c>
-    </row>
-    <row r="53" spans="8:20" x14ac:dyDescent="0.25">
+        <v>29388</v>
+      </c>
+      <c r="L52" s="16">
+        <f t="shared" si="7"/>
+        <v>5580</v>
+      </c>
+      <c r="R52" s="16"/>
+    </row>
+    <row r="53" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H53" t="s">
         <v>133</v>
       </c>
       <c r="I53" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J53" s="17">
+      <c r="J53" s="16">
         <f>J37*J51/(J51+J50)</f>
         <v>5733.9603658536589</v>
       </c>
-      <c r="K53" s="17">
+      <c r="K53" s="16">
         <f>K37*K51/(K51+K50)</f>
-        <v>5577.6776115211796</v>
-      </c>
-      <c r="L53" s="17">
-        <f t="shared" si="0"/>
-        <v>-156.28275433247927</v>
-      </c>
-    </row>
-    <row r="54" spans="8:20" x14ac:dyDescent="0.25">
+        <v>5733.9603658536589</v>
+      </c>
+      <c r="L53" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R53" s="16"/>
+    </row>
+    <row r="54" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H54" t="s">
         <v>134</v>
       </c>
       <c r="I54" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J54" s="17">
+      <c r="J54" s="16">
         <f>J52/1.2</f>
         <v>19840</v>
       </c>
-      <c r="K54" s="17">
+      <c r="K54" s="16">
         <f>(K52-0.1*(K52+K53))/1.2</f>
-        <v>17621.443532373236</v>
-      </c>
-      <c r="L54" s="17">
-        <f t="shared" si="0"/>
-        <v>-2218.5564676267641</v>
-      </c>
-    </row>
-    <row r="55" spans="8:20" x14ac:dyDescent="0.25">
+        <v>21563.169969512197</v>
+      </c>
+      <c r="L54" s="16">
+        <f t="shared" si="7"/>
+        <v>1723.169969512197</v>
+      </c>
+      <c r="R54" s="16"/>
+    </row>
+    <row r="55" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H55" t="s">
         <v>137</v>
       </c>
       <c r="I55" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J55" s="17">
+      <c r="J55" s="16">
         <f>J54</f>
         <v>19840</v>
       </c>
-      <c r="K55" s="17">
+      <c r="K55" s="16">
         <f>K54</f>
-        <v>17621.443532373236</v>
-      </c>
-      <c r="L55" s="17">
-        <f t="shared" si="0"/>
-        <v>-2218.5564676267641</v>
-      </c>
-    </row>
-    <row r="56" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="N56" s="26" t="str">
-        <f>"Økonomiske nøgletal: "&amp;C22&amp;" ton affald, "&amp;D22&amp;" ton bioaffald"</f>
-        <v>Økonomiske nøgletal: 12000 ton affald, 0 ton bioaffald</v>
-      </c>
-      <c r="O56" s="11"/>
-      <c r="P56" s="11"/>
-      <c r="Q56" s="11"/>
-      <c r="R56" s="11"/>
-      <c r="S56" s="11"/>
-      <c r="T56" s="11"/>
-    </row>
-    <row r="57" spans="8:20" x14ac:dyDescent="0.25">
+        <v>21563.169969512197</v>
+      </c>
+      <c r="L55" s="16">
+        <f t="shared" si="7"/>
+        <v>1723.169969512197</v>
+      </c>
+      <c r="R55" s="16"/>
+    </row>
+    <row r="57" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H57" s="5" t="s">
         <v>110</v>
       </c>
       <c r="I57" s="10"/>
-      <c r="J57" s="20" t="str">
+      <c r="J57" s="19" t="str">
         <f>J13</f>
         <v>Uden RGK</v>
       </c>
-      <c r="K57" s="20" t="str">
+      <c r="K57" s="19" t="str">
         <f>K13</f>
         <v>Med 100% RGK</v>
       </c>
       <c r="L57" s="5" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="58" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H58" s="19" t="s">
+      <c r="N57" s="5"/>
+      <c r="O57" s="10"/>
+      <c r="P57" s="19"/>
+      <c r="Q57" s="19"/>
+      <c r="R57" s="5"/>
+    </row>
+    <row r="58" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H58" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="I58" s="19" t="s">
+      <c r="I58" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="J58" s="23">
+      <c r="J58" s="22">
         <f>Varmesalgspris*J46</f>
         <v>7404288</v>
       </c>
-      <c r="K58" s="23">
+      <c r="K58" s="22">
         <f>Varmesalgspris*K46</f>
-        <v>7499765</v>
-      </c>
-      <c r="L58" s="24">
+        <v>9139668</v>
+      </c>
+      <c r="L58" s="23">
         <f>K58-J58</f>
-        <v>95477</v>
-      </c>
-    </row>
-    <row r="59" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H59" s="19" t="s">
+        <v>1735380</v>
+      </c>
+      <c r="N58" s="18"/>
+      <c r="O58" s="18"/>
+      <c r="P58" s="22"/>
+      <c r="Q58" s="22"/>
+      <c r="R58" s="23"/>
+    </row>
+    <row r="59" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H59" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="I59" s="19" t="s">
+      <c r="I59" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="J59" s="23">
+      <c r="J59" s="22">
         <f>(Elpris-ElprodTarif)*J39</f>
         <v>3947332.4512195126</v>
       </c>
-      <c r="K59" s="23">
+      <c r="K59" s="22">
         <f>(Elpris-ElprodTarif)*K39</f>
-        <v>3822931.378770859</v>
-      </c>
-      <c r="L59" s="24">
-        <f t="shared" ref="L59:L72" si="1">K59-J59</f>
-        <v>-124401.07244865363</v>
-      </c>
-    </row>
-    <row r="60" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H60" s="19" t="s">
+        <v>3947332.4512195126</v>
+      </c>
+      <c r="L59" s="23">
+        <f t="shared" ref="L59:L72" si="11">K59-J59</f>
+        <v>0</v>
+      </c>
+      <c r="N59" s="18"/>
+      <c r="O59" s="18"/>
+      <c r="P59" s="22"/>
+      <c r="Q59" s="22"/>
+      <c r="R59" s="23"/>
+    </row>
+    <row r="60" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H60" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="I60" s="19" t="s">
+      <c r="I60" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="J60" s="23">
-        <v>0</v>
-      </c>
-      <c r="K60" s="23">
+      <c r="J60" s="22">
+        <v>0</v>
+      </c>
+      <c r="K60" s="22">
         <f>IF(K43&lt;7%*K45,0,10%)*K66</f>
-        <v>201730.28555860883</v>
-      </c>
-      <c r="L60" s="24">
-        <f t="shared" si="1"/>
-        <v>201730.28555860883</v>
-      </c>
-    </row>
-    <row r="61" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H61" s="19" t="s">
+        <v>246855.16981097564</v>
+      </c>
+      <c r="L60" s="23">
+        <f t="shared" si="11"/>
+        <v>246855.16981097564</v>
+      </c>
+      <c r="N60" s="18"/>
+      <c r="O60" s="18"/>
+      <c r="P60" s="22"/>
+      <c r="Q60" s="22"/>
+      <c r="R60" s="23"/>
+    </row>
+    <row r="61" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H61" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="I61" s="19" t="s">
+      <c r="I61" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="J61" s="23">
+      <c r="J61" s="22">
         <f>$C$24*($C$22-J36*$C$23)</f>
         <v>4648141.7507472299</v>
       </c>
-      <c r="K61" s="23">
+      <c r="K61" s="22">
         <f>$C$24*($C$22-K36*$C$23)</f>
-        <v>4029987.0276944069</v>
-      </c>
-      <c r="L61" s="24">
-        <f t="shared" si="1"/>
-        <v>-618154.72305282298</v>
-      </c>
-    </row>
-    <row r="62" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="I62" s="19"/>
-      <c r="J62" s="24"/>
-      <c r="K62" s="24"/>
-      <c r="L62" s="24"/>
-    </row>
-    <row r="63" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H63" s="19" t="s">
+        <v>4648141.7507472299</v>
+      </c>
+      <c r="L61" s="23">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N61" s="18"/>
+      <c r="O61" s="18"/>
+      <c r="P61" s="22"/>
+      <c r="Q61" s="22"/>
+      <c r="R61" s="23"/>
+    </row>
+    <row r="62" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="I62" s="18"/>
+      <c r="J62" s="23"/>
+      <c r="K62" s="23"/>
+      <c r="L62" s="23"/>
+      <c r="O62" s="18"/>
+      <c r="P62" s="23"/>
+      <c r="Q62" s="23"/>
+      <c r="R62" s="23"/>
+    </row>
+    <row r="63" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H63" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="I63" s="19" t="s">
+      <c r="I63" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="J63" s="24">
+      <c r="J63" s="23">
         <f>$D$24*($D$22-J36*AndelBioaffald)</f>
         <v>0</v>
       </c>
-      <c r="K63" s="24">
+      <c r="K63" s="23">
         <f>$D$24*($D$22-K36*AndelBioaffald)</f>
         <v>0</v>
       </c>
-      <c r="L63" s="24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H64" s="19" t="s">
+      <c r="L63" s="23">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N63" s="18"/>
+      <c r="O63" s="18"/>
+      <c r="P63" s="23"/>
+      <c r="Q63" s="23"/>
+      <c r="R63" s="23"/>
+    </row>
+    <row r="64" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H64" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="I64" s="19" t="s">
+      <c r="I64" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="J64" s="23">
+      <c r="J64" s="22">
         <f>$C$18*J40+$D$18*J41+$E$18*J34</f>
         <v>1049040</v>
       </c>
-      <c r="K64" s="23">
+      <c r="K64" s="22">
         <f>J64+$F$18*$K$43</f>
-        <v>1100462.4495554105</v>
-      </c>
-      <c r="L64" s="24">
-        <f t="shared" si="1"/>
-        <v>51422.449555410538</v>
-      </c>
-    </row>
-    <row r="65" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H65" s="19" t="s">
+        <v>1107810.8046975606</v>
+      </c>
+      <c r="L64" s="23">
+        <f t="shared" si="11"/>
+        <v>58770.804697560612</v>
+      </c>
+      <c r="N64" s="18"/>
+      <c r="O64" s="18"/>
+      <c r="P64" s="22"/>
+      <c r="Q64" s="22"/>
+      <c r="R64" s="23"/>
+    </row>
+    <row r="65" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H65" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="I65" s="19" t="s">
+      <c r="I65" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="J65" s="23">
+      <c r="J65" s="22">
         <f>AFV*3.6*J46</f>
         <v>2211287.04</v>
       </c>
-      <c r="K65" s="23">
+      <c r="K65" s="22">
         <f>AFV*3.6*K46</f>
-        <v>2239801.2000000002</v>
-      </c>
-      <c r="L65" s="24">
-        <f t="shared" si="1"/>
-        <v>28514.160000000149</v>
-      </c>
-    </row>
-    <row r="66" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H66" s="19" t="s">
+        <v>2729557.4400000004</v>
+      </c>
+      <c r="L65" s="23">
+        <f t="shared" si="11"/>
+        <v>518270.40000000037</v>
+      </c>
+      <c r="N65" s="18"/>
+      <c r="O65" s="18"/>
+      <c r="P65" s="22"/>
+      <c r="Q65" s="22"/>
+      <c r="R65" s="23"/>
+    </row>
+    <row r="66" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H66" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I66" s="19" t="s">
+      <c r="I66" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="J66" s="24">
+      <c r="J66" s="23">
         <f>ATL*3.6*J54</f>
         <v>2271283.2000000002</v>
       </c>
-      <c r="K66" s="24">
+      <c r="K66" s="23">
         <f>ATL*3.6*K54</f>
-        <v>2017302.855586088</v>
-      </c>
-      <c r="L66" s="24">
-        <f t="shared" si="1"/>
-        <v>-253980.34441391216</v>
-      </c>
-    </row>
-    <row r="67" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H67" s="19" t="s">
+        <v>2468551.6981097562</v>
+      </c>
+      <c r="L66" s="23">
+        <f t="shared" si="11"/>
+        <v>197268.49810975604</v>
+      </c>
+      <c r="N66" s="18"/>
+      <c r="O66" s="18"/>
+      <c r="P66" s="23"/>
+      <c r="Q66" s="23"/>
+      <c r="R66" s="23"/>
+    </row>
+    <row r="67" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H67" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="I67" s="19" t="s">
+      <c r="I67" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="J67" s="24">
+      <c r="J67" s="23">
         <f>CO2afgift*$C$26 /1000 *3.6*J54</f>
         <v>471719.80799999996</v>
       </c>
-      <c r="K67" s="24">
+      <c r="K67" s="23">
         <f>CO2afgift*$C$26 /1000 *3.6*K54</f>
-        <v>418970.96571441251</v>
-      </c>
-      <c r="L67" s="24">
-        <f t="shared" si="1"/>
-        <v>-52748.842285587452</v>
-      </c>
-    </row>
-    <row r="68" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H68" s="19" t="s">
+        <v>512690.2418291159</v>
+      </c>
+      <c r="L67" s="23">
+        <f t="shared" si="11"/>
+        <v>40970.433829115937</v>
+      </c>
+      <c r="N67" s="18"/>
+      <c r="O67" s="18"/>
+      <c r="P67" s="23"/>
+      <c r="Q67" s="23"/>
+      <c r="R67" s="23"/>
+    </row>
+    <row r="68" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H68" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="I68" s="19" t="s">
+      <c r="I68" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="J68" s="24">
+      <c r="J68" s="23">
         <f>Kvotepris*$C$27/1000*C28*J35</f>
         <v>2093987.8587116271</v>
       </c>
-      <c r="K68" s="24">
+      <c r="K68" s="23">
         <f>Kvotepris*$C$27/1000*10.6*K35</f>
-        <v>1815509.1559763304</v>
-      </c>
-      <c r="L68" s="24">
-        <f t="shared" si="1"/>
-        <v>-278478.70273529668</v>
-      </c>
-    </row>
-    <row r="69" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="I69" s="19"/>
-      <c r="J69" s="24"/>
-      <c r="K69" s="24"/>
-      <c r="L69" s="24"/>
-    </row>
-    <row r="70" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H70" s="19" t="s">
+        <v>2093987.8587116271</v>
+      </c>
+      <c r="L68" s="23">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N68" s="18"/>
+      <c r="O68" s="18"/>
+      <c r="P68" s="23"/>
+      <c r="Q68" s="23"/>
+      <c r="R68" s="23"/>
+    </row>
+    <row r="69" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="I69" s="18"/>
+      <c r="J69" s="23"/>
+      <c r="K69" s="23"/>
+      <c r="L69" s="23"/>
+      <c r="O69" s="18"/>
+      <c r="P69" s="23"/>
+      <c r="Q69" s="23"/>
+      <c r="R69" s="23"/>
+    </row>
+    <row r="70" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H70" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="I70" s="19" t="s">
+      <c r="I70" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="J70" s="24">
+      <c r="J70" s="23">
         <f>SUM(J58:J61)</f>
         <v>15999762.201966742</v>
       </c>
-      <c r="K70" s="24">
+      <c r="K70" s="23">
         <f>SUM(K58:K61)</f>
-        <v>15554413.692023873</v>
-      </c>
-      <c r="L70" s="24">
-        <f t="shared" si="1"/>
-        <v>-445348.50994286872</v>
-      </c>
-    </row>
-    <row r="71" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H71" s="19" t="s">
+        <v>17981997.371777717</v>
+      </c>
+      <c r="L70" s="23">
+        <f t="shared" si="11"/>
+        <v>1982235.169810975</v>
+      </c>
+      <c r="N70" s="18"/>
+      <c r="O70" s="18"/>
+      <c r="P70" s="23"/>
+      <c r="Q70" s="23"/>
+      <c r="R70" s="23"/>
+    </row>
+    <row r="71" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H71" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="I71" s="19" t="s">
+      <c r="I71" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="J71" s="24">
+      <c r="J71" s="23">
         <f>SUM(J63:J68)</f>
         <v>8097317.9067116277</v>
       </c>
-      <c r="K71" s="24">
+      <c r="K71" s="23">
         <f>SUM(K63:K68)</f>
-        <v>7592046.6268322412</v>
-      </c>
-      <c r="L71" s="24">
-        <f t="shared" si="1"/>
-        <v>-505271.27987938654</v>
-      </c>
-    </row>
-    <row r="72" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H72" s="19" t="s">
+        <v>8912598.0433480591</v>
+      </c>
+      <c r="L71" s="23">
+        <f t="shared" si="11"/>
+        <v>815280.13663643133</v>
+      </c>
+      <c r="N71" s="18"/>
+      <c r="O71" s="18"/>
+      <c r="P71" s="23"/>
+      <c r="Q71" s="23"/>
+      <c r="R71" s="23"/>
+    </row>
+    <row r="72" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H72" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="I72" s="19" t="s">
+      <c r="I72" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="J72" s="24">
+      <c r="J72" s="23">
         <f>J70-J71</f>
         <v>7902444.2952551143</v>
       </c>
-      <c r="K72" s="24">
+      <c r="K72" s="23">
         <f>K70-K71</f>
-        <v>7962367.0651916321</v>
-      </c>
-      <c r="L72" s="24">
-        <f t="shared" si="1"/>
-        <v>59922.769936517812</v>
-      </c>
+        <v>9069399.328429658</v>
+      </c>
+      <c r="L72" s="23">
+        <f t="shared" si="11"/>
+        <v>1166955.0331745436</v>
+      </c>
+      <c r="N72" s="18"/>
+      <c r="O72" s="18"/>
+      <c r="P72" s="23"/>
+      <c r="Q72" s="23"/>
+      <c r="R72" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="H2:L2"/>
-    <mergeCell ref="N2:T2"/>
+    <mergeCell ref="T2:Z2"/>
+    <mergeCell ref="N2:R2"/>
   </mergeCells>
+  <conditionalFormatting sqref="J14:K72">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -7020,6 +7678,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7066,29 +7725,29 @@
       <c r="C4" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <v>11400.2114002</v>
       </c>
       <c r="F4" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="16">
         <v>1382.27949725194</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="16">
         <v>2526.36441138806</v>
       </c>
       <c r="J4" t="s">
         <v>77</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="17">
         <v>10.5</v>
       </c>
-      <c r="M4" s="17">
+      <c r="M4" s="16">
         <f>G4*$K4/3.6</f>
         <v>4031.6485336514916</v>
       </c>
-      <c r="N4" s="17">
+      <c r="N4" s="16">
         <f>H4*$K4/3.6</f>
         <v>7368.5628665485083</v>
       </c>
@@ -7097,29 +7756,29 @@
       <c r="C5" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="16">
         <v>0</v>
       </c>
       <c r="F5" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="17">
-        <v>0</v>
-      </c>
-      <c r="H5" s="17">
+      <c r="G5" s="16">
+        <v>0</v>
+      </c>
+      <c r="H5" s="16">
         <v>0</v>
       </c>
       <c r="J5" t="s">
         <v>78</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="17">
         <v>10.5</v>
       </c>
-      <c r="M5" s="17">
+      <c r="M5" s="16">
         <f t="shared" ref="M5:M24" si="0">G5*$K5/3.6</f>
         <v>0</v>
       </c>
-      <c r="N5" s="17">
+      <c r="N5" s="16">
         <f t="shared" ref="N5:N24" si="1">H5*$K5/3.6</f>
         <v>0</v>
       </c>
@@ -7128,29 +7787,29 @@
       <c r="C6" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <v>0</v>
       </c>
       <c r="F6" t="s">
         <v>79</v>
       </c>
-      <c r="G6" s="17">
-        <v>0</v>
-      </c>
-      <c r="H6" s="17">
+      <c r="G6" s="16">
+        <v>0</v>
+      </c>
+      <c r="H6" s="16">
         <v>0</v>
       </c>
       <c r="J6" t="s">
         <v>79</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="17">
         <v>10.5</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N6" s="17">
+      <c r="N6" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7159,29 +7818,29 @@
       <c r="C7" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <v>6154.3428210033298</v>
       </c>
       <c r="F7" t="s">
         <v>80</v>
       </c>
-      <c r="G7" s="17">
-        <v>0</v>
-      </c>
-      <c r="H7" s="17">
+      <c r="G7" s="16">
+        <v>0</v>
+      </c>
+      <c r="H7" s="16">
         <v>2356.9823569800001</v>
       </c>
       <c r="J7" t="s">
         <v>80</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="17">
         <v>9.4</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N7" s="17">
+      <c r="N7" s="16">
         <f t="shared" si="1"/>
         <v>6154.3428210033335</v>
       </c>
@@ -7190,29 +7849,29 @@
       <c r="C8" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>1276.2179428833299</v>
       </c>
       <c r="F8" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="16">
         <v>437.56043756000003</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="16">
         <v>0</v>
       </c>
       <c r="J8" t="s">
         <v>81</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="17">
         <v>10.5</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="16">
         <f t="shared" si="0"/>
         <v>1276.2179428833335</v>
       </c>
-      <c r="N8" s="17">
+      <c r="N8" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7221,29 +7880,29 @@
       <c r="C9" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <v>0</v>
       </c>
       <c r="F9" t="s">
         <v>82</v>
       </c>
-      <c r="G9" s="17">
-        <v>0</v>
-      </c>
-      <c r="H9" s="17">
+      <c r="G9" s="16">
+        <v>0</v>
+      </c>
+      <c r="H9" s="16">
         <v>0</v>
       </c>
       <c r="J9" t="s">
         <v>82</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="17">
         <v>14.5</v>
       </c>
-      <c r="M9" s="17">
+      <c r="M9" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N9" s="17">
+      <c r="N9" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7252,29 +7911,29 @@
       <c r="C10" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="16">
         <v>972.20097220000002</v>
       </c>
       <c r="F10" t="s">
         <v>83</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="16">
         <v>291.66029165999998</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="16">
         <v>0</v>
       </c>
       <c r="J10" t="s">
         <v>83</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="17">
         <v>12</v>
       </c>
-      <c r="M10" s="17">
+      <c r="M10" s="16">
         <f t="shared" si="0"/>
         <v>972.20097219999991</v>
       </c>
-      <c r="N10" s="17">
+      <c r="N10" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7283,29 +7942,29 @@
       <c r="C11" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="16">
         <v>15.375015375</v>
       </c>
       <c r="F11" t="s">
         <v>84</v>
       </c>
-      <c r="G11" s="17">
+      <c r="G11" s="16">
         <v>6.1500061500000003</v>
       </c>
-      <c r="H11" s="17">
+      <c r="H11" s="16">
         <v>0</v>
       </c>
       <c r="J11" t="s">
         <v>84</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="17">
         <v>9</v>
       </c>
-      <c r="M11" s="17">
+      <c r="M11" s="16">
         <f t="shared" si="0"/>
         <v>15.375015375</v>
       </c>
-      <c r="N11" s="17">
+      <c r="N11" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7314,29 +7973,29 @@
       <c r="C12" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="16">
         <v>785.27856305555599</v>
       </c>
       <c r="F12" t="s">
         <v>85</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12" s="16">
         <v>257.00025699999998</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="16">
         <v>0</v>
       </c>
       <c r="J12" t="s">
         <v>85</v>
       </c>
-      <c r="K12" s="18">
+      <c r="K12" s="17">
         <v>11</v>
       </c>
-      <c r="M12" s="17">
+      <c r="M12" s="16">
         <f t="shared" si="0"/>
         <v>785.27856305555542</v>
       </c>
-      <c r="N12" s="17">
+      <c r="N12" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7345,29 +8004,29 @@
       <c r="C13" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="16">
         <v>60.1667268333333</v>
       </c>
       <c r="F13" t="s">
         <v>86</v>
       </c>
-      <c r="G13" s="17">
+      <c r="G13" s="16">
         <v>22.800022800000001</v>
       </c>
-      <c r="H13" s="17">
+      <c r="H13" s="16">
         <v>0</v>
       </c>
       <c r="J13" t="s">
         <v>86</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="17">
         <v>9.5</v>
       </c>
-      <c r="M13" s="17">
+      <c r="M13" s="16">
         <f t="shared" si="0"/>
         <v>60.166726833333335</v>
       </c>
-      <c r="N13" s="17">
+      <c r="N13" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7376,29 +8035,29 @@
       <c r="C14" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="16">
         <v>2540.00254</v>
       </c>
       <c r="F14" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="17">
-        <v>0</v>
-      </c>
-      <c r="H14" s="17">
+      <c r="G14" s="16">
+        <v>0</v>
+      </c>
+      <c r="H14" s="16">
         <v>1016.001016</v>
       </c>
       <c r="J14" t="s">
         <v>87</v>
       </c>
-      <c r="K14" s="18">
+      <c r="K14" s="17">
         <v>9</v>
       </c>
-      <c r="M14" s="17">
+      <c r="M14" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N14" s="17">
+      <c r="N14" s="16">
         <f t="shared" si="1"/>
         <v>2540.00254</v>
       </c>
@@ -7407,29 +8066,29 @@
       <c r="C15" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="16">
         <v>45.100045100000003</v>
       </c>
       <c r="F15" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="17">
-        <v>0</v>
-      </c>
-      <c r="H15" s="17">
+      <c r="G15" s="16">
+        <v>0</v>
+      </c>
+      <c r="H15" s="16">
         <v>13.53001353</v>
       </c>
       <c r="J15" t="s">
         <v>88</v>
       </c>
-      <c r="K15" s="18">
+      <c r="K15" s="17">
         <v>12</v>
       </c>
-      <c r="M15" s="17">
+      <c r="M15" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N15" s="17">
+      <c r="N15" s="16">
         <f t="shared" si="1"/>
         <v>45.100045100000003</v>
       </c>
@@ -7438,29 +8097,29 @@
       <c r="C16" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="16">
         <v>18.861129972222201</v>
       </c>
       <c r="F16" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="17">
+      <c r="G16" s="16">
         <v>6.7900067899999996</v>
       </c>
-      <c r="H16" s="17">
+      <c r="H16" s="16">
         <v>0</v>
       </c>
       <c r="J16" t="s">
         <v>89</v>
       </c>
-      <c r="K16" s="18">
+      <c r="K16" s="17">
         <v>10</v>
       </c>
-      <c r="M16" s="17">
+      <c r="M16" s="16">
         <f t="shared" si="0"/>
         <v>18.861129972222219</v>
       </c>
-      <c r="N16" s="17">
+      <c r="N16" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7469,29 +8128,29 @@
       <c r="C17" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="16">
         <v>0</v>
       </c>
       <c r="F17" t="s">
         <v>90</v>
       </c>
-      <c r="G17" s="17">
-        <v>0</v>
-      </c>
-      <c r="H17" s="17">
+      <c r="G17" s="16">
+        <v>0</v>
+      </c>
+      <c r="H17" s="16">
         <v>0</v>
       </c>
       <c r="J17" t="s">
         <v>90</v>
       </c>
-      <c r="K17" s="18">
+      <c r="K17" s="17">
         <v>11</v>
       </c>
-      <c r="M17" s="17">
+      <c r="M17" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N17" s="17">
+      <c r="N17" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7500,29 +8159,29 @@
       <c r="C18" t="s">
         <v>91</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="16">
         <v>9410.2844102750005</v>
       </c>
       <c r="F18" t="s">
         <v>91</v>
       </c>
-      <c r="G18" s="17">
-        <v>0</v>
-      </c>
-      <c r="H18" s="17">
+      <c r="G18" s="16">
+        <v>0</v>
+      </c>
+      <c r="H18" s="16">
         <v>3226.38322638</v>
       </c>
       <c r="J18" t="s">
         <v>91</v>
       </c>
-      <c r="K18" s="18">
+      <c r="K18" s="17">
         <v>10.5</v>
       </c>
-      <c r="M18" s="17">
+      <c r="M18" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N18" s="17">
+      <c r="N18" s="16">
         <f t="shared" si="1"/>
         <v>9410.2844102750005</v>
       </c>
@@ -7531,29 +8190,29 @@
       <c r="C19" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="16">
         <v>0</v>
       </c>
       <c r="F19" t="s">
         <v>92</v>
       </c>
-      <c r="G19" s="17">
-        <v>0</v>
-      </c>
-      <c r="H19" s="17">
+      <c r="G19" s="16">
+        <v>0</v>
+      </c>
+      <c r="H19" s="16">
         <v>0</v>
       </c>
       <c r="J19" t="s">
         <v>92</v>
       </c>
-      <c r="K19" s="18">
+      <c r="K19" s="17">
         <v>10.5</v>
       </c>
-      <c r="M19" s="17">
+      <c r="M19" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N19" s="17">
+      <c r="N19" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7562,29 +8221,29 @@
       <c r="C20" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="16">
         <v>0</v>
       </c>
       <c r="F20" t="s">
         <v>93</v>
       </c>
-      <c r="G20" s="17">
-        <v>0</v>
-      </c>
-      <c r="H20" s="17">
+      <c r="G20" s="16">
+        <v>0</v>
+      </c>
+      <c r="H20" s="16">
         <v>0</v>
       </c>
       <c r="J20" t="s">
         <v>93</v>
       </c>
-      <c r="K20" s="18">
+      <c r="K20" s="17">
         <v>13</v>
       </c>
-      <c r="M20" s="17">
+      <c r="M20" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N20" s="17">
+      <c r="N20" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7593,29 +8252,29 @@
       <c r="C21" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="16">
         <v>231.59745381944401</v>
       </c>
       <c r="F21" t="s">
         <v>94</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G21" s="16">
         <v>57.500057499999997</v>
       </c>
-      <c r="H21" s="17">
+      <c r="H21" s="16">
         <v>0</v>
       </c>
       <c r="J21" t="s">
         <v>94</v>
       </c>
-      <c r="K21" s="18">
+      <c r="K21" s="17">
         <v>14.5</v>
       </c>
-      <c r="M21" s="17">
+      <c r="M21" s="16">
         <f t="shared" si="0"/>
         <v>231.59745381944444</v>
       </c>
-      <c r="N21" s="17">
+      <c r="N21" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7624,29 +8283,29 @@
       <c r="C22" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="16">
         <v>0</v>
       </c>
       <c r="F22" t="s">
         <v>95</v>
       </c>
-      <c r="G22" s="17">
-        <v>0</v>
-      </c>
-      <c r="H22" s="17">
+      <c r="G22" s="16">
+        <v>0</v>
+      </c>
+      <c r="H22" s="16">
         <v>0</v>
       </c>
       <c r="J22" t="s">
         <v>95</v>
       </c>
-      <c r="K22" s="18">
+      <c r="K22" s="17">
         <v>14.7</v>
       </c>
-      <c r="M22" s="17">
+      <c r="M22" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N22" s="17">
+      <c r="N22" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7655,29 +8314,29 @@
       <c r="C23" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="16">
         <v>41.300041299999997</v>
       </c>
       <c r="F23" t="s">
         <v>96</v>
       </c>
-      <c r="G23" s="17">
+      <c r="G23" s="16">
         <v>10.62001062</v>
       </c>
-      <c r="H23" s="17">
+      <c r="H23" s="16">
         <v>0</v>
       </c>
       <c r="J23" t="s">
         <v>96</v>
       </c>
-      <c r="K23" s="18">
+      <c r="K23" s="17">
         <v>14</v>
       </c>
-      <c r="M23" s="17">
+      <c r="M23" s="16">
         <f t="shared" si="0"/>
         <v>41.300041299999997</v>
       </c>
-      <c r="N23" s="17">
+      <c r="N23" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7686,47 +8345,47 @@
       <c r="C24" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="16">
         <v>37.975037974999999</v>
       </c>
       <c r="F24" t="s">
         <v>97</v>
       </c>
-      <c r="G24" s="17">
+      <c r="G24" s="16">
         <v>15.19001519</v>
       </c>
-      <c r="H24" s="17">
+      <c r="H24" s="16">
         <v>0</v>
       </c>
       <c r="J24" t="s">
         <v>97</v>
       </c>
-      <c r="K24" s="18">
+      <c r="K24" s="17">
         <v>9</v>
       </c>
-      <c r="M24" s="17">
+      <c r="M24" s="16">
         <f t="shared" si="0"/>
         <v>37.975037974999999</v>
       </c>
-      <c r="N24" s="17">
+      <c r="N24" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D25" s="17">
+      <c r="D25" s="16">
         <f>SUM(D4:D24)</f>
         <v>32988.914099992209</v>
       </c>
-      <c r="K25" s="17"/>
+      <c r="K25" s="16"/>
       <c r="L25" t="s">
         <v>102</v>
       </c>
-      <c r="M25" s="17">
+      <c r="M25" s="16">
         <f>SUM(M4:M24)</f>
         <v>7470.6214170653802</v>
       </c>
-      <c r="N25" s="17">
+      <c r="N25" s="16">
         <f>SUM(N4:N24)</f>
         <v>25518.29268292684</v>
       </c>
@@ -7742,17 +8401,17 @@
       <c r="L27" t="s">
         <v>101</v>
       </c>
-      <c r="M27" s="17">
+      <c r="M27" s="16">
         <f>M25*0.844</f>
         <v>6305.2044760031804</v>
       </c>
-      <c r="N27" s="17">
+      <c r="N27" s="16">
         <f>N25*0.656</f>
         <v>16740.000000000007</v>
       </c>
     </row>
     <row r="28" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D28" s="17">
+      <c r="D28" s="16">
         <f>SUMPRODUCT(G4:G24,K4:K24)+SUMPRODUCT(H4:H24,K4:K24)</f>
         <v>118760.09075997199</v>
       </c>
@@ -7785,16 +8444,16 @@
       <c r="L30" t="s">
         <v>76</v>
       </c>
-      <c r="M30" s="17">
+      <c r="M30" s="16">
         <v>6305.2044760031904</v>
       </c>
-      <c r="N30" s="17">
+      <c r="N30" s="16">
         <v>16740</v>
       </c>
-      <c r="O30" s="17">
+      <c r="O30" s="16">
         <v>4000</v>
       </c>
-      <c r="P30" s="17">
+      <c r="P30" s="16">
         <v>1069</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Yderligere omrokeringer på arket
</commit_message>
<xml_diff>
--- a/REFA Forenklet VPO-model.xlsx
+++ b/REFA Forenklet VPO-model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\REFA Affald\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C52EC4-B121-471A-9242-22A4A41DA308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDEC94F-257A-4739-BD44-E32ED873561F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{858EECC8-30FB-4D42-A70B-DA5455FDD71D}"/>
     <workbookView xWindow="-15" yWindow="0" windowWidth="14550" windowHeight="15510" activeTab="1" xr2:uid="{16E12CA9-1556-4394-AFAE-8F484516E35F}"/>
@@ -1167,17 +1167,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Model!$J$57</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Uden RGK</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1388,95 +1377,95 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Model!$H$58:$H$72</c:f>
+              <c:f>Model!$N$5:$N$19</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>Indtægter total</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Omkostninger total</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dækningsbidrag</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Varmesalg</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>Elsalg</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>RGK-rabat</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>Modtagebetaling affald</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>Betaling bioaffald</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>DV-omkostninger</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>Affaldvarme-afgift</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>Tillægsafgift</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
                   <c:v>CO2-afgift</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="14">
                   <c:v>Kvote-omkostning</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Indtægter total</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Omkostninger total</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Dækningsbidrag</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Model!$J$58:$J$72</c:f>
+              <c:f>Model!$P$5:$P$19</c:f>
               <c:numCache>
                 <c:formatCode>#,##0,</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>15999762.201966742</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8097317.9067116277</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7902444.2952551143</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>7404288</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>3947332.4512195126</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>4648141.7507472299</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>1049040</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>2211287.04</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>2271283.2000000002</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
                   <c:v>471719.80799999996</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="14">
                   <c:v>2093987.8587116271</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>15999762.201966742</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8097317.9067116277</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7902444.2952551143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1490,17 +1479,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Model!$K$57</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Med 100% RGK</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent2"/>
@@ -1570,95 +1548,95 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Model!$H$58:$H$72</c:f>
+              <c:f>Model!$N$5:$N$19</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>Indtægter total</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Omkostninger total</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dækningsbidrag</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Varmesalg</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>Elsalg</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>RGK-rabat</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>Modtagebetaling affald</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>Betaling bioaffald</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>DV-omkostninger</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>Affaldvarme-afgift</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>Tillægsafgift</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
                   <c:v>CO2-afgift</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="14">
                   <c:v>Kvote-omkostning</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Indtægter total</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Omkostninger total</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Dækningsbidrag</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Model!$K$58:$K$72</c:f>
+              <c:f>Model!$Q$5:$Q$19</c:f>
               <c:numCache>
                 <c:formatCode>#,##0,</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>17981997.371777717</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8912598.0433480591</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9069399.328429658</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>9139668</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>3947332.4512195126</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>246855.16981097564</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>4648141.7507472299</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>1107810.8046975606</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>2729557.4400000004</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>2468551.6981097562</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
                   <c:v>512690.2418291159</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="14">
                   <c:v>2093987.8587116271</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>17981997.371777717</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8912598.0433480591</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9069399.328429658</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1956,7 +1934,7 @@
     <c:title>
       <c:tx>
         <c:strRef>
-          <c:f>Model!$T$4</c:f>
+          <c:f>Model!$T$25</c:f>
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
@@ -2499,7 +2477,7 @@
     <c:title>
       <c:tx>
         <c:strRef>
-          <c:f>Model!$T$26</c:f>
+          <c:f>Model!$T$4</c:f>
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
@@ -2557,17 +2535,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Model!$L$57</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>RGK ift. nominel</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2638,95 +2605,95 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Model!$H$58:$H$72</c:f>
+              <c:f>Model!$N$5:$N$19</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>Indtægter total</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Omkostninger total</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dækningsbidrag</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Varmesalg</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>Elsalg</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>RGK-rabat</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>Modtagebetaling affald</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>Betaling bioaffald</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>DV-omkostninger</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>Affaldvarme-afgift</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>Tillægsafgift</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
                   <c:v>CO2-afgift</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="14">
                   <c:v>Kvote-omkostning</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Indtægter total</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Omkostninger total</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Dækningsbidrag</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Model!$L$58:$L$72</c:f>
+              <c:f>Model!$R$5:$R$19</c:f>
               <c:numCache>
                 <c:formatCode>#,##0,</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>1982235.169810975</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>815280.13663643133</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1166955.0331745436</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1735380</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>246855.16981097564</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>246855.16981097564</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>58770.804697560612</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>518270.40000000037</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>197268.49810975604</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
                   <c:v>40970.433829115937</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="14">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1982235.169810975</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>815280.13663643133</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1166955.0331745436</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4723,15 +4690,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>14007</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>31325</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>36368</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>587655</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>190050</xdr:rowOff>
+      <xdr:colOff>604973</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>16868</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4760,13 +4727,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>11206</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>22412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>584854</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>2912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5209,8 +5176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5354189-028E-4B88-AC75-E88799B17CAC}">
   <dimension ref="A2:Z72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AH42" sqref="AH42"/>
     </sheetView>
     <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
       <selection activeCell="J46" sqref="J46"/>
@@ -5223,13 +5190,13 @@
     <col min="3" max="5" width="9.140625" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="2.85546875" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="11" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="13.28515625" style="16" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="14.42578125" style="16" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="2.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="11" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="13.28515625" style="16" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="14.42578125" style="16" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="15.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="2.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10" style="16" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.42578125" style="16" bestFit="1" customWidth="1"/>
@@ -5310,15 +5277,15 @@
         <v>RGK ift. nominel</v>
       </c>
       <c r="T4" s="24" t="str">
-        <f>"Varmemængder: "&amp;C22&amp;" ton affald, "&amp;D22&amp;" ton bioaffald"</f>
-        <v>Varmemængder: 15000 ton affald, 0 ton bioaffald</v>
-      </c>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="12"/>
+        <f>"RGK ift. Nominel: "&amp;C22&amp;" ton affald, "&amp;D22&amp;" ton bioaffald"</f>
+        <v>RGK ift. Nominel: 15000 ton affald, 0 ton bioaffald</v>
+      </c>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -6296,6 +6263,16 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
+      <c r="T25" s="24" t="str">
+        <f>"Varmemængder: "&amp;C22&amp;" ton affald, "&amp;D22&amp;" ton bioaffald"</f>
+        <v>Varmemængder: 15000 ton affald, 0 ton bioaffald</v>
+      </c>
+      <c r="U25" s="12"/>
+      <c r="V25" s="12"/>
+      <c r="W25" s="12"/>
+      <c r="X25" s="12"/>
+      <c r="Y25" s="12"/>
+      <c r="Z25" s="12"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
@@ -6350,16 +6327,6 @@
         <f t="shared" si="8"/>
         <v>5580</v>
       </c>
-      <c r="T26" s="24" t="str">
-        <f>"RGK ift. Nominel: "&amp;C22&amp;" ton affald, "&amp;D22&amp;" ton bioaffald"</f>
-        <v>RGK ift. Nominel: 15000 ton affald, 0 ton bioaffald</v>
-      </c>
-      <c r="U26" s="11"/>
-      <c r="V26" s="11"/>
-      <c r="W26" s="11"/>
-      <c r="X26" s="11"/>
-      <c r="Y26" s="11"/>
-      <c r="Z26" s="11"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">

</xml_diff>